<commit_message>
SEK framework with MxContribution
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
@@ -99,21 +99,6 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Only to keep the usual name for discounting curve
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">1 fixing day
-publication lag -1
 </t>
         </r>
       </text>
@@ -1803,46 +1788,46 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:52:28</v>
         <stp/>
-        <stp>{5CD90A45-EC28-4749-84DA-4A6D4BF86F4E}</stp>
+        <stp>{0FE0AD45-EC15-403D-BB11-A5491B13F846}</stp>
+        <tr r="P5" s="69"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:57:43</v>
+        <stp/>
+        <stp>{D2E3642B-15D2-4619-86D5-E3A0BFBFEFD1}</stp>
+        <tr r="P5" s="67"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:58:43</v>
+        <stp/>
+        <stp>{D03E7A43-86EC-43D9-8887-9082AE3ACA30}</stp>
+        <tr r="O6" s="22"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:30</v>
+        <stp/>
+        <stp>{72E476C8-51A0-4F77-BABC-89C3B2D2301A}</stp>
+        <tr r="N5" s="16"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:30</v>
+        <stp/>
+        <stp>{09750DFC-EA08-4970-9B7F-3BFB05CF321E}</stp>
         <tr r="S3" s="64"/>
       </tp>
       <tp t="s">
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:05:30</v>
         <stp/>
-        <stp>{8D200708-481F-4AC1-A682-4A403E8ADF16}</stp>
-        <tr r="P5" s="66"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 10:28:55</v>
-        <stp/>
-        <stp>{0F5F8FE7-2BF8-4E1A-ADEC-A0D3CBF8D3A1}</stp>
+        <stp>{A36384B3-000D-4B3A-B43F-EAEC5AF36BC0}</stp>
         <tr r="K5" s="15"/>
       </tp>
       <tp t="s">
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:58:43</v>
         <stp/>
-        <stp>{C29D71BF-D042-49A7-B84D-F80E4B127C04}</stp>
-        <tr r="P5" s="67"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 10:28:55</v>
-        <stp/>
-        <stp>{D39C5586-B8F5-41B3-A554-5DCC1ECAFDCA}</stp>
-        <tr r="P5" s="69"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 10:28:55</v>
-        <stp/>
-        <stp>{1A58FEF8-A0A5-4E72-BC6F-9C5ACCF3DA87}</stp>
-        <tr r="N5" s="16"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 10:31:02</v>
-        <stp/>
-        <stp>{8ED45A6D-BE69-4ED0-A809-93EA1EE9E4F5}</stp>
-        <tr r="O6" s="22"/>
+        <stp>{037652E3-27F4-4CE1-8995-98610AE8EACF}</stp>
+        <tr r="P5" s="66"/>
       </tp>
     </main>
   </volType>
@@ -2158,7 +2143,7 @@
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="72" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov 18 2014 09:26:00</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov  4 2014 09:24:39</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -2166,14 +2151,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="75">
-        <v>42024.435601851852</v>
+        <v>42041.628310185188</v>
       </c>
       <c r="H3" s="114" t="s">
         <v>132</v>
       </c>
       <c r="I3" s="77">
         <f>_xll.ohTrigger(Deposits!S4,FRA3M!X4,OIS!Y5,Swaps3M!Z4,BasisSwap3M6M!Z4,BasisSwap1M3M!Z4)</f>
-        <v>24</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2220,7 +2205,7 @@
       </c>
       <c r="D8" s="85">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42025</v>
+        <v>42041</v>
       </c>
       <c r="E8" s="105"/>
       <c r="G8" s="97"/>
@@ -2539,9 +2524,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AC15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2654,7 +2637,7 @@
       </c>
       <c r="S3" s="183" t="str">
         <f>_xll.RData(S4:S10,T3:U3,"RTFEED:IDN",,,T4)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:05:30</v>
       </c>
       <c r="T3" s="177" t="s">
         <v>137</v>
@@ -2719,7 +2702,7 @@
         <v>104</v>
       </c>
       <c r="D5" s="122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="122" t="str">
         <f t="shared" ref="E5:E10" si="0">Calendar</f>
@@ -2744,11 +2727,11 @@
       </c>
       <c r="K5" s="123" t="str">
         <f>_xll.qlOvernightIndex(I5,,D5,Currency,Calendar,H5,J5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborON#0000</v>
+        <v>SekiborON#0001</v>
       </c>
       <c r="L5" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C5&amp;"LastFixing_Quote",K5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborONLastFixing_Quote#0000</v>
+        <v>SekiborONLastFixing_Quote#0001</v>
       </c>
       <c r="M5" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K5)</f>
@@ -2763,17 +2746,17 @@
       </c>
       <c r="R5" s="21" t="str">
         <f>K5</f>
-        <v>SekiborON#0000</v>
+        <v>SekiborON#0001</v>
       </c>
       <c r="S5" s="178" t="str">
         <f t="shared" ref="S5:S10" si="2">"STI"&amp;Currency&amp;Q5&amp;"DFI="</f>
         <v>STISEKTNDFI=</v>
       </c>
       <c r="T5" s="178">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U5" s="187">
-        <v>6.5999999999999989E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="V5" s="178" t="b">
         <f>IF(AND(ISNUMBER($U5),$U5&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2783,9 +2766,9 @@
         <f>IF(U5,_xll.qlIndexAddFixings(R5,T5,U5/100,TRUE),NA())</f>
         <v>1</v>
       </c>
-      <c r="X5" s="181" t="e">
+      <c r="X5" s="181">
         <f>_xll.qlQuoteValue(L5)</f>
-        <v>#NUM!</v>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="Y5" s="8"/>
     </row>
@@ -2844,10 +2827,10 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="T6" s="178">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U6" s="187">
-        <v>8.5999999999999993E-2</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="V6" s="178" t="b">
         <f>IF(AND(ISNUMBER($U6),$U6&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2859,7 +2842,7 @@
       </c>
       <c r="X6" s="181">
         <f>_xll.qlQuoteValue(L6)</f>
-        <v>9.7999999999999997E-4</v>
+        <v>8.5999999999999998E-4</v>
       </c>
       <c r="Y6" s="8"/>
     </row>
@@ -2921,10 +2904,10 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="T7" s="178">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U7" s="187">
-        <v>0.14499999999999999</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="V7" s="178" t="b">
         <f t="shared" ref="V7:V10" si="5">IF(AND(ISNUMBER($U7),$U7&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2936,7 +2919,7 @@
       </c>
       <c r="X7" s="181">
         <f>_xll.qlQuoteValue(L7)</f>
-        <v>1.5100000000000001E-3</v>
+        <v>1.4499999999999999E-3</v>
       </c>
       <c r="Y7" s="8"/>
     </row>
@@ -2995,10 +2978,10 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="T8" s="178">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U8" s="187">
-        <v>0.14399999999999999</v>
+        <v>1.2E-2</v>
       </c>
       <c r="V8" s="178" t="b">
         <f t="shared" si="5"/>
@@ -3010,7 +2993,7 @@
       </c>
       <c r="X8" s="181">
         <f>_xll.qlQuoteValue(L8)</f>
-        <v>1.91E-3</v>
+        <v>1.4399999999999999E-3</v>
       </c>
       <c r="Y8" s="8"/>
     </row>
@@ -3072,10 +3055,10 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="T9" s="178">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U9" s="187">
-        <v>0.20299999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="V9" s="178" t="b">
         <f t="shared" si="5"/>
@@ -3087,7 +3070,7 @@
       </c>
       <c r="X9" s="181">
         <f>_xll.qlQuoteValue(L9)</f>
-        <v>2.5500000000000002E-3</v>
+        <v>2.0299999999999997E-3</v>
       </c>
       <c r="Y9" s="8"/>
     </row>
@@ -3149,10 +3132,10 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="T10" s="179">
-        <v>42023</v>
+        <v>42040</v>
       </c>
       <c r="U10" s="187">
-        <v>0.29799999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="V10" s="179" t="b">
         <f t="shared" si="5"/>
@@ -3164,7 +3147,7 @@
       </c>
       <c r="X10" s="182">
         <f>_xll.qlQuoteValue(L10)</f>
-        <v>3.3799999999999998E-3</v>
+        <v>2.98E-3</v>
       </c>
       <c r="Y10" s="8"/>
     </row>
@@ -4561,7 +4544,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="33">
         <f>_xll.ohTrigger(S6:S23)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="T4" s="34"/>
     </row>
@@ -4583,7 +4566,7 @@
       <c r="J5" s="166"/>
       <c r="K5" s="176" t="str">
         <f>_xll.RData(K7:K23,L5:M5,,ReutersRtMode,,L7)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:05:30</v>
       </c>
       <c r="L5" s="167" t="s">
         <v>106</v>
@@ -4680,14 +4663,14 @@
         <v>STISEKTNDFI=</v>
       </c>
       <c r="L7" s="153">
-        <v>6.5999999999999989E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="M7" s="153">
         <v>0</v>
       </c>
       <c r="N7" s="47">
         <f>_xll.qlMidEquivalent(L7,M7)</f>
-        <v>6.5999999999999989E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="O7" s="32"/>
       <c r="P7" s="47">
@@ -4695,11 +4678,11 @@
       </c>
       <c r="Q7" s="32"/>
       <c r="R7" s="47">
-        <v>6.5999999999999989E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="S7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E7,R7/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.9999999999999987E-4</v>
       </c>
       <c r="T7" s="34"/>
     </row>
@@ -4778,14 +4761,14 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="L9" s="153">
-        <v>8.5999999999999993E-2</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="M9" s="153">
         <v>0</v>
       </c>
       <c r="N9" s="47">
         <f>_xll.qlMidEquivalent(L9,M9)</f>
-        <v>8.5999999999999993E-2</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="O9" s="32"/>
       <c r="P9" s="47">
@@ -4793,11 +4776,11 @@
       </c>
       <c r="Q9" s="32"/>
       <c r="R9" s="47">
-        <v>8.5999999999999993E-2</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="S9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E9,R9/100,Trigger)</f>
-        <v>0</v>
+        <v>-4.8999999999999998E-4</v>
       </c>
       <c r="T9" s="34"/>
     </row>
@@ -4925,14 +4908,14 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="L12" s="153">
-        <v>0.14499999999999999</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="M12" s="153">
         <v>0</v>
       </c>
       <c r="N12" s="47">
         <f>_xll.qlMidEquivalent(L12,M12)</f>
-        <v>0.14499999999999999</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="O12" s="32"/>
       <c r="P12" s="154">
@@ -4940,11 +4923,11 @@
       </c>
       <c r="Q12" s="32"/>
       <c r="R12" s="47">
-        <v>0.14499999999999999</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="S12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E12,R12/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.3399999999999998E-3</v>
       </c>
       <c r="T12" s="34"/>
     </row>
@@ -4974,14 +4957,14 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="L13" s="153">
-        <v>0.14399999999999999</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M13" s="153">
         <v>0</v>
       </c>
       <c r="N13" s="47">
         <f>_xll.qlMidEquivalent(L13,M13)</f>
-        <v>0.14399999999999999</v>
+        <v>1.2E-2</v>
       </c>
       <c r="O13" s="32"/>
       <c r="P13" s="154">
@@ -4989,11 +4972,11 @@
       </c>
       <c r="Q13" s="32"/>
       <c r="R13" s="47">
-        <v>0.14399999999999999</v>
+        <v>1.2E-2</v>
       </c>
       <c r="S13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E13,R13/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.3199999999999998E-3</v>
       </c>
       <c r="T13" s="34"/>
     </row>
@@ -5023,14 +5006,14 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="L14" s="153">
-        <v>0.20299999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="M14" s="153">
         <v>0</v>
       </c>
       <c r="N14" s="47">
         <f>_xll.qlMidEquivalent(L14,M14)</f>
-        <v>0.20299999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="O14" s="32"/>
       <c r="P14" s="154">
@@ -5038,11 +5021,11 @@
       </c>
       <c r="Q14" s="32"/>
       <c r="R14" s="47">
-        <v>0.20299999999999999</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="S14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E14,R14/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.4899999999999996E-3</v>
       </c>
       <c r="T14" s="34"/>
     </row>
@@ -5170,14 +5153,14 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="L17" s="153">
-        <v>0.29799999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="M17" s="153">
         <v>0</v>
       </c>
       <c r="N17" s="47">
         <f>_xll.qlMidEquivalent(L17,M17)</f>
-        <v>0.29799999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="O17" s="32"/>
       <c r="P17" s="154">
@@ -5185,11 +5168,11 @@
       </c>
       <c r="Q17" s="32"/>
       <c r="R17" s="47">
-        <v>0.29799999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="S17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E17,R17/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.65E-3</v>
       </c>
       <c r="T17" s="34"/>
     </row>
@@ -5664,7 +5647,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="33">
         <f>_xll.ohTrigger(X6:X20)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Y4" s="34"/>
       <c r="AA4" s="28"/>
@@ -5695,7 +5678,7 @@
       <c r="M5" s="175"/>
       <c r="N5" s="176" t="str">
         <f>_xll.RData(N6:N20,O5:R5,"RTFEED:IDN",ReutersRtMode,,O6)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:05:30</v>
       </c>
       <c r="O5" s="168" t="s">
         <v>106</v>
@@ -5778,10 +5761,10 @@
         <v>SEK3F1=HBCO</v>
       </c>
       <c r="O6" s="39">
-        <v>0.15</v>
+        <v>5.5E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>0.16999999999999998</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="Q6" s="37">
         <v>0</v>
@@ -5791,7 +5774,7 @@
       </c>
       <c r="S6" s="39">
         <f>IF(ISERROR(AVERAGE(O6,P6)),#NUM!,AVERAGE(O6,P6))</f>
-        <v>0.15999999999999998</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="T6" s="32"/>
       <c r="U6" s="40">
@@ -5800,11 +5783,11 @@
       <c r="V6" s="32"/>
       <c r="W6" s="40">
         <f t="array" ref="W6:W20">QuoteLive</f>
-        <v>0.15999999999999998</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="X6" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/100,Trigger)</f>
-        <v>0</v>
+        <v>-9.4999999999999989E-4</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="AA6" s="28"/>
@@ -5818,11 +5801,11 @@
       </c>
       <c r="AD6" s="199">
         <f>100-W6</f>
-        <v>99.84</v>
+        <v>99.935000000000002</v>
       </c>
       <c r="AE6" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC6,AD6,Trigger)</f>
-        <v>0</v>
+        <v>9.4999999999998863E-2</v>
       </c>
       <c r="AF6" s="59"/>
     </row>
@@ -5864,10 +5847,10 @@
         <v>SEK3F2=HBCO</v>
       </c>
       <c r="O7" s="46">
-        <v>0.1125</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="P7" s="46">
-        <v>0.13250000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="Q7" s="44">
         <v>0</v>
@@ -5877,7 +5860,7 @@
       </c>
       <c r="S7" s="46">
         <f t="shared" ref="S7:S20" si="4">IF(ISERROR(AVERAGE(O7,P7)),#NUM!,AVERAGE(O7,P7))</f>
-        <v>0.1225</v>
+        <v>0.04</v>
       </c>
       <c r="T7" s="32"/>
       <c r="U7" s="47">
@@ -5885,11 +5868,11 @@
       </c>
       <c r="V7" s="32"/>
       <c r="W7" s="47">
-        <v>0.1225</v>
+        <v>0.04</v>
       </c>
       <c r="X7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F7,W7/100,Trigger)</f>
-        <v>0</v>
+        <v>-8.25E-4</v>
       </c>
       <c r="Y7" s="34"/>
       <c r="AA7" s="28"/>
@@ -5903,11 +5886,11 @@
       </c>
       <c r="AD7" s="200">
         <f t="shared" ref="AD7:AD20" si="6">100-W7</f>
-        <v>99.877499999999998</v>
+        <v>99.96</v>
       </c>
       <c r="AE7" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC7,AD7,Trigger)</f>
-        <v>0</v>
+        <v>8.2499999999996021E-2</v>
       </c>
       <c r="AF7" s="59"/>
     </row>
@@ -5949,10 +5932,10 @@
         <v>SEK3F3=HBCO</v>
       </c>
       <c r="O8" s="46">
-        <v>0.10249999999999999</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="P8" s="46">
-        <v>0.12250000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="Q8" s="44">
         <v>0</v>
@@ -5962,7 +5945,7 @@
       </c>
       <c r="S8" s="46">
         <f t="shared" si="4"/>
-        <v>0.1125</v>
+        <v>0.04</v>
       </c>
       <c r="T8" s="32"/>
       <c r="U8" s="47">
@@ -5970,11 +5953,11 @@
       </c>
       <c r="V8" s="32"/>
       <c r="W8" s="47">
-        <v>0.1125</v>
+        <v>0.04</v>
       </c>
       <c r="X8" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F8,W8/100,Trigger)</f>
-        <v>0</v>
+        <v>-7.2500000000000017E-4</v>
       </c>
       <c r="Y8" s="34"/>
       <c r="AA8" s="28"/>
@@ -5988,11 +5971,11 @@
       </c>
       <c r="AD8" s="200">
         <f t="shared" si="6"/>
-        <v>99.887500000000003</v>
+        <v>99.96</v>
       </c>
       <c r="AE8" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC8,AD8,Trigger)</f>
-        <v>0</v>
+        <v>7.2499999999990905E-2</v>
       </c>
       <c r="AF8" s="59"/>
     </row>
@@ -6034,10 +6017,10 @@
         <v>SEK3F4=HBCO</v>
       </c>
       <c r="O9" s="46">
-        <v>0.1</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="P9" s="46">
-        <v>0.12</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="Q9" s="44">
         <v>0</v>
@@ -6047,7 +6030,7 @@
       </c>
       <c r="S9" s="46">
         <f t="shared" si="4"/>
-        <v>0.11</v>
+        <v>5.5000000000000007E-2</v>
       </c>
       <c r="T9" s="32"/>
       <c r="U9" s="47">
@@ -6055,11 +6038,11 @@
       </c>
       <c r="V9" s="32"/>
       <c r="W9" s="47">
-        <v>0.11</v>
+        <v>5.5000000000000007E-2</v>
       </c>
       <c r="X9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F9,W9/100,Trigger)</f>
-        <v>0</v>
+        <v>-5.5000000000000003E-4</v>
       </c>
       <c r="Y9" s="34"/>
       <c r="AA9" s="28"/>
@@ -6073,11 +6056,11 @@
       </c>
       <c r="AD9" s="200">
         <f t="shared" si="6"/>
-        <v>99.89</v>
+        <v>99.944999999999993</v>
       </c>
       <c r="AE9" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC9,AD9,Trigger)</f>
-        <v>0</v>
+        <v>5.499999999999261E-2</v>
       </c>
       <c r="AF9" s="59"/>
     </row>
@@ -6119,10 +6102,10 @@
         <v>SEK3F5=HBCO</v>
       </c>
       <c r="O10" s="46">
-        <v>0.10249999999999999</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="P10" s="46">
-        <v>0.13250000000000001</v>
+        <v>9.7500000000000003E-2</v>
       </c>
       <c r="Q10" s="44">
         <v>0</v>
@@ -6132,7 +6115,7 @@
       </c>
       <c r="S10" s="46">
         <f t="shared" si="4"/>
-        <v>0.11749999999999999</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="T10" s="32"/>
       <c r="U10" s="47">
@@ -6140,11 +6123,11 @@
       </c>
       <c r="V10" s="32"/>
       <c r="W10" s="47">
-        <v>0.11749999999999999</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="X10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/100,Trigger)</f>
-        <v>0</v>
+        <v>-3.4999999999999983E-4</v>
       </c>
       <c r="Y10" s="34"/>
       <c r="AA10" s="28"/>
@@ -6158,11 +6141,11 @@
       </c>
       <c r="AD10" s="200">
         <f t="shared" si="6"/>
-        <v>99.882499999999993</v>
+        <v>99.917500000000004</v>
       </c>
       <c r="AE10" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC10,AD10,Trigger)</f>
-        <v>0</v>
+        <v>3.50000000000108E-2</v>
       </c>
       <c r="AF10" s="59"/>
     </row>
@@ -6204,10 +6187,10 @@
         <v>SEK3F6=HBCO</v>
       </c>
       <c r="O11" s="46">
-        <v>0.12</v>
+        <v>0.10500000000000001</v>
       </c>
       <c r="P11" s="46">
-        <v>0.15</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="Q11" s="44">
         <v>0</v>
@@ -6217,7 +6200,7 @@
       </c>
       <c r="S11" s="46">
         <f t="shared" si="4"/>
-        <v>0.13500000000000001</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="T11" s="32"/>
       <c r="U11" s="47">
@@ -6225,11 +6208,11 @@
       </c>
       <c r="V11" s="32"/>
       <c r="W11" s="47">
-        <v>0.13500000000000001</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="X11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.4999999999999996E-4</v>
       </c>
       <c r="Y11" s="34"/>
       <c r="AA11" s="28"/>
@@ -6243,11 +6226,11 @@
       </c>
       <c r="AD11" s="200">
         <f t="shared" si="6"/>
-        <v>99.864999999999995</v>
+        <v>99.88</v>
       </c>
       <c r="AE11" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC11,AD11,Trigger)</f>
-        <v>0</v>
+        <v>1.5000000000000568E-2</v>
       </c>
       <c r="AF11" s="59"/>
     </row>
@@ -6289,10 +6272,10 @@
         <v>SEK3F7=HBCO</v>
       </c>
       <c r="O12" s="46">
-        <v>0.16</v>
+        <v>0.155</v>
       </c>
       <c r="P12" s="46">
-        <v>0.19</v>
+        <v>0.185</v>
       </c>
       <c r="Q12" s="44">
         <v>0</v>
@@ -6302,7 +6285,7 @@
       </c>
       <c r="S12" s="46">
         <f t="shared" si="4"/>
-        <v>0.17499999999999999</v>
+        <v>0.16999999999999998</v>
       </c>
       <c r="T12" s="32"/>
       <c r="U12" s="47">
@@ -6310,11 +6293,11 @@
       </c>
       <c r="V12" s="32"/>
       <c r="W12" s="47">
-        <v>0.17499999999999999</v>
+        <v>0.16999999999999998</v>
       </c>
       <c r="X12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/100,Trigger)</f>
-        <v>0</v>
+        <v>-4.9999999999999914E-5</v>
       </c>
       <c r="Y12" s="34"/>
       <c r="AA12" s="28"/>
@@ -6328,11 +6311,11 @@
       </c>
       <c r="AD12" s="200">
         <f t="shared" si="6"/>
-        <v>99.825000000000003</v>
+        <v>99.83</v>
       </c>
       <c r="AE12" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC12,AD12,Trigger)</f>
-        <v>0</v>
+        <v>4.9999999999954525E-3</v>
       </c>
       <c r="AF12" s="59"/>
     </row>
@@ -6374,10 +6357,10 @@
         <v>SEK3F8=HBCO</v>
       </c>
       <c r="O13" s="46">
-        <v>0.21000000000000002</v>
+        <v>0.215</v>
       </c>
       <c r="P13" s="46">
-        <v>0.24</v>
+        <v>0.24500000000000002</v>
       </c>
       <c r="Q13" s="44">
         <v>0</v>
@@ -6387,7 +6370,7 @@
       </c>
       <c r="S13" s="46">
         <f t="shared" si="4"/>
-        <v>0.22500000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="T13" s="32"/>
       <c r="U13" s="47">
@@ -6395,11 +6378,11 @@
       </c>
       <c r="V13" s="32"/>
       <c r="W13" s="47">
-        <v>0.22500000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="X13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/100,Trigger)</f>
-        <v>0</v>
+        <v>4.9999999999999697E-5</v>
       </c>
       <c r="Y13" s="34"/>
       <c r="AA13" s="28"/>
@@ -6413,11 +6396,11 @@
       </c>
       <c r="AD13" s="200">
         <f t="shared" si="6"/>
-        <v>99.775000000000006</v>
+        <v>99.77</v>
       </c>
       <c r="AE13" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC13,AD13,Trigger)</f>
-        <v>0</v>
+        <v>-5.0000000000096634E-3</v>
       </c>
       <c r="AF13" s="59"/>
     </row>
@@ -6459,10 +6442,10 @@
         <v>SEK3F9=HBCO</v>
       </c>
       <c r="O14" s="46">
-        <v>0.26250000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="P14" s="46">
-        <v>0.30249999999999999</v>
+        <v>0.32</v>
       </c>
       <c r="Q14" s="44">
         <v>0</v>
@@ -6472,7 +6455,7 @@
       </c>
       <c r="S14" s="46">
         <f t="shared" si="4"/>
-        <v>0.28249999999999997</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="T14" s="32"/>
       <c r="U14" s="47">
@@ -6480,11 +6463,11 @@
       </c>
       <c r="V14" s="32"/>
       <c r="W14" s="47">
-        <v>0.28249999999999997</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="X14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,W14/100,Trigger)</f>
-        <v>0</v>
+        <v>1.7500000000000068E-4</v>
       </c>
       <c r="Y14" s="34"/>
       <c r="AA14" s="28"/>
@@ -6498,11 +6481,11 @@
       </c>
       <c r="AD14" s="200">
         <f t="shared" si="6"/>
-        <v>99.717500000000001</v>
+        <v>99.7</v>
       </c>
       <c r="AE14" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC14,AD14,Trigger)</f>
-        <v>0</v>
+        <v>-1.7499999999998295E-2</v>
       </c>
       <c r="AF14" s="59"/>
     </row>
@@ -6544,10 +6527,10 @@
         <v>SEK3F10=HBCO</v>
       </c>
       <c r="O15" s="46">
-        <v>0.32750000000000001</v>
+        <v>0.35750000000000004</v>
       </c>
       <c r="P15" s="46">
-        <v>0.36749999999999999</v>
+        <v>0.39750000000000002</v>
       </c>
       <c r="Q15" s="44">
         <v>0</v>
@@ -6557,7 +6540,7 @@
       </c>
       <c r="S15" s="46">
         <f t="shared" si="4"/>
-        <v>0.34750000000000003</v>
+        <v>0.37750000000000006</v>
       </c>
       <c r="T15" s="32"/>
       <c r="U15" s="47">
@@ -6565,11 +6548,11 @@
       </c>
       <c r="V15" s="32"/>
       <c r="W15" s="47">
-        <v>0.34750000000000003</v>
+        <v>0.37750000000000006</v>
       </c>
       <c r="X15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/100,Trigger)</f>
-        <v>0</v>
+        <v>3.0000000000000035E-4</v>
       </c>
       <c r="Y15" s="34"/>
       <c r="AA15" s="28"/>
@@ -6583,11 +6566,11 @@
       </c>
       <c r="AD15" s="200">
         <f t="shared" si="6"/>
-        <v>99.652500000000003</v>
+        <v>99.622500000000002</v>
       </c>
       <c r="AE15" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC15,AD15,Trigger)</f>
-        <v>0</v>
+        <v>-3.0000000000001137E-2</v>
       </c>
       <c r="AF15" s="59"/>
     </row>
@@ -6629,10 +6612,10 @@
         <v>SEK3F11=HBCO</v>
       </c>
       <c r="O16" s="46">
-        <v>0.4</v>
+        <v>0.4375</v>
       </c>
       <c r="P16" s="46">
-        <v>0.44000000000000006</v>
+        <v>0.47750000000000004</v>
       </c>
       <c r="Q16" s="44">
         <v>0</v>
@@ -6642,7 +6625,7 @@
       </c>
       <c r="S16" s="46">
         <f t="shared" si="4"/>
-        <v>0.42000000000000004</v>
+        <v>0.45750000000000002</v>
       </c>
       <c r="T16" s="32"/>
       <c r="U16" s="47">
@@ -6650,11 +6633,11 @@
       </c>
       <c r="V16" s="32"/>
       <c r="W16" s="47">
-        <v>0.42000000000000004</v>
+        <v>0.45750000000000002</v>
       </c>
       <c r="X16" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F16,W16/100,Trigger)</f>
-        <v>0</v>
+        <v>3.7499999999999947E-4</v>
       </c>
       <c r="Y16" s="34"/>
       <c r="AA16" s="28"/>
@@ -6668,11 +6651,11 @@
       </c>
       <c r="AD16" s="200">
         <f t="shared" si="6"/>
-        <v>99.58</v>
+        <v>99.542500000000004</v>
       </c>
       <c r="AE16" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC16,AD16,Trigger)</f>
-        <v>0</v>
+        <v>-3.7499999999994316E-2</v>
       </c>
       <c r="AF16" s="59"/>
     </row>
@@ -6714,10 +6697,10 @@
         <v>SEK3F12=HBCO</v>
       </c>
       <c r="O17" s="46">
-        <v>0.47750000000000004</v>
+        <v>0.51750000000000007</v>
       </c>
       <c r="P17" s="46">
-        <v>0.51749999999999996</v>
+        <v>0.5575</v>
       </c>
       <c r="Q17" s="44">
         <v>0</v>
@@ -6727,7 +6710,7 @@
       </c>
       <c r="S17" s="46">
         <f t="shared" si="4"/>
-        <v>0.4975</v>
+        <v>0.53750000000000009</v>
       </c>
       <c r="T17" s="32"/>
       <c r="U17" s="47">
@@ -6735,11 +6718,11 @@
       </c>
       <c r="V17" s="32"/>
       <c r="W17" s="47">
-        <v>0.4975</v>
+        <v>0.53750000000000009</v>
       </c>
       <c r="X17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F17,W17/100,Trigger)</f>
-        <v>0</v>
+        <v>4.0000000000000105E-4</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="AA17" s="28"/>
@@ -6753,11 +6736,11 @@
       </c>
       <c r="AD17" s="200">
         <f t="shared" si="6"/>
-        <v>99.502499999999998</v>
+        <v>99.462500000000006</v>
       </c>
       <c r="AE17" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC17,AD17,Trigger)</f>
-        <v>0</v>
+        <v>-3.9999999999992042E-2</v>
       </c>
       <c r="AF17" s="59"/>
     </row>
@@ -7208,7 +7191,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="33">
         <f>_xll.ohTrigger(Y7:Y61)</f>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="Z5" s="34"/>
     </row>
@@ -7234,7 +7217,7 @@
       <c r="N6" s="234"/>
       <c r="O6" s="235" t="str">
         <f>_xll.RData(O7:O61,P6:S6,"RTFEED:IDN",ReutersRtMode,,P7)</f>
-        <v>Updated at 10:31:02</v>
+        <v>Updated at 15:58:43</v>
       </c>
       <c r="P6" s="190" t="s">
         <v>106</v>
@@ -7517,10 +7500,10 @@
         <v>SEKAMTNS1M=HBCO</v>
       </c>
       <c r="P10" s="46">
-        <v>5.5000000000000007E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="Q10" s="46">
-        <v>8.4999999999999992E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="R10" s="46">
         <v>0</v>
@@ -7530,7 +7513,7 @@
       </c>
       <c r="T10" s="46">
         <f t="shared" si="2"/>
-        <v>7.0000000000000007E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="U10" s="231"/>
       <c r="V10" s="233">
@@ -7538,7 +7521,7 @@
       </c>
       <c r="W10" s="231"/>
       <c r="X10" s="46">
-        <v>7.0000000000000007E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="Y10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,X10/100,Trigger)</f>
@@ -7588,10 +7571,10 @@
         <v>SEKAMTNS2M=HBCO</v>
       </c>
       <c r="P11" s="46">
-        <v>2.8999999999999998E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="Q11" s="46">
-        <v>5.9000000000000011E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="R11" s="46">
         <v>0</v>
@@ -7601,7 +7584,7 @@
       </c>
       <c r="T11" s="46">
         <f t="shared" si="2"/>
-        <v>4.4000000000000004E-2</v>
+        <v>-6.9999999999999993E-3</v>
       </c>
       <c r="U11" s="231"/>
       <c r="V11" s="233">
@@ -7609,7 +7592,7 @@
       </c>
       <c r="W11" s="231"/>
       <c r="X11" s="46">
-        <v>4.4000000000000004E-2</v>
+        <v>-6.9999999999999993E-3</v>
       </c>
       <c r="Y11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
@@ -7658,10 +7641,10 @@
         <v>SEKAMTNS3M=HBCO</v>
       </c>
       <c r="P12" s="46">
-        <v>1.9E-2</v>
+        <v>-2.8000000000000001E-2</v>
       </c>
       <c r="Q12" s="46">
-        <v>4.9000000000000002E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="R12" s="46">
         <v>0</v>
@@ -7671,7 +7654,7 @@
       </c>
       <c r="T12" s="46">
         <f t="shared" si="2"/>
-        <v>3.4000000000000002E-2</v>
+        <v>-1.3000000000000001E-2</v>
       </c>
       <c r="U12" s="231"/>
       <c r="V12" s="233">
@@ -7679,7 +7662,7 @@
       </c>
       <c r="W12" s="231"/>
       <c r="X12" s="46">
-        <v>3.4000000000000002E-2</v>
+        <v>-1.3000000000000001E-2</v>
       </c>
       <c r="Y12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
@@ -7728,10 +7711,10 @@
         <v>SEKAMTNS4M=HBCO</v>
       </c>
       <c r="P13" s="46">
-        <v>1.3000000000000001E-2</v>
+        <v>-3.6999999999999998E-2</v>
       </c>
       <c r="Q13" s="46">
-        <v>4.2999999999999997E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="R13" s="46">
         <v>0</v>
@@ -7741,7 +7724,7 @@
       </c>
       <c r="T13" s="46">
         <f t="shared" si="2"/>
-        <v>2.7999999999999997E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="U13" s="231"/>
       <c r="V13" s="233">
@@ -7749,7 +7732,7 @@
       </c>
       <c r="W13" s="231"/>
       <c r="X13" s="46">
-        <v>2.7999999999999997E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="Y13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,X13/100,Trigger)</f>
@@ -7798,10 +7781,10 @@
         <v>SEKAMTNS5M=HBCO</v>
       </c>
       <c r="P14" s="46">
-        <v>0.01</v>
+        <v>-4.3000000000000003E-2</v>
       </c>
       <c r="Q14" s="46">
-        <v>0.04</v>
+        <v>-1.3000000000000001E-2</v>
       </c>
       <c r="R14" s="46">
         <v>0</v>
@@ -7811,7 +7794,7 @@
       </c>
       <c r="T14" s="46">
         <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
+        <v>-2.8000000000000004E-2</v>
       </c>
       <c r="U14" s="231"/>
       <c r="V14" s="233">
@@ -7819,7 +7802,7 @@
       </c>
       <c r="W14" s="231"/>
       <c r="X14" s="46">
-        <v>2.5000000000000001E-2</v>
+        <v>-2.8000000000000004E-2</v>
       </c>
       <c r="Y14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,X14/100,Trigger)</f>
@@ -7868,10 +7851,10 @@
         <v>SEKAMTNS6M=HBCO</v>
       </c>
       <c r="P15" s="46">
-        <v>6.0000000000000001E-3</v>
+        <v>-4.8000000000000001E-2</v>
       </c>
       <c r="Q15" s="46">
-        <v>3.5999999999999997E-2</v>
+        <v>-1.8000000000000002E-2</v>
       </c>
       <c r="R15" s="46">
         <v>0</v>
@@ -7881,7 +7864,7 @@
       </c>
       <c r="T15" s="46">
         <f t="shared" si="2"/>
-        <v>2.0999999999999998E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="U15" s="231"/>
       <c r="V15" s="233">
@@ -7889,7 +7872,7 @@
       </c>
       <c r="W15" s="231"/>
       <c r="X15" s="46">
-        <v>2.0999999999999998E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="Y15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,X15/100,Trigger)</f>
@@ -8079,10 +8062,10 @@
         <v>SEKAMTNS9M=HBCO</v>
       </c>
       <c r="P18" s="46">
-        <v>-0.01</v>
+        <v>-5.7000000000000002E-2</v>
       </c>
       <c r="Q18" s="46">
-        <v>0.02</v>
+        <v>-2.7E-2</v>
       </c>
       <c r="R18" s="46">
         <v>0</v>
@@ -8092,7 +8075,7 @@
       </c>
       <c r="T18" s="46">
         <f t="shared" si="2"/>
-        <v>5.0000000000000001E-3</v>
+        <v>-4.2000000000000003E-2</v>
       </c>
       <c r="U18" s="231"/>
       <c r="V18" s="233">
@@ -8100,11 +8083,11 @@
       </c>
       <c r="W18" s="231"/>
       <c r="X18" s="46">
-        <v>5.0000000000000001E-3</v>
+        <v>-4.2000000000000003E-2</v>
       </c>
       <c r="Y18" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F18,X18/100,Trigger)</f>
-        <v>-1.5000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="34"/>
       <c r="AC18" s="237"/>
@@ -8290,10 +8273,10 @@
         <v>SEKAMTNS12M=HBCO</v>
       </c>
       <c r="P21" s="46">
-        <v>-2.1000000000000001E-2</v>
+        <v>-6.0999999999999999E-2</v>
       </c>
       <c r="Q21" s="46">
-        <v>8.9999999999999993E-3</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="R21" s="46">
         <v>0</v>
@@ -8303,7 +8286,7 @@
       </c>
       <c r="T21" s="46">
         <f t="shared" si="2"/>
-        <v>-6.000000000000001E-3</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="U21" s="231"/>
       <c r="V21" s="233">
@@ -8311,11 +8294,11 @@
       </c>
       <c r="W21" s="231"/>
       <c r="X21" s="46">
-        <v>-6.000000000000001E-3</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
       <c r="Y21" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F21,X21/100,Trigger)</f>
-        <v>-1.5000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="34"/>
     </row>
@@ -8359,7 +8342,7 @@
         <v>SEKAMTNS1Y=ICAP</v>
       </c>
       <c r="P22" s="39">
-        <v>-5.0000000000000001E-3</v>
+        <v>-4.5000000000000005E-2</v>
       </c>
       <c r="Q22" s="39">
         <v>0</v>
@@ -8372,7 +8355,7 @@
       </c>
       <c r="T22" s="39">
         <f t="shared" si="2"/>
-        <v>-2.5000000000000001E-3</v>
+        <v>-2.2500000000000003E-2</v>
       </c>
       <c r="U22" s="231"/>
       <c r="V22" s="232">
@@ -8380,11 +8363,11 @@
       </c>
       <c r="W22" s="231"/>
       <c r="X22" s="39">
-        <v>-2.5000000000000001E-3</v>
-      </c>
-      <c r="Y22" s="41" t="e">
+        <v>-2.2500000000000003E-2</v>
+      </c>
+      <c r="Y22" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F22,X22/100,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="34"/>
     </row>
@@ -9200,7 +9183,7 @@
         <v>SEKAMTNS2Y=ICAP</v>
       </c>
       <c r="P34" s="46">
-        <v>-4.4999999999999998E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="Q34" s="46">
         <v>0</v>
@@ -9213,7 +9196,7 @@
       </c>
       <c r="T34" s="46">
         <f t="shared" si="2"/>
-        <v>-2.2499999999999999E-2</v>
+        <v>-6.25E-2</v>
       </c>
       <c r="U34" s="231"/>
       <c r="V34" s="233">
@@ -9221,11 +9204,11 @@
       </c>
       <c r="W34" s="231"/>
       <c r="X34" s="46">
-        <v>-2.2499999999999999E-2</v>
-      </c>
-      <c r="Y34" s="48" t="e">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="Y34" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F34,X34/100,Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="34"/>
     </row>
@@ -9480,7 +9463,7 @@
         <v>SEKAMTNS3Y=ICAP</v>
       </c>
       <c r="P38" s="46">
-        <v>2.2499999999999999E-2</v>
+        <v>-2.75E-2</v>
       </c>
       <c r="Q38" s="46">
         <v>0</v>
@@ -9493,7 +9476,7 @@
       </c>
       <c r="T38" s="46">
         <f t="shared" si="2"/>
-        <v>1.125E-2</v>
+        <v>-1.375E-2</v>
       </c>
       <c r="U38" s="231"/>
       <c r="V38" s="233">
@@ -9501,11 +9484,11 @@
       </c>
       <c r="W38" s="231"/>
       <c r="X38" s="46">
-        <v>1.125E-2</v>
+        <v>-1.375E-2</v>
       </c>
       <c r="Y38" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F38,X38/100,Trigger)</f>
-        <v>-1.125E-4</v>
+        <v>0</v>
       </c>
       <c r="Z38" s="34"/>
     </row>
@@ -9760,7 +9743,7 @@
         <v>SEKAMTNS4Y=ICAP</v>
       </c>
       <c r="P42" s="46">
-        <v>0.1125</v>
+        <v>8.2500000000000004E-2</v>
       </c>
       <c r="Q42" s="46">
         <v>0</v>
@@ -9773,7 +9756,7 @@
       </c>
       <c r="T42" s="46">
         <f t="shared" si="2"/>
-        <v>5.6250000000000001E-2</v>
+        <v>4.1250000000000002E-2</v>
       </c>
       <c r="U42" s="231"/>
       <c r="V42" s="233">
@@ -9781,11 +9764,11 @@
       </c>
       <c r="W42" s="231"/>
       <c r="X42" s="46">
-        <v>5.6250000000000001E-2</v>
+        <v>4.1250000000000002E-2</v>
       </c>
       <c r="Y42" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F42,X42/100,Trigger)</f>
-        <v>-5.6250000000000007E-4</v>
+        <v>0</v>
       </c>
       <c r="Z42" s="34"/>
     </row>
@@ -10040,7 +10023,7 @@
         <v>SEKAMTNS5Y=ICAP</v>
       </c>
       <c r="P46" s="46">
-        <v>0.23500000000000001</v>
+        <v>0.21250000000000002</v>
       </c>
       <c r="Q46" s="46">
         <v>0</v>
@@ -10053,7 +10036,7 @@
       </c>
       <c r="T46" s="46">
         <f t="shared" si="2"/>
-        <v>0.11750000000000001</v>
+        <v>0.10625000000000001</v>
       </c>
       <c r="U46" s="231"/>
       <c r="V46" s="233">
@@ -10061,11 +10044,11 @@
       </c>
       <c r="W46" s="231"/>
       <c r="X46" s="46">
-        <v>0.11750000000000001</v>
+        <v>0.10625000000000001</v>
       </c>
       <c r="Y46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>-1.175E-3</v>
+        <v>0</v>
       </c>
       <c r="Z46" s="34"/>
     </row>
@@ -10110,7 +10093,7 @@
         <v>SEKAMTNS6Y=ICAP</v>
       </c>
       <c r="P47" s="46">
-        <v>0.36249999999999999</v>
+        <v>0.34500000000000003</v>
       </c>
       <c r="Q47" s="46">
         <v>0</v>
@@ -10123,7 +10106,7 @@
       </c>
       <c r="T47" s="46">
         <f t="shared" si="2"/>
-        <v>0.18124999999999999</v>
+        <v>0.17250000000000001</v>
       </c>
       <c r="U47" s="231"/>
       <c r="V47" s="233">
@@ -10131,11 +10114,11 @@
       </c>
       <c r="W47" s="231"/>
       <c r="X47" s="46">
-        <v>0.18124999999999999</v>
+        <v>0.17250000000000001</v>
       </c>
       <c r="Y47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>-1.8124999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="34"/>
     </row>
@@ -10180,7 +10163,7 @@
         <v>SEKAMTNS7Y=ICAP</v>
       </c>
       <c r="P48" s="46">
-        <v>0.48499999999999999</v>
+        <v>0.47250000000000003</v>
       </c>
       <c r="Q48" s="46">
         <v>0</v>
@@ -10193,7 +10176,7 @@
       </c>
       <c r="T48" s="46">
         <f t="shared" si="2"/>
-        <v>0.24249999999999999</v>
+        <v>0.23625000000000002</v>
       </c>
       <c r="U48" s="231"/>
       <c r="V48" s="233">
@@ -10201,11 +10184,11 @@
       </c>
       <c r="W48" s="231"/>
       <c r="X48" s="46">
-        <v>0.24249999999999999</v>
+        <v>0.23625000000000002</v>
       </c>
       <c r="Y48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>-2.4250000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Z48" s="34"/>
     </row>
@@ -10250,7 +10233,7 @@
         <v>SEKAMTNS8Y=ICAP</v>
       </c>
       <c r="P49" s="46">
-        <v>0.59749999999999992</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="Q49" s="46">
         <v>0</v>
@@ -10263,7 +10246,7 @@
       </c>
       <c r="T49" s="46">
         <f t="shared" si="2"/>
-        <v>0.29874999999999996</v>
+        <v>0.29375000000000001</v>
       </c>
       <c r="U49" s="231"/>
       <c r="V49" s="233">
@@ -10271,11 +10254,11 @@
       </c>
       <c r="W49" s="231"/>
       <c r="X49" s="46">
-        <v>0.29874999999999996</v>
+        <v>0.29375000000000001</v>
       </c>
       <c r="Y49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>-2.9874999999999997E-3</v>
+        <v>1.2499999999999491E-5</v>
       </c>
       <c r="Z49" s="34"/>
     </row>
@@ -10320,7 +10303,7 @@
         <v>SEKAMTNS9Y=ICAP</v>
       </c>
       <c r="P50" s="46">
-        <v>0.69500000000000006</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="Q50" s="46">
         <v>0</v>
@@ -10333,7 +10316,7 @@
       </c>
       <c r="T50" s="46">
         <f t="shared" si="2"/>
-        <v>0.34750000000000003</v>
+        <v>0.34250000000000003</v>
       </c>
       <c r="U50" s="231"/>
       <c r="V50" s="233">
@@ -10341,11 +10324,11 @@
       </c>
       <c r="W50" s="231"/>
       <c r="X50" s="46">
-        <v>0.34750000000000003</v>
+        <v>0.34250000000000003</v>
       </c>
       <c r="Y50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>-3.4750000000000002E-3</v>
+        <v>1.2499999999999924E-5</v>
       </c>
       <c r="Z50" s="34"/>
     </row>
@@ -10390,7 +10373,7 @@
         <v>SEKAMTNS10Y=ICAP</v>
       </c>
       <c r="P51" s="46">
-        <v>0.78249999999999997</v>
+        <v>0.76750000000000007</v>
       </c>
       <c r="Q51" s="46">
         <v>0</v>
@@ -10403,7 +10386,7 @@
       </c>
       <c r="T51" s="46">
         <f t="shared" si="2"/>
-        <v>0.39124999999999999</v>
+        <v>0.38375000000000004</v>
       </c>
       <c r="U51" s="231"/>
       <c r="V51" s="233">
@@ -10411,11 +10394,11 @@
       </c>
       <c r="W51" s="231"/>
       <c r="X51" s="46">
-        <v>0.39124999999999999</v>
+        <v>0.38375000000000004</v>
       </c>
       <c r="Y51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>-3.9125000000000002E-3</v>
+        <v>1.2499999999999924E-5</v>
       </c>
       <c r="Z51" s="34"/>
     </row>
@@ -10460,7 +10443,7 @@
         <v>SEKAMTNS12Y=ICAP</v>
       </c>
       <c r="P52" s="46">
-        <v>0.92749999999999999</v>
+        <v>0.91</v>
       </c>
       <c r="Q52" s="46">
         <v>0</v>
@@ -10473,7 +10456,7 @@
       </c>
       <c r="T52" s="46">
         <f t="shared" si="2"/>
-        <v>0.46375</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="U52" s="231"/>
       <c r="V52" s="233">
@@ -10481,11 +10464,11 @@
       </c>
       <c r="W52" s="231"/>
       <c r="X52" s="46">
-        <v>0.46375</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="Y52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>-4.6375000000000001E-3</v>
+        <v>1.2499999999999491E-5</v>
       </c>
       <c r="Z52" s="34"/>
     </row>
@@ -10530,7 +10513,7 @@
         <v>SEKAMTNS15Y=ICAP</v>
       </c>
       <c r="P53" s="46">
-        <v>1.1025</v>
+        <v>1.0775000000000001</v>
       </c>
       <c r="Q53" s="46">
         <v>0</v>
@@ -10543,7 +10526,7 @@
       </c>
       <c r="T53" s="46">
         <f t="shared" si="2"/>
-        <v>0.55125000000000002</v>
+        <v>0.53875000000000006</v>
       </c>
       <c r="U53" s="231"/>
       <c r="V53" s="233">
@@ -10551,11 +10534,11 @@
       </c>
       <c r="W53" s="231"/>
       <c r="X53" s="46">
-        <v>0.55125000000000002</v>
+        <v>0.53875000000000006</v>
       </c>
       <c r="Y53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F53,X53/100,Trigger)</f>
-        <v>-5.5125E-3</v>
+        <v>1.2500000000001225E-5</v>
       </c>
       <c r="Z53" s="34"/>
     </row>
@@ -10600,7 +10583,7 @@
         <v>SEKAMTNS20Y=ICAP</v>
       </c>
       <c r="P54" s="46">
-        <v>1.2925</v>
+        <v>1.2650000000000001</v>
       </c>
       <c r="Q54" s="46">
         <v>0</v>
@@ -10613,7 +10596,7 @@
       </c>
       <c r="T54" s="46">
         <f t="shared" si="2"/>
-        <v>0.64624999999999999</v>
+        <v>0.63250000000000006</v>
       </c>
       <c r="U54" s="231"/>
       <c r="V54" s="233">
@@ -10621,11 +10604,11 @@
       </c>
       <c r="W54" s="231"/>
       <c r="X54" s="46">
-        <v>0.64624999999999999</v>
+        <v>0.63250000000000006</v>
       </c>
       <c r="Y54" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>-6.4624999999999995E-3</v>
+        <v>1.2500000000001225E-5</v>
       </c>
       <c r="Z54" s="34"/>
     </row>
@@ -10670,7 +10653,7 @@
         <v>SEKAMTNS25Y=ICAP</v>
       </c>
       <c r="P55" s="46">
-        <v>1.3674999999999999</v>
+        <v>1.3425</v>
       </c>
       <c r="Q55" s="46">
         <v>0</v>
@@ -10683,7 +10666,7 @@
       </c>
       <c r="T55" s="46">
         <f t="shared" si="2"/>
-        <v>0.68374999999999997</v>
+        <v>0.67125000000000001</v>
       </c>
       <c r="U55" s="231"/>
       <c r="V55" s="233">
@@ -10691,11 +10674,11 @@
       </c>
       <c r="W55" s="231"/>
       <c r="X55" s="46">
-        <v>0.68374999999999997</v>
+        <v>0.67125000000000001</v>
       </c>
       <c r="Y55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F55,X55/100,Trigger)</f>
-        <v>-6.8374999999999998E-3</v>
+        <v>1.2499999999999491E-5</v>
       </c>
       <c r="Z55" s="34"/>
     </row>
@@ -10810,7 +10793,7 @@
         <v>SEKAMTNS30Y=ICAP</v>
       </c>
       <c r="P57" s="46">
-        <v>1.3900000000000001</v>
+        <v>1.3675000000000002</v>
       </c>
       <c r="Q57" s="46">
         <v>0</v>
@@ -10823,7 +10806,7 @@
       </c>
       <c r="T57" s="46">
         <f t="shared" si="2"/>
-        <v>0.69500000000000006</v>
+        <v>0.68375000000000008</v>
       </c>
       <c r="U57" s="231"/>
       <c r="V57" s="233">
@@ -10831,11 +10814,11 @@
       </c>
       <c r="W57" s="231"/>
       <c r="X57" s="46">
-        <v>0.69500000000000006</v>
+        <v>0.68375000000000008</v>
       </c>
       <c r="Y57" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F57,X57/100,Trigger)</f>
-        <v>-6.9500000000000004E-3</v>
+        <v>1.2500000000000358E-5</v>
       </c>
       <c r="Z57" s="34"/>
     </row>
@@ -11392,7 +11375,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -11419,7 +11402,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:58:43</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -12520,10 +12503,10 @@
         <v>SEKAB3S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>0.1125</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="R20" s="46">
-        <v>0.16250000000000001</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="S20" s="46">
         <v>0</v>
@@ -12533,7 +12516,7 @@
       </c>
       <c r="U20" s="46">
         <f t="shared" si="2"/>
-        <v>0.13750000000000001</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -12541,7 +12524,7 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>0.13750000000000001</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/100,Trigger)</f>
@@ -13397,10 +13380,10 @@
         <v>SEKAB3S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>0.11750000000000001</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="R32" s="46">
-        <v>0.16750000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="S32" s="46">
         <v>0</v>
@@ -13410,7 +13393,7 @@
       </c>
       <c r="U32" s="46">
         <f t="shared" si="2"/>
-        <v>0.14250000000000002</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -13418,7 +13401,7 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>0.14250000000000002</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/100,Trigger)</f>
@@ -13689,10 +13672,10 @@
         <v>SEKAB3S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>0.1875</v>
+        <v>0.1575</v>
       </c>
       <c r="R36" s="46">
-        <v>0.23749999999999999</v>
+        <v>0.20750000000000002</v>
       </c>
       <c r="S36" s="46">
         <v>0</v>
@@ -13702,7 +13685,7 @@
       </c>
       <c r="U36" s="46">
         <f t="shared" si="2"/>
-        <v>0.21249999999999999</v>
+        <v>0.1825</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -13710,7 +13693,7 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>0.21249999999999999</v>
+        <v>0.1825</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/100,Trigger)</f>
@@ -13981,10 +13964,10 @@
         <v>SEKAB3S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>0.29249999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R40" s="46">
-        <v>0.34249999999999997</v>
+        <v>0.33</v>
       </c>
       <c r="S40" s="46">
         <v>0</v>
@@ -13994,7 +13977,7 @@
       </c>
       <c r="U40" s="46">
         <f t="shared" si="2"/>
-        <v>0.3175</v>
+        <v>0.30500000000000005</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -14002,7 +13985,7 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>0.3175</v>
+        <v>0.30500000000000005</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/100,Trigger)</f>
@@ -14273,10 +14256,10 @@
         <v>SEKAB3S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>0.42499999999999999</v>
+        <v>0.41500000000000004</v>
       </c>
       <c r="R44" s="46">
-        <v>0.47499999999999998</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="S44" s="46">
         <v>0</v>
@@ -14286,7 +14269,7 @@
       </c>
       <c r="U44" s="46">
         <f t="shared" si="2"/>
-        <v>0.44999999999999996</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -14294,7 +14277,7 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>0.44999999999999996</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/100,Trigger)</f>
@@ -14346,10 +14329,10 @@
         <v>SEKAB3S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>0.5575</v>
+        <v>0.54749999999999999</v>
       </c>
       <c r="R45" s="46">
-        <v>0.60750000000000004</v>
+        <v>0.59750000000000003</v>
       </c>
       <c r="S45" s="46">
         <v>0</v>
@@ -14359,7 +14342,7 @@
       </c>
       <c r="U45" s="46">
         <f t="shared" si="2"/>
-        <v>0.58250000000000002</v>
+        <v>0.57250000000000001</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -14367,7 +14350,7 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>0.58250000000000002</v>
+        <v>0.57250000000000001</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/100,Trigger)</f>
@@ -14419,10 +14402,10 @@
         <v>SEKAB3S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>0.68499999999999994</v>
+        <v>0.67749999999999999</v>
       </c>
       <c r="R46" s="46">
-        <v>0.73499999999999999</v>
+        <v>0.72750000000000004</v>
       </c>
       <c r="S46" s="46">
         <v>0</v>
@@ -14432,7 +14415,7 @@
       </c>
       <c r="U46" s="46">
         <f t="shared" si="2"/>
-        <v>0.71</v>
+        <v>0.70250000000000001</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -14440,7 +14423,7 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>0.71</v>
+        <v>0.70250000000000001</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/100,Trigger)</f>
@@ -14492,10 +14475,10 @@
         <v>SEKAB3S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>0.79749999999999999</v>
+        <v>0.79250000000000009</v>
       </c>
       <c r="R47" s="46">
-        <v>0.84749999999999992</v>
+        <v>0.84250000000000003</v>
       </c>
       <c r="S47" s="46">
         <v>0</v>
@@ -14505,7 +14488,7 @@
       </c>
       <c r="U47" s="46">
         <f t="shared" si="2"/>
-        <v>0.82250000000000001</v>
+        <v>0.81750000000000012</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -14513,11 +14496,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>0.82250000000000001</v>
+        <v>0.81750000000000012</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000716E-5</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -14565,10 +14548,10 @@
         <v>SEKAB3S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>0.89749999999999996</v>
+        <v>0.89</v>
       </c>
       <c r="R48" s="46">
-        <v>0.94750000000000001</v>
+        <v>0.94000000000000006</v>
       </c>
       <c r="S48" s="46">
         <v>0</v>
@@ -14578,7 +14561,7 @@
       </c>
       <c r="U48" s="46">
         <f t="shared" si="2"/>
-        <v>0.92249999999999999</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -14586,7 +14569,7 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>0.92249999999999999</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/100,Trigger)</f>
@@ -14638,10 +14621,10 @@
         <v>SEKAB3S10Y=ICAP</v>
       </c>
       <c r="Q49" s="46">
-        <v>0.98499999999999999</v>
+        <v>0.97250000000000003</v>
       </c>
       <c r="R49" s="46">
-        <v>1.0349999999999999</v>
+        <v>1.0225</v>
       </c>
       <c r="S49" s="46">
         <v>0</v>
@@ -14651,7 +14634,7 @@
       </c>
       <c r="U49" s="46">
         <f t="shared" si="2"/>
-        <v>1.01</v>
+        <v>0.99750000000000005</v>
       </c>
       <c r="V49" s="231"/>
       <c r="W49" s="233">
@@ -14659,11 +14642,11 @@
       </c>
       <c r="X49" s="231"/>
       <c r="Y49" s="46">
-        <v>1.01</v>
+        <v>0.99750000000000005</v>
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000716E-5</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -14711,10 +14694,10 @@
         <v>SEKAB3S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>1.1225000000000001</v>
+        <v>1.1075000000000002</v>
       </c>
       <c r="R50" s="46">
-        <v>1.1825000000000001</v>
+        <v>1.1675</v>
       </c>
       <c r="S50" s="46">
         <v>0</v>
@@ -14724,7 +14707,7 @@
       </c>
       <c r="U50" s="46">
         <f t="shared" si="2"/>
-        <v>1.1525000000000001</v>
+        <v>1.1375000000000002</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -14732,7 +14715,7 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>1.1525000000000001</v>
+        <v>1.1375000000000002</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/100,Trigger)</f>
@@ -14784,10 +14767,10 @@
         <v>SEKAB3S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>1.2949999999999999</v>
+        <v>1.2725</v>
       </c>
       <c r="R51" s="46">
-        <v>1.355</v>
+        <v>1.3325</v>
       </c>
       <c r="S51" s="46">
         <v>0</v>
@@ -14797,7 +14780,7 @@
       </c>
       <c r="U51" s="46">
         <f t="shared" si="2"/>
-        <v>1.325</v>
+        <v>1.3025</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -14805,11 +14788,11 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>1.325</v>
+        <v>1.3025</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/100,Trigger)</f>
-        <v>0</v>
+        <v>2.4999999999998981E-5</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -14857,10 +14840,10 @@
         <v>SEKAB3S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>1.47</v>
+        <v>1.4475</v>
       </c>
       <c r="R52" s="46">
-        <v>1.55</v>
+        <v>1.5275000000000001</v>
       </c>
       <c r="S52" s="46">
         <v>0</v>
@@ -14870,7 +14853,7 @@
       </c>
       <c r="U52" s="46">
         <f t="shared" si="2"/>
-        <v>1.51</v>
+        <v>1.4875</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -14878,11 +14861,11 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>1.51</v>
+        <v>1.4875</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000716E-5</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -14930,10 +14913,10 @@
         <v>SEKAB3S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>1.54</v>
+        <v>1.5175000000000001</v>
       </c>
       <c r="R53" s="46">
-        <v>1.62</v>
+        <v>1.5975000000000001</v>
       </c>
       <c r="S53" s="46">
         <v>0</v>
@@ -14943,7 +14926,7 @@
       </c>
       <c r="U53" s="46">
         <f t="shared" si="2"/>
-        <v>1.58</v>
+        <v>1.5575000000000001</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -14951,11 +14934,11 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>1.58</v>
+        <v>1.5575000000000001</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/100,Trigger)</f>
-        <v>0</v>
+        <v>2.4999999999998981E-5</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -15076,10 +15059,10 @@
         <v>SEKAB3S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>1.55</v>
+        <v>1.5275000000000001</v>
       </c>
       <c r="R55" s="46">
-        <v>1.65</v>
+        <v>1.6275000000000002</v>
       </c>
       <c r="S55" s="46">
         <v>0</v>
@@ -15089,7 +15072,7 @@
       </c>
       <c r="U55" s="46">
         <f t="shared" si="2"/>
-        <v>1.6</v>
+        <v>1.5775000000000001</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -15097,11 +15080,11 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>1.6</v>
+        <v>1.5775000000000001</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000716E-5</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -15671,7 +15654,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -15698,7 +15681,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:57:43</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -16799,7 +16782,7 @@
         <v>SEK3S6S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>10.6</v>
+        <v>8.6</v>
       </c>
       <c r="R20" s="46">
         <v>0</v>
@@ -16812,7 +16795,7 @@
       </c>
       <c r="U20" s="46">
         <f>_xll.qlMidEquivalent($Q20,$R20,$S20,$T20)</f>
-        <v>10.6</v>
+        <v>8.6</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -16820,7 +16803,7 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>10.6</v>
+        <v>8.6</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
@@ -17676,7 +17659,7 @@
         <v>SEK3S6S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>10.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="R32" s="46">
         <v>0</v>
@@ -17689,7 +17672,7 @@
       </c>
       <c r="U32" s="46">
         <f>_xll.qlMidEquivalent($Q32,$R32,$S32,$T32)</f>
-        <v>10.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -17697,7 +17680,7 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>10.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
@@ -17968,7 +17951,7 @@
         <v>SEK3S6S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>10.19</v>
+        <v>9.52</v>
       </c>
       <c r="R36" s="46">
         <v>0</v>
@@ -17981,7 +17964,7 @@
       </c>
       <c r="U36" s="46">
         <f>_xll.qlMidEquivalent($Q36,$R36,$S36,$T36)</f>
-        <v>10.19</v>
+        <v>9.52</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -17989,7 +17972,7 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>10.19</v>
+        <v>9.52</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/10000,Trigger)</f>
@@ -18260,7 +18243,7 @@
         <v>SEK3S6S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>10.130000000000001</v>
+        <v>9.620000000000001</v>
       </c>
       <c r="R40" s="46">
         <v>0</v>
@@ -18273,7 +18256,7 @@
       </c>
       <c r="U40" s="46">
         <f>_xll.qlMidEquivalent($Q40,$R40,$S40,$T40)</f>
-        <v>10.130000000000001</v>
+        <v>9.620000000000001</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -18281,7 +18264,7 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>10.130000000000001</v>
+        <v>9.620000000000001</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
@@ -18552,7 +18535,7 @@
         <v>SEK3S6S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>10.08</v>
+        <v>9.67</v>
       </c>
       <c r="R44" s="46">
         <v>0</v>
@@ -18565,7 +18548,7 @@
       </c>
       <c r="U44" s="46">
         <f>_xll.qlMidEquivalent($Q44,$R44,$S44,$T44)</f>
-        <v>10.08</v>
+        <v>9.67</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -18573,7 +18556,7 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>10.08</v>
+        <v>9.67</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
@@ -18625,7 +18608,7 @@
         <v>SEK3S6S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>10.029999999999999</v>
+        <v>9.69</v>
       </c>
       <c r="R45" s="46">
         <v>0</v>
@@ -18638,7 +18621,7 @@
       </c>
       <c r="U45" s="46">
         <f>_xll.qlMidEquivalent($Q45,$R45,$S45,$T45)</f>
-        <v>10.029999999999999</v>
+        <v>9.69</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -18646,7 +18629,7 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>10.029999999999999</v>
+        <v>9.69</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
@@ -18698,7 +18681,7 @@
         <v>SEK3S6S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>9.99</v>
+        <v>9.69</v>
       </c>
       <c r="R46" s="46">
         <v>0</v>
@@ -18711,7 +18694,7 @@
       </c>
       <c r="U46" s="46">
         <f>_xll.qlMidEquivalent($Q46,$R46,$S46,$T46)</f>
-        <v>9.99</v>
+        <v>9.69</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -18719,7 +18702,7 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>9.99</v>
+        <v>9.69</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/10000,Trigger)</f>
@@ -18771,7 +18754,7 @@
         <v>SEK3S6S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>9.9499999999999993</v>
+        <v>9.69</v>
       </c>
       <c r="R47" s="46">
         <v>0</v>
@@ -18784,7 +18767,7 @@
       </c>
       <c r="U47" s="46">
         <f>_xll.qlMidEquivalent($Q47,$R47,$S47,$T47)</f>
-        <v>9.9499999999999993</v>
+        <v>9.69</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -18792,7 +18775,7 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>9.9499999999999993</v>
+        <v>9.69</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
@@ -18844,7 +18827,7 @@
         <v>SEK3S6S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>9.92</v>
+        <v>9.68</v>
       </c>
       <c r="R48" s="46">
         <v>0</v>
@@ -18857,7 +18840,7 @@
       </c>
       <c r="U48" s="46">
         <f>_xll.qlMidEquivalent($Q48,$R48,$S48,$T48)</f>
-        <v>9.92</v>
+        <v>9.68</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -18865,11 +18848,11 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>9.92</v>
+        <v>9.68</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.9999999999991589E-7</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -18917,7 +18900,7 @@
         <v>SEK3S6S10Y=ICAP</v>
       </c>
       <c r="Q49" s="46">
-        <v>9.84</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -18930,7 +18913,7 @@
       </c>
       <c r="U49" s="46">
         <f>_xll.qlMidEquivalent($Q49,$R49,$S49,$T49)</f>
-        <v>9.84</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="V49" s="231"/>
       <c r="W49" s="233">
@@ -18938,7 +18921,7 @@
       </c>
       <c r="X49" s="231"/>
       <c r="Y49" s="46">
-        <v>9.84</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/10000,Trigger)</f>
@@ -18990,7 +18973,7 @@
         <v>SEK3S6S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>9.5399999999999991</v>
+        <v>9.370000000000001</v>
       </c>
       <c r="R50" s="46">
         <v>0</v>
@@ -19003,7 +18986,7 @@
       </c>
       <c r="U50" s="46">
         <f>_xll.qlMidEquivalent($Q50,$R50,$S50,$T50)</f>
-        <v>9.5399999999999991</v>
+        <v>9.370000000000001</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -19011,7 +18994,7 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>9.5399999999999991</v>
+        <v>9.370000000000001</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/10000,Trigger)</f>
@@ -19063,7 +19046,7 @@
         <v>SEK3S6S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>8.82</v>
+        <v>8.68</v>
       </c>
       <c r="R51" s="46">
         <v>0</v>
@@ -19076,7 +19059,7 @@
       </c>
       <c r="U51" s="46">
         <f>_xll.qlMidEquivalent($Q51,$R51,$S51,$T51)</f>
-        <v>8.82</v>
+        <v>8.68</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -19084,7 +19067,7 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>8.82</v>
+        <v>8.68</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
@@ -19136,7 +19119,7 @@
         <v>SEK3S6S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>7.77</v>
+        <v>7.65</v>
       </c>
       <c r="R52" s="46">
         <v>0</v>
@@ -19149,7 +19132,7 @@
       </c>
       <c r="U52" s="46">
         <f>_xll.qlMidEquivalent($Q52,$R52,$S52,$T52)</f>
-        <v>7.77</v>
+        <v>7.65</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -19157,7 +19140,7 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>7.77</v>
+        <v>7.65</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/10000,Trigger)</f>
@@ -19209,7 +19192,7 @@
         <v>SEK3S6S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>7.01</v>
+        <v>6.92</v>
       </c>
       <c r="R53" s="46">
         <v>0</v>
@@ -19222,7 +19205,7 @@
       </c>
       <c r="U53" s="46">
         <f>_xll.qlMidEquivalent($Q53,$R53,$S53,$T53)</f>
-        <v>7.01</v>
+        <v>6.92</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -19230,7 +19213,7 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>7.01</v>
+        <v>6.92</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
@@ -19355,7 +19338,7 @@
         <v>SEK3S6S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>6.41</v>
+        <v>6.32</v>
       </c>
       <c r="R55" s="46">
         <v>0</v>
@@ -19368,7 +19351,7 @@
       </c>
       <c r="U55" s="46">
         <f>_xll.qlMidEquivalent($Q55,$R55,$S55,$T55)</f>
-        <v>6.41</v>
+        <v>6.32</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -19376,7 +19359,7 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>6.41</v>
+        <v>6.32</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/10000,Trigger)</f>
@@ -19950,7 +19933,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -19977,7 +19960,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 10:28:55</v>
+        <v>Updated at 15:52:28</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -22539,7 +22522,7 @@
         <v>SEK1S3S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>10.11</v>
+        <v>10.1</v>
       </c>
       <c r="R40" s="46">
         <v>0</v>
@@ -22552,7 +22535,7 @@
       </c>
       <c r="U40" s="46">
         <f>_xll.qlMidEquivalent($Q40,$R40,$S40,$T40)</f>
-        <v>10.11</v>
+        <v>10.1</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -22560,7 +22543,7 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>10.11</v>
+        <v>10.1</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
@@ -22831,7 +22814,7 @@
         <v>SEK1S3S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>10.16</v>
+        <v>10.15</v>
       </c>
       <c r="R44" s="46">
         <v>0</v>
@@ -22844,7 +22827,7 @@
       </c>
       <c r="U44" s="46">
         <f>_xll.qlMidEquivalent($Q44,$R44,$S44,$T44)</f>
-        <v>10.16</v>
+        <v>10.15</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -22852,7 +22835,7 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>10.16</v>
+        <v>10.15</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
@@ -22904,7 +22887,7 @@
         <v>SEK1S3S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="R45" s="46">
         <v>0</v>
@@ -22917,7 +22900,7 @@
       </c>
       <c r="U45" s="46">
         <f>_xll.qlMidEquivalent($Q45,$R45,$S45,$T45)</f>
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -22925,7 +22908,7 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
@@ -23050,7 +23033,7 @@
         <v>SEK1S3S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="R47" s="46">
         <v>0</v>
@@ -23063,7 +23046,7 @@
       </c>
       <c r="U47" s="46">
         <f>_xll.qlMidEquivalent($Q47,$R47,$S47,$T47)</f>
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -23071,11 +23054,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>10.18</v>
+        <v>10.17</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.0000000000001327E-6</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -23342,7 +23325,7 @@
         <v>SEK1S3S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>9.91</v>
+        <v>9.92</v>
       </c>
       <c r="R51" s="46">
         <v>0</v>
@@ -23355,7 +23338,7 @@
       </c>
       <c r="U51" s="46">
         <f>_xll.qlMidEquivalent($Q51,$R51,$S51,$T51)</f>
-        <v>9.91</v>
+        <v>9.92</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -23363,7 +23346,7 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>9.91</v>
+        <v>9.92</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
@@ -23488,7 +23471,7 @@
         <v>SEK1S3S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>8.9499999999999993</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="R53" s="46">
         <v>0</v>
@@ -23501,7 +23484,7 @@
       </c>
       <c r="U53" s="46">
         <f>_xll.qlMidEquivalent($Q53,$R53,$S53,$T53)</f>
-        <v>8.9499999999999993</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -23509,7 +23492,7 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>8.9499999999999993</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
@@ -23634,7 +23617,7 @@
         <v>SEK1S3S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>8.67</v>
+        <v>8.68</v>
       </c>
       <c r="R55" s="46">
         <v>0</v>
@@ -23647,7 +23630,7 @@
       </c>
       <c r="U55" s="46">
         <f>_xll.qlMidEquivalent($Q55,$R55,$S55,$T55)</f>
-        <v>8.67</v>
+        <v>8.68</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -23655,7 +23638,7 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>8.67</v>
+        <v>8.68</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/10000,Trigger)</f>

</xml_diff>

<commit_message>
SEK Market modified for negative rates
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="190">
   <si>
     <t>Currency</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>SIOR= is a chain. It must be requested separately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -1788,46 +1791,46 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 15:52:28</v>
+        <v>Updated at 09:25:07</v>
         <stp/>
-        <stp>{0FE0AD45-EC15-403D-BB11-A5491B13F846}</stp>
+        <stp>{B51EDCFF-A915-49AB-AAF4-837E709DDFD5}</stp>
+        <tr r="P5" s="66"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:25:07</v>
+        <stp/>
+        <stp>{1D3416D1-5DA5-4A84-A20C-DF84ADE45C57}</stp>
+        <tr r="O6" s="22"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:25:07</v>
+        <stp/>
+        <stp>{DD259B0A-751E-4597-BC2C-6D4A4E8445A4}</stp>
+        <tr r="N5" s="16"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:25:07</v>
+        <stp/>
+        <stp>{FB0569B8-6AC8-4782-897B-C360AD203C3B}</stp>
         <tr r="P5" s="69"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:57:43</v>
+        <v>Updated at 09:25:07</v>
         <stp/>
-        <stp>{D2E3642B-15D2-4619-86D5-E3A0BFBFEFD1}</stp>
+        <stp>{2F48653C-77B6-41ED-B8E4-065BC0D2314F}</stp>
+        <tr r="S3" s="64"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:25:07</v>
+        <stp/>
+        <stp>{7DA82CC9-E1FE-4A63-BF8B-C15F488B9368}</stp>
         <tr r="P5" s="67"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:58:43</v>
+        <v>Updated at 09:25:07</v>
         <stp/>
-        <stp>{D03E7A43-86EC-43D9-8887-9082AE3ACA30}</stp>
-        <tr r="O6" s="22"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:05:30</v>
-        <stp/>
-        <stp>{72E476C8-51A0-4F77-BABC-89C3B2D2301A}</stp>
-        <tr r="N5" s="16"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:05:30</v>
-        <stp/>
-        <stp>{09750DFC-EA08-4970-9B7F-3BFB05CF321E}</stp>
-        <tr r="S3" s="64"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:05:30</v>
-        <stp/>
-        <stp>{A36384B3-000D-4B3A-B43F-EAEC5AF36BC0}</stp>
+        <stp>{97700A76-B804-4895-A845-C4B8145E523B}</stp>
         <tr r="K5" s="15"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:58:43</v>
-        <stp/>
-        <stp>{037652E3-27F4-4CE1-8995-98610AE8EACF}</stp>
-        <tr r="P5" s="66"/>
       </tp>
     </main>
   </volType>
@@ -2151,14 +2154,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="75">
-        <v>42041.628310185188</v>
+        <v>42044.391979166663</v>
       </c>
       <c r="H3" s="114" t="s">
         <v>132</v>
       </c>
       <c r="I3" s="77">
         <f>_xll.ohTrigger(Deposits!S4,FRA3M!X4,OIS!Y5,Swaps3M!Z4,BasisSwap3M6M!Z4,BasisSwap1M3M!Z4)</f>
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2167,7 +2170,7 @@
       </c>
       <c r="I4" s="78">
         <f>_xll.ohTrigger(Stibor!W5:W10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -2205,7 +2208,7 @@
       </c>
       <c r="D8" s="85">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="E8" s="105"/>
       <c r="G8" s="97"/>
@@ -2637,7 +2640,7 @@
       </c>
       <c r="S3" s="183" t="str">
         <f>_xll.RData(S4:S10,T3:U3,"RTFEED:IDN",,,T4)</f>
-        <v>Updated at 15:05:30</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="T3" s="177" t="s">
         <v>137</v>
@@ -2727,11 +2730,11 @@
       </c>
       <c r="K5" s="123" t="str">
         <f>_xll.qlOvernightIndex(I5,,D5,Currency,Calendar,H5,J5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborON#0001</v>
+        <v>SekiborON#0000</v>
       </c>
       <c r="L5" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C5&amp;"LastFixing_Quote",K5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborONLastFixing_Quote#0001</v>
+        <v>SekiborONLastFixing_Quote#0000</v>
       </c>
       <c r="M5" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K5)</f>
@@ -2746,14 +2749,14 @@
       </c>
       <c r="R5" s="21" t="str">
         <f>K5</f>
-        <v>SekiborON#0001</v>
+        <v>SekiborON#0000</v>
       </c>
       <c r="S5" s="178" t="str">
         <f t="shared" ref="S5:S10" si="2">"STI"&amp;Currency&amp;Q5&amp;"DFI="</f>
         <v>STISEKTNDFI=</v>
       </c>
       <c r="T5" s="178">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U5" s="187">
         <v>3.6000000000000004E-2</v>
@@ -2827,10 +2830,10 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="T6" s="178">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U6" s="187">
-        <v>3.7000000000000005E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="V6" s="178" t="b">
         <f>IF(AND(ISNUMBER($U6),$U6&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2842,7 +2845,7 @@
       </c>
       <c r="X6" s="181">
         <f>_xll.qlQuoteValue(L6)</f>
-        <v>8.5999999999999998E-4</v>
+        <v>3.7000000000000005E-4</v>
       </c>
       <c r="Y6" s="8"/>
     </row>
@@ -2904,10 +2907,10 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="T7" s="178">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U7" s="187">
-        <v>1.1000000000000001E-2</v>
+        <v>-1.1000000000000001E-2</v>
       </c>
       <c r="V7" s="178" t="b">
         <f t="shared" ref="V7:V10" si="5">IF(AND(ISNUMBER($U7),$U7&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2919,7 +2922,7 @@
       </c>
       <c r="X7" s="181">
         <f>_xll.qlQuoteValue(L7)</f>
-        <v>1.4499999999999999E-3</v>
+        <v>1.1000000000000002E-4</v>
       </c>
       <c r="Y7" s="8"/>
     </row>
@@ -2978,10 +2981,10 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="T8" s="178">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U8" s="187">
-        <v>1.2E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="V8" s="178" t="b">
         <f t="shared" si="5"/>
@@ -2993,7 +2996,7 @@
       </c>
       <c r="X8" s="181">
         <f>_xll.qlQuoteValue(L8)</f>
-        <v>1.4399999999999999E-3</v>
+        <v>1.2E-4</v>
       </c>
       <c r="Y8" s="8"/>
     </row>
@@ -3055,10 +3058,10 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="T9" s="178">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U9" s="187">
-        <v>5.3999999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="V9" s="178" t="b">
         <f t="shared" si="5"/>
@@ -3070,7 +3073,7 @@
       </c>
       <c r="X9" s="181">
         <f>_xll.qlQuoteValue(L9)</f>
-        <v>2.0299999999999997E-3</v>
+        <v>5.4000000000000001E-4</v>
       </c>
       <c r="Y9" s="8"/>
     </row>
@@ -3132,10 +3135,10 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="T10" s="179">
-        <v>42040</v>
+        <v>42041</v>
       </c>
       <c r="U10" s="187">
-        <v>0.13300000000000001</v>
+        <v>0.129</v>
       </c>
       <c r="V10" s="179" t="b">
         <f t="shared" si="5"/>
@@ -3147,7 +3150,7 @@
       </c>
       <c r="X10" s="182">
         <f>_xll.qlQuoteValue(L10)</f>
-        <v>2.98E-3</v>
+        <v>1.33E-3</v>
       </c>
       <c r="Y10" s="8"/>
     </row>
@@ -4453,7 +4456,7 @@
   <dimension ref="B1:T28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4467,9 +4470,9 @@
     <col min="10" max="10" width="3.85546875" style="184" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.140625" style="184" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.7109375" style="184" customWidth="1"/>
-    <col min="14" max="14" width="7" style="184" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" style="184" customWidth="1"/>
     <col min="15" max="15" width="2.7109375" style="184" customWidth="1"/>
-    <col min="16" max="16" width="7" style="184" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="184" customWidth="1"/>
     <col min="17" max="17" width="2.7109375" style="184" customWidth="1"/>
     <col min="18" max="18" width="10" style="184" customWidth="1"/>
     <col min="19" max="19" width="9" style="184" bestFit="1" customWidth="1"/>
@@ -4544,7 +4547,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="33">
         <f>_xll.ohTrigger(S6:S23)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="T4" s="34"/>
     </row>
@@ -4566,7 +4569,7 @@
       <c r="J5" s="166"/>
       <c r="K5" s="176" t="str">
         <f>_xll.RData(K7:K23,L5:M5,,ReutersRtMode,,L7)</f>
-        <v>Updated at 15:05:30</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="L5" s="167" t="s">
         <v>106</v>
@@ -4577,7 +4580,9 @@
       <c r="N5" s="168" t="s">
         <v>139</v>
       </c>
-      <c r="O5" s="32"/>
+      <c r="O5" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P5" s="168" t="s">
         <v>121</v>
       </c>
@@ -4618,16 +4623,18 @@
       </c>
       <c r="L6" s="152"/>
       <c r="M6" s="152"/>
-      <c r="N6" s="40" t="e">
-        <f>_xll.qlMidEquivalent(L6,M6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O6" s="32"/>
+      <c r="N6" s="39" t="e">
+        <f>IF(ISNUMBER(L6),L6,#NUM!)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P6" s="40" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q6" s="32"/>
-      <c r="R6" s="40" t="e">
+      <c r="R6" s="39" t="e">
         <f t="array" ref="R6:R23">QuoteLive</f>
         <v>#NUM!</v>
       </c>
@@ -4668,21 +4675,23 @@
       <c r="M7" s="153">
         <v>0</v>
       </c>
-      <c r="N7" s="47">
-        <f>_xll.qlMidEquivalent(L7,M7)</f>
+      <c r="N7" s="46">
+        <f t="shared" ref="N7:N23" si="1">IF(ISNUMBER(L7),L7,#NUM!)</f>
         <v>3.6000000000000004E-2</v>
       </c>
-      <c r="O7" s="32"/>
+      <c r="O7" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P7" s="47">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="Q7" s="32"/>
-      <c r="R7" s="47">
+      <c r="R7" s="46">
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="S7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E7,R7/100,Trigger)</f>
-        <v>-2.9999999999999987E-4</v>
+        <v>0</v>
       </c>
       <c r="T7" s="34"/>
     </row>
@@ -4717,16 +4726,18 @@
       <c r="M8" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N8" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L8,M8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O8" s="32"/>
+      <c r="N8" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P8" s="47" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q8" s="32"/>
-      <c r="R8" s="47" t="e">
+      <c r="R8" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S8" s="48">
@@ -4761,26 +4772,28 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="L9" s="153">
-        <v>3.7000000000000005E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M9" s="153">
         <v>0</v>
       </c>
-      <c r="N9" s="47">
-        <f>_xll.qlMidEquivalent(L9,M9)</f>
-        <v>3.7000000000000005E-2</v>
-      </c>
-      <c r="O9" s="32"/>
+      <c r="N9" s="46">
+        <f t="shared" si="1"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P9" s="47">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="Q9" s="32"/>
-      <c r="R9" s="47">
-        <v>3.7000000000000005E-2</v>
+      <c r="R9" s="46">
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="S9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E9,R9/100,Trigger)</f>
-        <v>-4.8999999999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="T9" s="34"/>
     </row>
@@ -4815,16 +4828,18 @@
       <c r="M10" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N10" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L10,M10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O10" s="32"/>
+      <c r="N10" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>189</v>
+      </c>
       <c r="P10" s="47" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q10" s="32"/>
-      <c r="R10" s="47" t="e">
+      <c r="R10" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S10" s="48">
@@ -4864,16 +4879,18 @@
       <c r="M11" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N11" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L11,M11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O11" s="32"/>
+      <c r="N11" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P11" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q11" s="32"/>
-      <c r="R11" s="47" t="e">
+      <c r="R11" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S11" s="48">
@@ -4908,26 +4925,28 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="L12" s="153">
-        <v>1.1000000000000001E-2</v>
+        <v>-1.1000000000000001E-2</v>
       </c>
       <c r="M12" s="153">
         <v>0</v>
       </c>
-      <c r="N12" s="47">
-        <f>_xll.qlMidEquivalent(L12,M12)</f>
-        <v>1.1000000000000001E-2</v>
-      </c>
-      <c r="O12" s="32"/>
+      <c r="N12" s="46">
+        <f t="shared" si="1"/>
+        <v>-1.1000000000000001E-2</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P12" s="154">
         <v>0.151</v>
       </c>
       <c r="Q12" s="32"/>
-      <c r="R12" s="47">
-        <v>1.1000000000000001E-2</v>
+      <c r="R12" s="46">
+        <v>-1.1000000000000001E-2</v>
       </c>
       <c r="S12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E12,R12/100,Trigger)</f>
-        <v>-1.3399999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="T12" s="34"/>
     </row>
@@ -4957,26 +4976,28 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="L13" s="153">
-        <v>1.2E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="M13" s="153">
         <v>0</v>
       </c>
-      <c r="N13" s="47">
-        <f>_xll.qlMidEquivalent(L13,M13)</f>
-        <v>1.2E-2</v>
-      </c>
-      <c r="O13" s="32"/>
+      <c r="N13" s="46">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P13" s="154">
         <v>0.191</v>
       </c>
       <c r="Q13" s="32"/>
-      <c r="R13" s="47">
-        <v>1.2E-2</v>
+      <c r="R13" s="46">
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="S13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E13,R13/100,Trigger)</f>
-        <v>-1.3199999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="T13" s="34"/>
     </row>
@@ -5006,26 +5027,28 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="L14" s="153">
-        <v>5.3999999999999999E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M14" s="153">
         <v>0</v>
       </c>
-      <c r="N14" s="47">
-        <f>_xll.qlMidEquivalent(L14,M14)</f>
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="O14" s="32"/>
+      <c r="N14" s="46">
+        <f t="shared" si="1"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P14" s="154">
         <v>0.255</v>
       </c>
       <c r="Q14" s="32"/>
-      <c r="R14" s="47">
-        <v>5.3999999999999999E-2</v>
+      <c r="R14" s="46">
+        <v>4.7E-2</v>
       </c>
       <c r="S14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E14,R14/100,Trigger)</f>
-        <v>-1.4899999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="T14" s="34"/>
     </row>
@@ -5060,16 +5083,18 @@
       <c r="M15" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N15" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L15,M15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O15" s="32"/>
+      <c r="N15" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O15" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P15" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q15" s="32"/>
-      <c r="R15" s="47" t="e">
+      <c r="R15" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S15" s="48">
@@ -5109,16 +5134,18 @@
       <c r="M16" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N16" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L16,M16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O16" s="32"/>
+      <c r="N16" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P16" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q16" s="32"/>
-      <c r="R16" s="47" t="e">
+      <c r="R16" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S16" s="48">
@@ -5153,26 +5180,28 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="L17" s="153">
-        <v>0.13300000000000001</v>
+        <v>0.129</v>
       </c>
       <c r="M17" s="153">
         <v>0</v>
       </c>
-      <c r="N17" s="47">
-        <f>_xll.qlMidEquivalent(L17,M17)</f>
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="O17" s="32"/>
+      <c r="N17" s="46">
+        <f t="shared" si="1"/>
+        <v>0.129</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P17" s="154">
         <v>0.33799999999999997</v>
       </c>
       <c r="Q17" s="32"/>
-      <c r="R17" s="47">
-        <v>0.13300000000000001</v>
+      <c r="R17" s="46">
+        <v>0.129</v>
       </c>
       <c r="S17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E17,R17/100,Trigger)</f>
-        <v>-1.65E-3</v>
+        <v>0</v>
       </c>
       <c r="T17" s="34"/>
     </row>
@@ -5207,16 +5236,18 @@
       <c r="M18" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N18" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L18,M18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O18" s="32"/>
+      <c r="N18" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P18" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q18" s="32"/>
-      <c r="R18" s="47" t="e">
+      <c r="R18" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S18" s="48">
@@ -5256,16 +5287,18 @@
       <c r="M19" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N19" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L19,M19)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O19" s="32"/>
+      <c r="N19" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P19" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q19" s="32"/>
-      <c r="R19" s="47" t="e">
+      <c r="R19" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S19" s="48">
@@ -5305,16 +5338,18 @@
       <c r="M20" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N20" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L20,M20)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O20" s="32"/>
+      <c r="N20" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P20" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q20" s="32"/>
-      <c r="R20" s="47" t="e">
+      <c r="R20" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S20" s="48">
@@ -5354,16 +5389,18 @@
       <c r="M21" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N21" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L21,M21)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O21" s="32"/>
+      <c r="N21" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O21" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P21" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q21" s="32"/>
-      <c r="R21" s="47" t="e">
+      <c r="R21" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S21" s="48">
@@ -5403,16 +5440,18 @@
       <c r="M22" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N22" s="47" t="e">
-        <f>_xll.qlMidEquivalent(L22,M22)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O22" s="32"/>
+      <c r="N22" s="46" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O22" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P22" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q22" s="32"/>
-      <c r="R22" s="47" t="e">
+      <c r="R22" s="46" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S22" s="48">
@@ -5452,16 +5491,18 @@
       <c r="M23" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="N23" s="54" t="e">
-        <f>_xll.qlMidEquivalent(L23,M23)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O23" s="32"/>
+      <c r="N23" s="53" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O23" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="P23" s="154" t="e">
         <v>#NUM!</v>
       </c>
       <c r="Q23" s="32"/>
-      <c r="R23" s="54" t="e">
+      <c r="R23" s="53" t="e">
         <v>#NUM!</v>
       </c>
       <c r="S23" s="55">
@@ -5483,7 +5524,9 @@
       <c r="L24" s="155"/>
       <c r="M24" s="155"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="O24" s="10" t="s">
+        <v>154</v>
+      </c>
       <c r="P24" s="155"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="155"/>
@@ -5523,7 +5566,7 @@
   <dimension ref="B1:AF21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5678,7 +5721,7 @@
       <c r="M5" s="175"/>
       <c r="N5" s="176" t="str">
         <f>_xll.RData(N6:N20,O5:R5,"RTFEED:IDN",ReutersRtMode,,O6)</f>
-        <v>Updated at 15:05:30</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="O5" s="168" t="s">
         <v>106</v>
@@ -5761,10 +5804,10 @@
         <v>SEK3F1=HBCO</v>
       </c>
       <c r="O6" s="39">
-        <v>5.5E-2</v>
+        <v>5.2500000000000005E-2</v>
       </c>
       <c r="P6" s="39">
-        <v>7.4999999999999997E-2</v>
+        <v>7.2500000000000009E-2</v>
       </c>
       <c r="Q6" s="37">
         <v>0</v>
@@ -5774,7 +5817,7 @@
       </c>
       <c r="S6" s="39">
         <f>IF(ISERROR(AVERAGE(O6,P6)),#NUM!,AVERAGE(O6,P6))</f>
-        <v>6.5000000000000002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="T6" s="32"/>
       <c r="U6" s="40">
@@ -5783,11 +5826,11 @@
       <c r="V6" s="32"/>
       <c r="W6" s="40">
         <f t="array" ref="W6:W20">QuoteLive</f>
-        <v>6.5000000000000002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="X6" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/100,Trigger)</f>
-        <v>-9.4999999999999989E-4</v>
+        <v>-2.4999999999999957E-5</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="AA6" s="28"/>
@@ -5801,11 +5844,11 @@
       </c>
       <c r="AD6" s="199">
         <f>100-W6</f>
-        <v>99.935000000000002</v>
+        <v>99.9375</v>
       </c>
       <c r="AE6" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC6,AD6,Trigger)</f>
-        <v>9.4999999999998863E-2</v>
+        <v>2.4999999999977263E-3</v>
       </c>
       <c r="AF6" s="59"/>
     </row>
@@ -5847,10 +5890,10 @@
         <v>SEK3F2=HBCO</v>
       </c>
       <c r="O7" s="46">
-        <v>3.0000000000000002E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="P7" s="46">
-        <v>0.05</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="Q7" s="44">
         <v>0</v>
@@ -5860,7 +5903,7 @@
       </c>
       <c r="S7" s="46">
         <f t="shared" ref="S7:S20" si="4">IF(ISERROR(AVERAGE(O7,P7)),#NUM!,AVERAGE(O7,P7))</f>
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T7" s="32"/>
       <c r="U7" s="47">
@@ -5868,11 +5911,11 @@
       </c>
       <c r="V7" s="32"/>
       <c r="W7" s="47">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="X7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F7,W7/100,Trigger)</f>
-        <v>-8.25E-4</v>
+        <v>-4.9999999999999969E-5</v>
       </c>
       <c r="Y7" s="34"/>
       <c r="AA7" s="28"/>
@@ -5886,11 +5929,11 @@
       </c>
       <c r="AD7" s="200">
         <f t="shared" ref="AD7:AD20" si="6">100-W7</f>
-        <v>99.96</v>
+        <v>99.965000000000003</v>
       </c>
       <c r="AE7" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC7,AD7,Trigger)</f>
-        <v>8.2499999999996021E-2</v>
+        <v>5.0000000000096634E-3</v>
       </c>
       <c r="AF7" s="59"/>
     </row>
@@ -5932,10 +5975,10 @@
         <v>SEK3F3=HBCO</v>
       </c>
       <c r="O8" s="46">
-        <v>3.0000000000000002E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="P8" s="46">
-        <v>0.05</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="Q8" s="44">
         <v>0</v>
@@ -5945,7 +5988,7 @@
       </c>
       <c r="S8" s="46">
         <f t="shared" si="4"/>
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T8" s="32"/>
       <c r="U8" s="47">
@@ -5953,11 +5996,11 @@
       </c>
       <c r="V8" s="32"/>
       <c r="W8" s="47">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="X8" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F8,W8/100,Trigger)</f>
-        <v>-7.2500000000000017E-4</v>
+        <v>-4.9999999999999969E-5</v>
       </c>
       <c r="Y8" s="34"/>
       <c r="AA8" s="28"/>
@@ -5971,11 +6014,11 @@
       </c>
       <c r="AD8" s="200">
         <f t="shared" si="6"/>
-        <v>99.96</v>
+        <v>99.965000000000003</v>
       </c>
       <c r="AE8" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC8,AD8,Trigger)</f>
-        <v>7.2499999999990905E-2</v>
+        <v>5.0000000000096634E-3</v>
       </c>
       <c r="AF8" s="59"/>
     </row>
@@ -6017,10 +6060,10 @@
         <v>SEK3F4=HBCO</v>
       </c>
       <c r="O9" s="46">
-        <v>4.5000000000000005E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="P9" s="46">
-        <v>6.5000000000000002E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="Q9" s="44">
         <v>0</v>
@@ -6030,7 +6073,7 @@
       </c>
       <c r="S9" s="46">
         <f t="shared" si="4"/>
-        <v>5.5000000000000007E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="T9" s="32"/>
       <c r="U9" s="47">
@@ -6038,11 +6081,11 @@
       </c>
       <c r="V9" s="32"/>
       <c r="W9" s="47">
-        <v>5.5000000000000007E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="X9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F9,W9/100,Trigger)</f>
-        <v>-5.5000000000000003E-4</v>
+        <v>-1.0000000000000005E-4</v>
       </c>
       <c r="Y9" s="34"/>
       <c r="AA9" s="28"/>
@@ -6056,11 +6099,11 @@
       </c>
       <c r="AD9" s="200">
         <f t="shared" si="6"/>
-        <v>99.944999999999993</v>
+        <v>99.954999999999998</v>
       </c>
       <c r="AE9" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC9,AD9,Trigger)</f>
-        <v>5.499999999999261E-2</v>
+        <v>1.0000000000005116E-2</v>
       </c>
       <c r="AF9" s="59"/>
     </row>
@@ -6102,10 +6145,10 @@
         <v>SEK3F5=HBCO</v>
       </c>
       <c r="O10" s="46">
-        <v>6.7500000000000004E-2</v>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="P10" s="46">
-        <v>9.7500000000000003E-2</v>
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="Q10" s="44">
         <v>0</v>
@@ -6115,7 +6158,7 @@
       </c>
       <c r="S10" s="46">
         <f t="shared" si="4"/>
-        <v>8.2500000000000004E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="T10" s="32"/>
       <c r="U10" s="47">
@@ -6123,11 +6166,11 @@
       </c>
       <c r="V10" s="32"/>
       <c r="W10" s="47">
-        <v>8.2500000000000004E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="X10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/100,Trigger)</f>
-        <v>-3.4999999999999983E-4</v>
+        <v>-7.4999999999999871E-5</v>
       </c>
       <c r="Y10" s="34"/>
       <c r="AA10" s="28"/>
@@ -6141,11 +6184,11 @@
       </c>
       <c r="AD10" s="200">
         <f t="shared" si="6"/>
-        <v>99.917500000000004</v>
+        <v>99.924999999999997</v>
       </c>
       <c r="AE10" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC10,AD10,Trigger)</f>
-        <v>3.50000000000108E-2</v>
+        <v>7.4999999999931788E-3</v>
       </c>
       <c r="AF10" s="59"/>
     </row>
@@ -6187,10 +6230,10 @@
         <v>SEK3F6=HBCO</v>
       </c>
       <c r="O11" s="46">
-        <v>0.10500000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="P11" s="46">
-        <v>0.13500000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="Q11" s="44">
         <v>0</v>
@@ -6200,7 +6243,7 @@
       </c>
       <c r="S11" s="46">
         <f t="shared" si="4"/>
-        <v>0.12000000000000001</v>
+        <v>0.115</v>
       </c>
       <c r="T11" s="32"/>
       <c r="U11" s="47">
@@ -6208,11 +6251,11 @@
       </c>
       <c r="V11" s="32"/>
       <c r="W11" s="47">
-        <v>0.12000000000000001</v>
+        <v>0.115</v>
       </c>
       <c r="X11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/100,Trigger)</f>
-        <v>-1.4999999999999996E-4</v>
+        <v>-5.0000000000000131E-5</v>
       </c>
       <c r="Y11" s="34"/>
       <c r="AA11" s="28"/>
@@ -6226,11 +6269,11 @@
       </c>
       <c r="AD11" s="200">
         <f t="shared" si="6"/>
-        <v>99.88</v>
+        <v>99.885000000000005</v>
       </c>
       <c r="AE11" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC11,AD11,Trigger)</f>
-        <v>1.5000000000000568E-2</v>
+        <v>5.0000000000096634E-3</v>
       </c>
       <c r="AF11" s="59"/>
     </row>
@@ -6297,7 +6340,7 @@
       </c>
       <c r="X12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/100,Trigger)</f>
-        <v>-4.9999999999999914E-5</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="34"/>
       <c r="AA12" s="28"/>
@@ -6315,7 +6358,7 @@
       </c>
       <c r="AE12" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC12,AD12,Trigger)</f>
-        <v>4.9999999999954525E-3</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="59"/>
     </row>
@@ -6357,10 +6400,10 @@
         <v>SEK3F8=HBCO</v>
       </c>
       <c r="O13" s="46">
-        <v>0.215</v>
+        <v>0.22</v>
       </c>
       <c r="P13" s="46">
-        <v>0.24500000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="Q13" s="44">
         <v>0</v>
@@ -6370,7 +6413,7 @@
       </c>
       <c r="S13" s="46">
         <f t="shared" si="4"/>
-        <v>0.23</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="T13" s="32"/>
       <c r="U13" s="47">
@@ -6378,7 +6421,7 @@
       </c>
       <c r="V13" s="32"/>
       <c r="W13" s="47">
-        <v>0.23</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="X13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/100,Trigger)</f>
@@ -6396,11 +6439,11 @@
       </c>
       <c r="AD13" s="200">
         <f t="shared" si="6"/>
-        <v>99.77</v>
+        <v>99.765000000000001</v>
       </c>
       <c r="AE13" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC13,AD13,Trigger)</f>
-        <v>-5.0000000000096634E-3</v>
+        <v>-4.9999999999954525E-3</v>
       </c>
       <c r="AF13" s="59"/>
     </row>
@@ -6467,7 +6510,7 @@
       </c>
       <c r="X14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,W14/100,Trigger)</f>
-        <v>1.7500000000000068E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="34"/>
       <c r="AA14" s="28"/>
@@ -6485,7 +6528,7 @@
       </c>
       <c r="AE14" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC14,AD14,Trigger)</f>
-        <v>-1.7499999999998295E-2</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="59"/>
     </row>
@@ -6527,10 +6570,10 @@
         <v>SEK3F10=HBCO</v>
       </c>
       <c r="O15" s="46">
-        <v>0.35750000000000004</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="P15" s="46">
-        <v>0.39750000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="Q15" s="44">
         <v>0</v>
@@ -6540,7 +6583,7 @@
       </c>
       <c r="S15" s="46">
         <f t="shared" si="4"/>
-        <v>0.37750000000000006</v>
+        <v>0.37</v>
       </c>
       <c r="T15" s="32"/>
       <c r="U15" s="47">
@@ -6548,11 +6591,11 @@
       </c>
       <c r="V15" s="32"/>
       <c r="W15" s="47">
-        <v>0.37750000000000006</v>
+        <v>0.37</v>
       </c>
       <c r="X15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/100,Trigger)</f>
-        <v>3.0000000000000035E-4</v>
+        <v>-7.5000000000000414E-5</v>
       </c>
       <c r="Y15" s="34"/>
       <c r="AA15" s="28"/>
@@ -6566,11 +6609,11 @@
       </c>
       <c r="AD15" s="200">
         <f t="shared" si="6"/>
-        <v>99.622500000000002</v>
+        <v>99.63</v>
       </c>
       <c r="AE15" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC15,AD15,Trigger)</f>
-        <v>-3.0000000000001137E-2</v>
+        <v>7.4999999999931788E-3</v>
       </c>
       <c r="AF15" s="59"/>
     </row>
@@ -6612,10 +6655,10 @@
         <v>SEK3F11=HBCO</v>
       </c>
       <c r="O16" s="46">
-        <v>0.4375</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="P16" s="46">
-        <v>0.47750000000000004</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="Q16" s="44">
         <v>0</v>
@@ -6625,7 +6668,7 @@
       </c>
       <c r="S16" s="46">
         <f t="shared" si="4"/>
-        <v>0.45750000000000002</v>
+        <v>0.44500000000000006</v>
       </c>
       <c r="T16" s="32"/>
       <c r="U16" s="47">
@@ -6633,11 +6676,11 @@
       </c>
       <c r="V16" s="32"/>
       <c r="W16" s="47">
-        <v>0.45750000000000002</v>
+        <v>0.44500000000000006</v>
       </c>
       <c r="X16" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F16,W16/100,Trigger)</f>
-        <v>3.7499999999999947E-4</v>
+        <v>-1.2499999999999924E-4</v>
       </c>
       <c r="Y16" s="34"/>
       <c r="AA16" s="28"/>
@@ -6651,11 +6694,11 @@
       </c>
       <c r="AD16" s="200">
         <f t="shared" si="6"/>
-        <v>99.542500000000004</v>
+        <v>99.555000000000007</v>
       </c>
       <c r="AE16" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC16,AD16,Trigger)</f>
-        <v>-3.7499999999994316E-2</v>
+        <v>1.2500000000002842E-2</v>
       </c>
       <c r="AF16" s="59"/>
     </row>
@@ -6697,10 +6740,10 @@
         <v>SEK3F12=HBCO</v>
       </c>
       <c r="O17" s="46">
-        <v>0.51750000000000007</v>
+        <v>0.5</v>
       </c>
       <c r="P17" s="46">
-        <v>0.5575</v>
+        <v>0.54</v>
       </c>
       <c r="Q17" s="44">
         <v>0</v>
@@ -6710,7 +6753,7 @@
       </c>
       <c r="S17" s="46">
         <f t="shared" si="4"/>
-        <v>0.53750000000000009</v>
+        <v>0.52</v>
       </c>
       <c r="T17" s="32"/>
       <c r="U17" s="47">
@@ -6718,11 +6761,11 @@
       </c>
       <c r="V17" s="32"/>
       <c r="W17" s="47">
-        <v>0.53750000000000009</v>
+        <v>0.52</v>
       </c>
       <c r="X17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F17,W17/100,Trigger)</f>
-        <v>4.0000000000000105E-4</v>
+        <v>-1.7500000000000154E-4</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="AA17" s="28"/>
@@ -6736,11 +6779,11 @@
       </c>
       <c r="AD17" s="200">
         <f t="shared" si="6"/>
-        <v>99.462500000000006</v>
+        <v>99.48</v>
       </c>
       <c r="AE17" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC17,AD17,Trigger)</f>
-        <v>-3.9999999999992042E-2</v>
+        <v>1.7499999999998295E-2</v>
       </c>
       <c r="AF17" s="59"/>
     </row>
@@ -7056,7 +7099,7 @@
   <dimension ref="B1:AC99"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7191,7 +7234,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="33">
         <f>_xll.ohTrigger(Y7:Y61)</f>
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="34"/>
     </row>
@@ -7217,7 +7260,7 @@
       <c r="N6" s="234"/>
       <c r="O6" s="235" t="str">
         <f>_xll.RData(O7:O61,P6:S6,"RTFEED:IDN",ReutersRtMode,,P7)</f>
-        <v>Updated at 15:58:43</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="P6" s="190" t="s">
         <v>106</v>
@@ -7500,10 +7543,10 @@
         <v>SEKAMTNS1M=HBCO</v>
       </c>
       <c r="P10" s="46">
-        <v>-7.0000000000000001E-3</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="Q10" s="46">
-        <v>2.3E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="R10" s="46">
         <v>0</v>
@@ -7513,7 +7556,7 @@
       </c>
       <c r="T10" s="46">
         <f t="shared" si="2"/>
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="U10" s="231"/>
       <c r="V10" s="233">
@@ -7521,11 +7564,11 @@
       </c>
       <c r="W10" s="231"/>
       <c r="X10" s="46">
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,X10/100,Trigger)</f>
-        <v>0</v>
+        <v>-4.0000000000000003E-5</v>
       </c>
       <c r="Z10" s="34"/>
       <c r="AB10" s="237"/>
@@ -7571,10 +7614,10 @@
         <v>SEKAMTNS2M=HBCO</v>
       </c>
       <c r="P11" s="46">
-        <v>-2.1999999999999999E-2</v>
+        <v>-2.4E-2</v>
       </c>
       <c r="Q11" s="46">
-        <v>8.0000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="R11" s="46">
         <v>0</v>
@@ -7584,7 +7627,7 @@
       </c>
       <c r="T11" s="46">
         <f t="shared" si="2"/>
-        <v>-6.9999999999999993E-3</v>
+        <v>-9.0000000000000011E-3</v>
       </c>
       <c r="U11" s="231"/>
       <c r="V11" s="233">
@@ -7592,11 +7635,11 @@
       </c>
       <c r="W11" s="231"/>
       <c r="X11" s="46">
-        <v>-6.9999999999999993E-3</v>
+        <v>-9.0000000000000011E-3</v>
       </c>
       <c r="Y11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.0000000000000012E-5</v>
       </c>
       <c r="Z11" s="34"/>
     </row>
@@ -7641,10 +7684,10 @@
         <v>SEKAMTNS3M=HBCO</v>
       </c>
       <c r="P12" s="46">
-        <v>-2.8000000000000001E-2</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="Q12" s="46">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="R12" s="46">
         <v>0</v>
@@ -7654,7 +7697,7 @@
       </c>
       <c r="T12" s="46">
         <f t="shared" si="2"/>
-        <v>-1.3000000000000001E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="U12" s="231"/>
       <c r="V12" s="233">
@@ -7662,11 +7705,11 @@
       </c>
       <c r="W12" s="231"/>
       <c r="X12" s="46">
-        <v>-1.3000000000000001E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="Y12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
-        <v>0</v>
+        <v>-9.9999999999999991E-6</v>
       </c>
       <c r="Z12" s="34"/>
     </row>
@@ -7711,10 +7754,10 @@
         <v>SEKAMTNS4M=HBCO</v>
       </c>
       <c r="P13" s="46">
-        <v>-3.6999999999999998E-2</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="Q13" s="46">
-        <v>-7.0000000000000001E-3</v>
+        <v>-9.0000000000000011E-3</v>
       </c>
       <c r="R13" s="46">
         <v>0</v>
@@ -7724,7 +7767,7 @@
       </c>
       <c r="T13" s="46">
         <f t="shared" si="2"/>
-        <v>-2.1999999999999999E-2</v>
+        <v>-2.4E-2</v>
       </c>
       <c r="U13" s="231"/>
       <c r="V13" s="233">
@@ -7732,11 +7775,11 @@
       </c>
       <c r="W13" s="231"/>
       <c r="X13" s="46">
-        <v>-2.1999999999999999E-2</v>
+        <v>-2.4E-2</v>
       </c>
       <c r="Y13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,X13/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.0000000000000025E-5</v>
       </c>
       <c r="Z13" s="34"/>
     </row>
@@ -7781,10 +7824,10 @@
         <v>SEKAMTNS5M=HBCO</v>
       </c>
       <c r="P14" s="46">
-        <v>-4.3000000000000003E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="Q14" s="46">
-        <v>-1.3000000000000001E-2</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="R14" s="46">
         <v>0</v>
@@ -7794,7 +7837,7 @@
       </c>
       <c r="T14" s="46">
         <f t="shared" si="2"/>
-        <v>-2.8000000000000004E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="U14" s="231"/>
       <c r="V14" s="233">
@@ -7802,11 +7845,11 @@
       </c>
       <c r="W14" s="231"/>
       <c r="X14" s="46">
-        <v>-2.8000000000000004E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="Y14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,X14/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.9999999999999944E-5</v>
       </c>
       <c r="Z14" s="34"/>
     </row>
@@ -7851,10 +7894,10 @@
         <v>SEKAMTNS6M=HBCO</v>
       </c>
       <c r="P15" s="46">
-        <v>-4.8000000000000001E-2</v>
+        <v>-5.1000000000000004E-2</v>
       </c>
       <c r="Q15" s="46">
-        <v>-1.8000000000000002E-2</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="R15" s="46">
         <v>0</v>
@@ -7864,7 +7907,7 @@
       </c>
       <c r="T15" s="46">
         <f t="shared" si="2"/>
-        <v>-3.3000000000000002E-2</v>
+        <v>-3.6000000000000004E-2</v>
       </c>
       <c r="U15" s="231"/>
       <c r="V15" s="233">
@@ -7872,11 +7915,11 @@
       </c>
       <c r="W15" s="231"/>
       <c r="X15" s="46">
-        <v>-3.3000000000000002E-2</v>
+        <v>-3.6000000000000004E-2</v>
       </c>
       <c r="Y15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,X15/100,Trigger)</f>
-        <v>0</v>
+        <v>-3.0000000000000024E-5</v>
       </c>
       <c r="Z15" s="34"/>
     </row>
@@ -8062,10 +8105,10 @@
         <v>SEKAMTNS9M=HBCO</v>
       </c>
       <c r="P18" s="46">
-        <v>-5.7000000000000002E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="Q18" s="46">
-        <v>-2.7E-2</v>
+        <v>-0.03</v>
       </c>
       <c r="R18" s="46">
         <v>0</v>
@@ -8075,7 +8118,7 @@
       </c>
       <c r="T18" s="46">
         <f t="shared" si="2"/>
-        <v>-4.2000000000000003E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="U18" s="231"/>
       <c r="V18" s="233">
@@ -8083,11 +8126,11 @@
       </c>
       <c r="W18" s="231"/>
       <c r="X18" s="46">
-        <v>-4.2000000000000003E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="Y18" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F18,X18/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.999999999999997E-5</v>
       </c>
       <c r="Z18" s="34"/>
       <c r="AC18" s="237"/>
@@ -8273,10 +8316,10 @@
         <v>SEKAMTNS12M=HBCO</v>
       </c>
       <c r="P21" s="46">
-        <v>-6.0999999999999999E-2</v>
+        <v>-6.6000000000000003E-2</v>
       </c>
       <c r="Q21" s="46">
-        <v>-3.1E-2</v>
+        <v>-3.6000000000000004E-2</v>
       </c>
       <c r="R21" s="46">
         <v>0</v>
@@ -8286,7 +8329,7 @@
       </c>
       <c r="T21" s="46">
         <f t="shared" si="2"/>
-        <v>-4.5999999999999999E-2</v>
+        <v>-5.1000000000000004E-2</v>
       </c>
       <c r="U21" s="231"/>
       <c r="V21" s="233">
@@ -8294,11 +8337,11 @@
       </c>
       <c r="W21" s="231"/>
       <c r="X21" s="46">
-        <v>-4.5999999999999999E-2</v>
+        <v>-5.1000000000000004E-2</v>
       </c>
       <c r="Y21" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F21,X21/100,Trigger)</f>
-        <v>0</v>
+        <v>-5.0000000000000023E-5</v>
       </c>
       <c r="Z21" s="34"/>
     </row>
@@ -8342,7 +8385,7 @@
         <v>SEKAMTNS1Y=ICAP</v>
       </c>
       <c r="P22" s="39">
-        <v>-4.5000000000000005E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="Q22" s="39">
         <v>0</v>
@@ -8355,7 +8398,7 @@
       </c>
       <c r="T22" s="39">
         <f t="shared" si="2"/>
-        <v>-2.2500000000000003E-2</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="U22" s="231"/>
       <c r="V22" s="232">
@@ -8363,11 +8406,11 @@
       </c>
       <c r="W22" s="231"/>
       <c r="X22" s="39">
-        <v>-2.2500000000000003E-2</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="Y22" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F22,X22/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999999984E-5</v>
       </c>
       <c r="Z22" s="34"/>
     </row>
@@ -9463,7 +9506,7 @@
         <v>SEKAMTNS3Y=ICAP</v>
       </c>
       <c r="P38" s="46">
-        <v>-2.75E-2</v>
+        <v>-3.0000000000000002E-2</v>
       </c>
       <c r="Q38" s="46">
         <v>0</v>
@@ -9476,7 +9519,7 @@
       </c>
       <c r="T38" s="46">
         <f t="shared" si="2"/>
-        <v>-1.375E-2</v>
+        <v>-1.5000000000000001E-2</v>
       </c>
       <c r="U38" s="231"/>
       <c r="V38" s="233">
@@ -9484,11 +9527,11 @@
       </c>
       <c r="W38" s="231"/>
       <c r="X38" s="46">
-        <v>-1.375E-2</v>
+        <v>-1.5000000000000001E-2</v>
       </c>
       <c r="Y38" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F38,X38/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.2500000000000006E-5</v>
       </c>
       <c r="Z38" s="34"/>
     </row>
@@ -9743,7 +9786,7 @@
         <v>SEKAMTNS4Y=ICAP</v>
       </c>
       <c r="P42" s="46">
-        <v>8.2500000000000004E-2</v>
+        <v>0.08</v>
       </c>
       <c r="Q42" s="46">
         <v>0</v>
@@ -9756,7 +9799,7 @@
       </c>
       <c r="T42" s="46">
         <f t="shared" si="2"/>
-        <v>4.1250000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="U42" s="231"/>
       <c r="V42" s="233">
@@ -9764,11 +9807,11 @@
       </c>
       <c r="W42" s="231"/>
       <c r="X42" s="46">
-        <v>4.1250000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="Y42" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F42,X42/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.2499999999999979E-5</v>
       </c>
       <c r="Z42" s="34"/>
     </row>
@@ -10023,7 +10066,7 @@
         <v>SEKAMTNS5Y=ICAP</v>
       </c>
       <c r="P46" s="46">
-        <v>0.21250000000000002</v>
+        <v>0.20750000000000002</v>
       </c>
       <c r="Q46" s="46">
         <v>0</v>
@@ -10036,7 +10079,7 @@
       </c>
       <c r="T46" s="46">
         <f t="shared" si="2"/>
-        <v>0.10625000000000001</v>
+        <v>0.10375000000000001</v>
       </c>
       <c r="U46" s="231"/>
       <c r="V46" s="233">
@@ -10044,11 +10087,11 @@
       </c>
       <c r="W46" s="231"/>
       <c r="X46" s="46">
-        <v>0.10625000000000001</v>
+        <v>0.10375000000000001</v>
       </c>
       <c r="Y46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.5000000000000066E-5</v>
       </c>
       <c r="Z46" s="34"/>
     </row>
@@ -10093,7 +10136,7 @@
         <v>SEKAMTNS6Y=ICAP</v>
       </c>
       <c r="P47" s="46">
-        <v>0.34500000000000003</v>
+        <v>0.34250000000000003</v>
       </c>
       <c r="Q47" s="46">
         <v>0</v>
@@ -10106,7 +10149,7 @@
       </c>
       <c r="T47" s="46">
         <f t="shared" si="2"/>
-        <v>0.17250000000000001</v>
+        <v>0.17125000000000001</v>
       </c>
       <c r="U47" s="231"/>
       <c r="V47" s="233">
@@ -10114,11 +10157,11 @@
       </c>
       <c r="W47" s="231"/>
       <c r="X47" s="46">
-        <v>0.17250000000000001</v>
+        <v>0.17125000000000001</v>
       </c>
       <c r="Y47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.2500000000000141E-5</v>
       </c>
       <c r="Z47" s="34"/>
     </row>
@@ -10163,7 +10206,7 @@
         <v>SEKAMTNS7Y=ICAP</v>
       </c>
       <c r="P48" s="46">
-        <v>0.47250000000000003</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="Q48" s="46">
         <v>0</v>
@@ -10176,7 +10219,7 @@
       </c>
       <c r="T48" s="46">
         <f t="shared" si="2"/>
-        <v>0.23625000000000002</v>
+        <v>0.23500000000000001</v>
       </c>
       <c r="U48" s="231"/>
       <c r="V48" s="233">
@@ -10184,11 +10227,11 @@
       </c>
       <c r="W48" s="231"/>
       <c r="X48" s="46">
-        <v>0.23625000000000002</v>
+        <v>0.23500000000000001</v>
       </c>
       <c r="Y48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.2499999999999924E-5</v>
       </c>
       <c r="Z48" s="34"/>
     </row>
@@ -10233,7 +10276,7 @@
         <v>SEKAMTNS8Y=ICAP</v>
       </c>
       <c r="P49" s="46">
-        <v>0.58750000000000002</v>
+        <v>0.58500000000000008</v>
       </c>
       <c r="Q49" s="46">
         <v>0</v>
@@ -10246,7 +10289,7 @@
       </c>
       <c r="T49" s="46">
         <f t="shared" si="2"/>
-        <v>0.29375000000000001</v>
+        <v>0.29250000000000004</v>
       </c>
       <c r="U49" s="231"/>
       <c r="V49" s="233">
@@ -10254,11 +10297,11 @@
       </c>
       <c r="W49" s="231"/>
       <c r="X49" s="46">
-        <v>0.29375000000000001</v>
+        <v>0.29250000000000004</v>
       </c>
       <c r="Y49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>1.2499999999999491E-5</v>
+        <v>-1.2499999999999491E-5</v>
       </c>
       <c r="Z49" s="34"/>
     </row>
@@ -10328,7 +10371,7 @@
       </c>
       <c r="Y50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>1.2499999999999924E-5</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="34"/>
     </row>
@@ -10373,7 +10416,7 @@
         <v>SEKAMTNS10Y=ICAP</v>
       </c>
       <c r="P51" s="46">
-        <v>0.76750000000000007</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="Q51" s="46">
         <v>0</v>
@@ -10386,7 +10429,7 @@
       </c>
       <c r="T51" s="46">
         <f t="shared" si="2"/>
-        <v>0.38375000000000004</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="U51" s="231"/>
       <c r="V51" s="233">
@@ -10394,11 +10437,11 @@
       </c>
       <c r="W51" s="231"/>
       <c r="X51" s="46">
-        <v>0.38375000000000004</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="Y51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>1.2499999999999924E-5</v>
+        <v>-1.2499999999999924E-5</v>
       </c>
       <c r="Z51" s="34"/>
     </row>
@@ -10443,7 +10486,7 @@
         <v>SEKAMTNS12Y=ICAP</v>
       </c>
       <c r="P52" s="46">
-        <v>0.91</v>
+        <v>0.90750000000000008</v>
       </c>
       <c r="Q52" s="46">
         <v>0</v>
@@ -10456,7 +10499,7 @@
       </c>
       <c r="T52" s="46">
         <f t="shared" si="2"/>
-        <v>0.45500000000000002</v>
+        <v>0.45375000000000004</v>
       </c>
       <c r="U52" s="231"/>
       <c r="V52" s="233">
@@ -10464,11 +10507,11 @@
       </c>
       <c r="W52" s="231"/>
       <c r="X52" s="46">
-        <v>0.45500000000000002</v>
+        <v>0.45375000000000004</v>
       </c>
       <c r="Y52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>1.2499999999999491E-5</v>
+        <v>-1.2499999999999491E-5</v>
       </c>
       <c r="Z52" s="34"/>
     </row>
@@ -10513,7 +10556,7 @@
         <v>SEKAMTNS15Y=ICAP</v>
       </c>
       <c r="P53" s="46">
-        <v>1.0775000000000001</v>
+        <v>1.075</v>
       </c>
       <c r="Q53" s="46">
         <v>0</v>
@@ -10526,7 +10569,7 @@
       </c>
       <c r="T53" s="46">
         <f t="shared" si="2"/>
-        <v>0.53875000000000006</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="U53" s="231"/>
       <c r="V53" s="233">
@@ -10534,11 +10577,11 @@
       </c>
       <c r="W53" s="231"/>
       <c r="X53" s="46">
-        <v>0.53875000000000006</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="Y53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F53,X53/100,Trigger)</f>
-        <v>1.2500000000001225E-5</v>
+        <v>-1.2500000000001225E-5</v>
       </c>
       <c r="Z53" s="34"/>
     </row>
@@ -10608,7 +10651,7 @@
       </c>
       <c r="Y54" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>1.2500000000001225E-5</v>
+        <v>0</v>
       </c>
       <c r="Z54" s="34"/>
     </row>
@@ -10653,7 +10696,7 @@
         <v>SEKAMTNS25Y=ICAP</v>
       </c>
       <c r="P55" s="46">
-        <v>1.3425</v>
+        <v>1.34</v>
       </c>
       <c r="Q55" s="46">
         <v>0</v>
@@ -10666,7 +10709,7 @@
       </c>
       <c r="T55" s="46">
         <f t="shared" si="2"/>
-        <v>0.67125000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="U55" s="231"/>
       <c r="V55" s="233">
@@ -10674,11 +10717,11 @@
       </c>
       <c r="W55" s="231"/>
       <c r="X55" s="46">
-        <v>0.67125000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="Y55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F55,X55/100,Trigger)</f>
-        <v>1.2499999999999491E-5</v>
+        <v>-1.2499999999999491E-5</v>
       </c>
       <c r="Z55" s="34"/>
     </row>
@@ -10793,7 +10836,7 @@
         <v>SEKAMTNS30Y=ICAP</v>
       </c>
       <c r="P57" s="46">
-        <v>1.3675000000000002</v>
+        <v>1.365</v>
       </c>
       <c r="Q57" s="46">
         <v>0</v>
@@ -10806,7 +10849,7 @@
       </c>
       <c r="T57" s="46">
         <f t="shared" si="2"/>
-        <v>0.68375000000000008</v>
+        <v>0.6825</v>
       </c>
       <c r="U57" s="231"/>
       <c r="V57" s="233">
@@ -10814,11 +10857,11 @@
       </c>
       <c r="W57" s="231"/>
       <c r="X57" s="46">
-        <v>0.68375000000000008</v>
+        <v>0.6825</v>
       </c>
       <c r="Y57" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F57,X57/100,Trigger)</f>
-        <v>1.2500000000000358E-5</v>
+        <v>-1.2500000000000358E-5</v>
       </c>
       <c r="Z57" s="34"/>
     </row>
@@ -11264,7 +11307,7 @@
   <dimension ref="B1:AD97"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11375,7 +11418,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -11402,7 +11445,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 15:58:43</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -12503,10 +12546,10 @@
         <v>SEKAB3S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>1.7500000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="R20" s="46">
-        <v>6.7500000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="S20" s="46">
         <v>0</v>
@@ -12516,7 +12559,7 @@
       </c>
       <c r="U20" s="46">
         <f t="shared" si="2"/>
-        <v>4.2500000000000003E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -12524,11 +12567,11 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>4.2500000000000003E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/100,Trigger)</f>
-        <v>0</v>
+        <v>2.5000000000000011E-5</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -13672,10 +13715,10 @@
         <v>SEKAB3S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>0.1575</v>
+        <v>0.155</v>
       </c>
       <c r="R36" s="46">
-        <v>0.20750000000000002</v>
+        <v>0.20500000000000002</v>
       </c>
       <c r="S36" s="46">
         <v>0</v>
@@ -13685,7 +13728,7 @@
       </c>
       <c r="U36" s="46">
         <f t="shared" si="2"/>
-        <v>0.1825</v>
+        <v>0.18</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -13693,11 +13736,11 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>0.1825</v>
+        <v>0.18</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.5000000000000066E-5</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -13964,10 +14007,10 @@
         <v>SEKAB3S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>0.28000000000000003</v>
+        <v>0.27750000000000002</v>
       </c>
       <c r="R40" s="46">
-        <v>0.33</v>
+        <v>0.32750000000000001</v>
       </c>
       <c r="S40" s="46">
         <v>0</v>
@@ -13977,7 +14020,7 @@
       </c>
       <c r="U40" s="46">
         <f t="shared" si="2"/>
-        <v>0.30500000000000005</v>
+        <v>0.30249999999999999</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -13985,11 +14028,11 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>0.30500000000000005</v>
+        <v>0.30249999999999999</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -14256,10 +14299,10 @@
         <v>SEKAB3S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>0.41500000000000004</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="R44" s="46">
-        <v>0.46500000000000002</v>
+        <v>0.46250000000000002</v>
       </c>
       <c r="S44" s="46">
         <v>0</v>
@@ -14269,7 +14312,7 @@
       </c>
       <c r="U44" s="46">
         <f t="shared" si="2"/>
-        <v>0.44000000000000006</v>
+        <v>0.4375</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -14277,11 +14320,11 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>0.44000000000000006</v>
+        <v>0.4375</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999999849E-5</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -14329,10 +14372,10 @@
         <v>SEKAB3S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>0.54749999999999999</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="R45" s="46">
-        <v>0.59750000000000003</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="S45" s="46">
         <v>0</v>
@@ -14342,7 +14385,7 @@
       </c>
       <c r="U45" s="46">
         <f t="shared" si="2"/>
-        <v>0.57250000000000001</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -14350,11 +14393,11 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>0.57250000000000001</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999999849E-5</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -14402,10 +14445,10 @@
         <v>SEKAB3S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>0.67749999999999999</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="R46" s="46">
-        <v>0.72750000000000004</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="S46" s="46">
         <v>0</v>
@@ -14415,7 +14458,7 @@
       </c>
       <c r="U46" s="46">
         <f t="shared" si="2"/>
-        <v>0.70250000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -14423,11 +14466,11 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>0.70250000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999998981E-5</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -14475,10 +14518,10 @@
         <v>SEKAB3S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>0.79250000000000009</v>
+        <v>0.79</v>
       </c>
       <c r="R47" s="46">
-        <v>0.84250000000000003</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="S47" s="46">
         <v>0</v>
@@ -14488,7 +14531,7 @@
       </c>
       <c r="U47" s="46">
         <f t="shared" si="2"/>
-        <v>0.81750000000000012</v>
+        <v>0.81500000000000006</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -14496,11 +14539,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>0.81750000000000012</v>
+        <v>0.81500000000000006</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/100,Trigger)</f>
-        <v>2.5000000000000716E-5</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -14548,10 +14591,10 @@
         <v>SEKAB3S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>0.89</v>
+        <v>0.88750000000000007</v>
       </c>
       <c r="R48" s="46">
-        <v>0.94000000000000006</v>
+        <v>0.9375</v>
       </c>
       <c r="S48" s="46">
         <v>0</v>
@@ -14561,7 +14604,7 @@
       </c>
       <c r="U48" s="46">
         <f t="shared" si="2"/>
-        <v>0.91500000000000004</v>
+        <v>0.91250000000000009</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -14569,11 +14612,11 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>0.91500000000000004</v>
+        <v>0.91250000000000009</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999998981E-5</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -14621,10 +14664,10 @@
         <v>SEKAB3S10Y=ICAP</v>
       </c>
       <c r="Q49" s="46">
-        <v>0.97250000000000003</v>
+        <v>0.97000000000000008</v>
       </c>
       <c r="R49" s="46">
-        <v>1.0225</v>
+        <v>1.02</v>
       </c>
       <c r="S49" s="46">
         <v>0</v>
@@ -14634,7 +14677,7 @@
       </c>
       <c r="U49" s="46">
         <f t="shared" si="2"/>
-        <v>0.99750000000000005</v>
+        <v>0.99500000000000011</v>
       </c>
       <c r="V49" s="231"/>
       <c r="W49" s="233">
@@ -14642,11 +14685,11 @@
       </c>
       <c r="X49" s="231"/>
       <c r="Y49" s="46">
-        <v>0.99750000000000005</v>
+        <v>0.99500000000000011</v>
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/100,Trigger)</f>
-        <v>2.5000000000000716E-5</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -14694,10 +14737,10 @@
         <v>SEKAB3S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>1.1075000000000002</v>
+        <v>1.105</v>
       </c>
       <c r="R50" s="46">
-        <v>1.1675</v>
+        <v>1.165</v>
       </c>
       <c r="S50" s="46">
         <v>0</v>
@@ -14707,7 +14750,7 @@
       </c>
       <c r="U50" s="46">
         <f t="shared" si="2"/>
-        <v>1.1375000000000002</v>
+        <v>1.135</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -14715,11 +14758,11 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>1.1375000000000002</v>
+        <v>1.135</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/100,Trigger)</f>
-        <v>0</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -14767,10 +14810,10 @@
         <v>SEKAB3S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>1.2725</v>
+        <v>1.27</v>
       </c>
       <c r="R51" s="46">
-        <v>1.3325</v>
+        <v>1.33</v>
       </c>
       <c r="S51" s="46">
         <v>0</v>
@@ -14780,7 +14823,7 @@
       </c>
       <c r="U51" s="46">
         <f t="shared" si="2"/>
-        <v>1.3025</v>
+        <v>1.3</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -14788,11 +14831,11 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>1.3025</v>
+        <v>1.3</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/100,Trigger)</f>
-        <v>2.4999999999998981E-5</v>
+        <v>-2.4999999999998981E-5</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -14840,10 +14883,10 @@
         <v>SEKAB3S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>1.4475</v>
+        <v>1.4450000000000001</v>
       </c>
       <c r="R52" s="46">
-        <v>1.5275000000000001</v>
+        <v>1.5250000000000001</v>
       </c>
       <c r="S52" s="46">
         <v>0</v>
@@ -14853,7 +14896,7 @@
       </c>
       <c r="U52" s="46">
         <f t="shared" si="2"/>
-        <v>1.4875</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -14861,11 +14904,11 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>1.4875</v>
+        <v>1.4850000000000001</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/100,Trigger)</f>
-        <v>2.5000000000000716E-5</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -14913,10 +14956,10 @@
         <v>SEKAB3S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>1.5175000000000001</v>
+        <v>1.5150000000000001</v>
       </c>
       <c r="R53" s="46">
-        <v>1.5975000000000001</v>
+        <v>1.595</v>
       </c>
       <c r="S53" s="46">
         <v>0</v>
@@ -14926,7 +14969,7 @@
       </c>
       <c r="U53" s="46">
         <f t="shared" si="2"/>
-        <v>1.5575000000000001</v>
+        <v>1.5550000000000002</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -14934,11 +14977,11 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>1.5575000000000001</v>
+        <v>1.5550000000000002</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/100,Trigger)</f>
-        <v>2.4999999999998981E-5</v>
+        <v>-2.4999999999998981E-5</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -15059,10 +15102,10 @@
         <v>SEKAB3S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>1.5275000000000001</v>
+        <v>1.5250000000000001</v>
       </c>
       <c r="R55" s="46">
-        <v>1.6275000000000002</v>
+        <v>1.625</v>
       </c>
       <c r="S55" s="46">
         <v>0</v>
@@ -15072,7 +15115,7 @@
       </c>
       <c r="U55" s="46">
         <f t="shared" si="2"/>
-        <v>1.5775000000000001</v>
+        <v>1.5750000000000002</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -15080,11 +15123,11 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>1.5775000000000001</v>
+        <v>1.5750000000000002</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/100,Trigger)</f>
-        <v>2.5000000000000716E-5</v>
+        <v>-2.5000000000000716E-5</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -15654,7 +15697,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -15681,7 +15724,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 15:57:43</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -15768,7 +15811,7 @@
         <v>153</v>
       </c>
       <c r="U6" s="39" t="e">
-        <f>_xll.qlMidEquivalent($Q6,$R6,$S6,$T6)</f>
+        <f>IF(ISNUMBER(Q6),Q6,#NUM!)</f>
         <v>#NUM!</v>
       </c>
       <c r="V6" s="231"/>
@@ -15842,7 +15885,7 @@
         <v>153</v>
       </c>
       <c r="U7" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q7,$R7,$S7,$T7)</f>
+        <f t="shared" ref="U7:U59" si="2">IF(ISNUMBER(Q7),Q7,#NUM!)</f>
         <v>#NUM!</v>
       </c>
       <c r="V7" s="231"/>
@@ -15915,7 +15958,7 @@
         <v>153</v>
       </c>
       <c r="U8" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q8,$R8,$S8,$T8)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V8" s="231"/>
@@ -15988,7 +16031,7 @@
         <v>153</v>
       </c>
       <c r="U9" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q9,$R9,$S9,$T9)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V9" s="231"/>
@@ -16062,7 +16105,7 @@
         <v>153</v>
       </c>
       <c r="U10" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q10,$R10,$S10,$T10)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V10" s="231"/>
@@ -16135,7 +16178,7 @@
         <v>153</v>
       </c>
       <c r="U11" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q11,$R11,$S11,$T11)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V11" s="231"/>
@@ -16208,7 +16251,7 @@
         <v>153</v>
       </c>
       <c r="U12" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q12,$R12,$S12,$T12)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V12" s="231"/>
@@ -16281,7 +16324,7 @@
         <v>153</v>
       </c>
       <c r="U13" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q13,$R13,$S13,$T13)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V13" s="231"/>
@@ -16354,7 +16397,7 @@
         <v>153</v>
       </c>
       <c r="U14" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q14,$R14,$S14,$T14)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V14" s="231"/>
@@ -16427,7 +16470,7 @@
         <v>153</v>
       </c>
       <c r="U15" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q15,$R15,$S15,$T15)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V15" s="231"/>
@@ -16501,7 +16544,7 @@
         <v>153</v>
       </c>
       <c r="U16" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q16,$R16,$S16,$T16)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V16" s="231"/>
@@ -16574,7 +16617,7 @@
         <v>153</v>
       </c>
       <c r="U17" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q17,$R17,$S17,$T17)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V17" s="231"/>
@@ -16648,7 +16691,7 @@
         <v>153</v>
       </c>
       <c r="U18" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q18,$R18,$S18,$T18)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V18" s="231"/>
@@ -16721,7 +16764,7 @@
         <v>153</v>
       </c>
       <c r="U19" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q19,$R19,$S19,$T19)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V19" s="231"/>
@@ -16782,7 +16825,7 @@
         <v>SEK3S6S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>8.6</v>
+        <v>8.57</v>
       </c>
       <c r="R20" s="46">
         <v>0</v>
@@ -16794,8 +16837,8 @@
         <v>0</v>
       </c>
       <c r="U20" s="46">
-        <f>_xll.qlMidEquivalent($Q20,$R20,$S20,$T20)</f>
-        <v>8.6</v>
+        <f t="shared" si="2"/>
+        <v>8.57</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -16803,7 +16846,7 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>8.6</v>
+        <v>8.57</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
@@ -16867,7 +16910,7 @@
         <v>153</v>
       </c>
       <c r="U21" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q21,$R21,$S21,$T21)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V21" s="231"/>
@@ -16940,7 +16983,7 @@
         <v>153</v>
       </c>
       <c r="U22" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q22,$R22,$S22,$T22)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V22" s="231"/>
@@ -17013,7 +17056,7 @@
         <v>153</v>
       </c>
       <c r="U23" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q23,$R23,$S23,$T23)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V23" s="231"/>
@@ -17086,7 +17129,7 @@
         <v>153</v>
       </c>
       <c r="U24" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q24,$R24,$S24,$T24)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V24" s="231"/>
@@ -17159,7 +17202,7 @@
         <v>153</v>
       </c>
       <c r="U25" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q25,$R25,$S25,$T25)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V25" s="231"/>
@@ -17232,7 +17275,7 @@
         <v>153</v>
       </c>
       <c r="U26" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q26,$R26,$S26,$T26)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V26" s="231"/>
@@ -17305,7 +17348,7 @@
         <v>153</v>
       </c>
       <c r="U27" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q27,$R27,$S27,$T27)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V27" s="231"/>
@@ -17379,7 +17422,7 @@
         <v>153</v>
       </c>
       <c r="U28" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q28,$R28,$S28,$T28)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V28" s="231"/>
@@ -17452,7 +17495,7 @@
         <v>153</v>
       </c>
       <c r="U29" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q29,$R29,$S29,$T29)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V29" s="231"/>
@@ -17525,7 +17568,7 @@
         <v>153</v>
       </c>
       <c r="U30" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q30,$R30,$S30,$T30)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V30" s="231"/>
@@ -17598,7 +17641,7 @@
         <v>153</v>
       </c>
       <c r="U31" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q31,$R31,$S31,$T31)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V31" s="231"/>
@@ -17659,7 +17702,7 @@
         <v>SEK3S6S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>9.3000000000000007</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="R32" s="46">
         <v>0</v>
@@ -17671,8 +17714,8 @@
         <v>0</v>
       </c>
       <c r="U32" s="46">
-        <f>_xll.qlMidEquivalent($Q32,$R32,$S32,$T32)</f>
-        <v>9.3000000000000007</v>
+        <f t="shared" si="2"/>
+        <v>9.2799999999999994</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -17680,7 +17723,7 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>9.3000000000000007</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
@@ -17744,7 +17787,7 @@
         <v>153</v>
       </c>
       <c r="U33" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q33,$R33,$S33,$T33)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V33" s="231"/>
@@ -17817,7 +17860,7 @@
         <v>153</v>
       </c>
       <c r="U34" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q34,$R34,$S34,$T34)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V34" s="231"/>
@@ -17890,7 +17933,7 @@
         <v>153</v>
       </c>
       <c r="U35" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q35,$R35,$S35,$T35)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V35" s="231"/>
@@ -17951,7 +17994,7 @@
         <v>SEK3S6S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>9.52</v>
+        <v>9.51</v>
       </c>
       <c r="R36" s="46">
         <v>0</v>
@@ -17963,8 +18006,8 @@
         <v>0</v>
       </c>
       <c r="U36" s="46">
-        <f>_xll.qlMidEquivalent($Q36,$R36,$S36,$T36)</f>
-        <v>9.52</v>
+        <f t="shared" si="2"/>
+        <v>9.51</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -17972,7 +18015,7 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>9.52</v>
+        <v>9.51</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/10000,Trigger)</f>
@@ -18036,7 +18079,7 @@
         <v>153</v>
       </c>
       <c r="U37" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q37,$R37,$S37,$T37)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V37" s="231"/>
@@ -18065,7 +18108,7 @@
         <v>160</v>
       </c>
       <c r="F38" s="42" t="str">
-        <f t="shared" ref="F38:F59" si="2">Currency&amp;$D38&amp;$E38&amp;$C38&amp;QuoteSuffix</f>
+        <f t="shared" ref="F38:F59" si="3">Currency&amp;$D38&amp;$E38&amp;$C38&amp;QuoteSuffix</f>
         <v>SEK3S6S42M_Quote</v>
       </c>
       <c r="G38" s="42" t="str">
@@ -18109,7 +18152,7 @@
         <v>153</v>
       </c>
       <c r="U38" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q38,$R38,$S38,$T38)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V38" s="231"/>
@@ -18138,7 +18181,7 @@
         <v>160</v>
       </c>
       <c r="F39" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S45M_Quote</v>
       </c>
       <c r="G39" s="42" t="str">
@@ -18182,7 +18225,7 @@
         <v>153</v>
       </c>
       <c r="U39" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q39,$R39,$S39,$T39)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V39" s="231"/>
@@ -18211,7 +18254,7 @@
         <v>160</v>
       </c>
       <c r="F40" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S4Y_Quote</v>
       </c>
       <c r="G40" s="42" t="str">
@@ -18243,7 +18286,7 @@
         <v>SEK3S6S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>9.620000000000001</v>
+        <v>9.61</v>
       </c>
       <c r="R40" s="46">
         <v>0</v>
@@ -18255,8 +18298,8 @@
         <v>0</v>
       </c>
       <c r="U40" s="46">
-        <f>_xll.qlMidEquivalent($Q40,$R40,$S40,$T40)</f>
-        <v>9.620000000000001</v>
+        <f t="shared" si="2"/>
+        <v>9.61</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -18264,7 +18307,7 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>9.620000000000001</v>
+        <v>9.61</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
@@ -18284,7 +18327,7 @@
         <v>160</v>
       </c>
       <c r="F41" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S51M_Quote</v>
       </c>
       <c r="G41" s="42" t="str">
@@ -18328,7 +18371,7 @@
         <v>153</v>
       </c>
       <c r="U41" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q41,$R41,$S41,$T41)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V41" s="231"/>
@@ -18357,7 +18400,7 @@
         <v>160</v>
       </c>
       <c r="F42" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S54M_Quote</v>
       </c>
       <c r="G42" s="42" t="str">
@@ -18401,7 +18444,7 @@
         <v>153</v>
       </c>
       <c r="U42" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q42,$R42,$S42,$T42)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V42" s="231"/>
@@ -18430,7 +18473,7 @@
         <v>160</v>
       </c>
       <c r="F43" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S57M_Quote</v>
       </c>
       <c r="G43" s="42" t="str">
@@ -18474,7 +18517,7 @@
         <v>153</v>
       </c>
       <c r="U43" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q43,$R43,$S43,$T43)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V43" s="231"/>
@@ -18503,7 +18546,7 @@
         <v>160</v>
       </c>
       <c r="F44" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S5Y_Quote</v>
       </c>
       <c r="G44" s="42" t="str">
@@ -18535,7 +18578,7 @@
         <v>SEK3S6S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>9.67</v>
+        <v>9.66</v>
       </c>
       <c r="R44" s="46">
         <v>0</v>
@@ -18547,8 +18590,8 @@
         <v>0</v>
       </c>
       <c r="U44" s="46">
-        <f>_xll.qlMidEquivalent($Q44,$R44,$S44,$T44)</f>
-        <v>9.67</v>
+        <f t="shared" si="2"/>
+        <v>9.66</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -18556,7 +18599,7 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>9.67</v>
+        <v>9.66</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
@@ -18576,7 +18619,7 @@
         <v>160</v>
       </c>
       <c r="F45" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S6Y_Quote</v>
       </c>
       <c r="G45" s="42" t="str">
@@ -18608,7 +18651,7 @@
         <v>SEK3S6S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>9.69</v>
+        <v>9.68</v>
       </c>
       <c r="R45" s="46">
         <v>0</v>
@@ -18620,8 +18663,8 @@
         <v>0</v>
       </c>
       <c r="U45" s="46">
-        <f>_xll.qlMidEquivalent($Q45,$R45,$S45,$T45)</f>
-        <v>9.69</v>
+        <f t="shared" si="2"/>
+        <v>9.68</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -18629,7 +18672,7 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>9.69</v>
+        <v>9.68</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
@@ -18649,7 +18692,7 @@
         <v>160</v>
       </c>
       <c r="F46" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S7Y_Quote</v>
       </c>
       <c r="G46" s="42" t="str">
@@ -18693,7 +18736,7 @@
         <v>0</v>
       </c>
       <c r="U46" s="46">
-        <f>_xll.qlMidEquivalent($Q46,$R46,$S46,$T46)</f>
+        <f t="shared" si="2"/>
         <v>9.69</v>
       </c>
       <c r="V46" s="231"/>
@@ -18722,7 +18765,7 @@
         <v>160</v>
       </c>
       <c r="F47" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S8Y_Quote</v>
       </c>
       <c r="G47" s="42" t="str">
@@ -18766,7 +18809,7 @@
         <v>0</v>
       </c>
       <c r="U47" s="46">
-        <f>_xll.qlMidEquivalent($Q47,$R47,$S47,$T47)</f>
+        <f t="shared" si="2"/>
         <v>9.69</v>
       </c>
       <c r="V47" s="231"/>
@@ -18795,7 +18838,7 @@
         <v>160</v>
       </c>
       <c r="F48" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S9Y_Quote</v>
       </c>
       <c r="G48" s="42" t="str">
@@ -18839,7 +18882,7 @@
         <v>0</v>
       </c>
       <c r="U48" s="46">
-        <f>_xll.qlMidEquivalent($Q48,$R48,$S48,$T48)</f>
+        <f t="shared" si="2"/>
         <v>9.68</v>
       </c>
       <c r="V48" s="231"/>
@@ -18852,7 +18895,7 @@
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>-9.9999999999991589E-7</v>
+        <v>0</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -18868,7 +18911,7 @@
         <v>160</v>
       </c>
       <c r="F49" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S10Y_Quote</v>
       </c>
       <c r="G49" s="42" t="str">
@@ -18912,7 +18955,7 @@
         <v>0</v>
       </c>
       <c r="U49" s="46">
-        <f>_xll.qlMidEquivalent($Q49,$R49,$S49,$T49)</f>
+        <f t="shared" si="2"/>
         <v>9.6300000000000008</v>
       </c>
       <c r="V49" s="231"/>
@@ -18941,7 +18984,7 @@
         <v>160</v>
       </c>
       <c r="F50" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S12Y_Quote</v>
       </c>
       <c r="G50" s="42" t="str">
@@ -18985,7 +19028,7 @@
         <v>0</v>
       </c>
       <c r="U50" s="46">
-        <f>_xll.qlMidEquivalent($Q50,$R50,$S50,$T50)</f>
+        <f t="shared" si="2"/>
         <v>9.370000000000001</v>
       </c>
       <c r="V50" s="231"/>
@@ -19014,7 +19057,7 @@
         <v>160</v>
       </c>
       <c r="F51" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S15Y_Quote</v>
       </c>
       <c r="G51" s="42" t="str">
@@ -19058,7 +19101,7 @@
         <v>0</v>
       </c>
       <c r="U51" s="46">
-        <f>_xll.qlMidEquivalent($Q51,$R51,$S51,$T51)</f>
+        <f t="shared" si="2"/>
         <v>8.68</v>
       </c>
       <c r="V51" s="231"/>
@@ -19087,7 +19130,7 @@
         <v>160</v>
       </c>
       <c r="F52" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S20Y_Quote</v>
       </c>
       <c r="G52" s="42" t="str">
@@ -19131,7 +19174,7 @@
         <v>0</v>
       </c>
       <c r="U52" s="46">
-        <f>_xll.qlMidEquivalent($Q52,$R52,$S52,$T52)</f>
+        <f t="shared" si="2"/>
         <v>7.65</v>
       </c>
       <c r="V52" s="231"/>
@@ -19160,7 +19203,7 @@
         <v>160</v>
       </c>
       <c r="F53" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S25Y_Quote</v>
       </c>
       <c r="G53" s="42" t="str">
@@ -19204,7 +19247,7 @@
         <v>0</v>
       </c>
       <c r="U53" s="46">
-        <f>_xll.qlMidEquivalent($Q53,$R53,$S53,$T53)</f>
+        <f t="shared" si="2"/>
         <v>6.92</v>
       </c>
       <c r="V53" s="231"/>
@@ -19233,7 +19276,7 @@
         <v>160</v>
       </c>
       <c r="F54" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S27Y_Quote</v>
       </c>
       <c r="G54" s="42" t="str">
@@ -19277,7 +19320,7 @@
         <v>153</v>
       </c>
       <c r="U54" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q54,$R54,$S54,$T54)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V54" s="231"/>
@@ -19306,7 +19349,7 @@
         <v>160</v>
       </c>
       <c r="F55" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S30Y_Quote</v>
       </c>
       <c r="G55" s="42" t="str">
@@ -19350,7 +19393,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="46">
-        <f>_xll.qlMidEquivalent($Q55,$R55,$S55,$T55)</f>
+        <f t="shared" si="2"/>
         <v>6.32</v>
       </c>
       <c r="V55" s="231"/>
@@ -19379,7 +19422,7 @@
         <v>160</v>
       </c>
       <c r="F56" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S35Y_Quote</v>
       </c>
       <c r="G56" s="42" t="str">
@@ -19423,7 +19466,7 @@
         <v>153</v>
       </c>
       <c r="U56" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q56,$R56,$S56,$T56)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V56" s="231"/>
@@ -19452,7 +19495,7 @@
         <v>160</v>
       </c>
       <c r="F57" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S40Y_Quote</v>
       </c>
       <c r="G57" s="42" t="str">
@@ -19496,7 +19539,7 @@
         <v>153</v>
       </c>
       <c r="U57" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q57,$R57,$S57,$T57)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V57" s="231"/>
@@ -19525,7 +19568,7 @@
         <v>160</v>
       </c>
       <c r="F58" s="42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S45Y_Quote</v>
       </c>
       <c r="G58" s="42" t="str">
@@ -19569,7 +19612,7 @@
         <v>153</v>
       </c>
       <c r="U58" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q58,$R58,$S58,$T58)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V58" s="231"/>
@@ -19598,7 +19641,7 @@
         <v>160</v>
       </c>
       <c r="F59" s="49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>SEK3S6S50Y_Quote</v>
       </c>
       <c r="G59" s="49" t="str">
@@ -19642,7 +19685,7 @@
         <v>153</v>
       </c>
       <c r="U59" s="53" t="e">
-        <f>_xll.qlMidEquivalent($Q59,$R59,$S59,$T59)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V59" s="231"/>
@@ -19933,7 +19976,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -19960,7 +20003,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 15:52:28</v>
+        <v>Updated at 09:25:07</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -20047,7 +20090,7 @@
         <v>153</v>
       </c>
       <c r="U6" s="39" t="e">
-        <f>_xll.qlMidEquivalent($Q6,$R6,$S6,$T6)</f>
+        <f>IF(ISNUMBER(Q6),Q6,#NUM!)</f>
         <v>#NUM!</v>
       </c>
       <c r="V6" s="231"/>
@@ -20121,7 +20164,7 @@
         <v>153</v>
       </c>
       <c r="U7" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q7,$R7,$S7,$T7)</f>
+        <f t="shared" ref="U7:U59" si="2">IF(ISNUMBER(Q7),Q7,#NUM!)</f>
         <v>#NUM!</v>
       </c>
       <c r="V7" s="231"/>
@@ -20194,7 +20237,7 @@
         <v>153</v>
       </c>
       <c r="U8" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q8,$R8,$S8,$T8)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V8" s="231"/>
@@ -20267,7 +20310,7 @@
         <v>153</v>
       </c>
       <c r="U9" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q9,$R9,$S9,$T9)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V9" s="231"/>
@@ -20341,7 +20384,7 @@
         <v>153</v>
       </c>
       <c r="U10" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q10,$R10,$S10,$T10)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V10" s="231"/>
@@ -20414,7 +20457,7 @@
         <v>153</v>
       </c>
       <c r="U11" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q11,$R11,$S11,$T11)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V11" s="231"/>
@@ -20487,7 +20530,7 @@
         <v>153</v>
       </c>
       <c r="U12" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q12,$R12,$S12,$T12)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V12" s="231"/>
@@ -20560,7 +20603,7 @@
         <v>153</v>
       </c>
       <c r="U13" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q13,$R13,$S13,$T13)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V13" s="231"/>
@@ -20633,7 +20676,7 @@
         <v>153</v>
       </c>
       <c r="U14" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q14,$R14,$S14,$T14)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V14" s="231"/>
@@ -20706,7 +20749,7 @@
         <v>153</v>
       </c>
       <c r="U15" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q15,$R15,$S15,$T15)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V15" s="231"/>
@@ -20780,7 +20823,7 @@
         <v>153</v>
       </c>
       <c r="U16" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q16,$R16,$S16,$T16)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V16" s="231"/>
@@ -20853,7 +20896,7 @@
         <v>153</v>
       </c>
       <c r="U17" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q17,$R17,$S17,$T17)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V17" s="231"/>
@@ -20927,7 +20970,7 @@
         <v>153</v>
       </c>
       <c r="U18" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q18,$R18,$S18,$T18)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V18" s="231"/>
@@ -21000,7 +21043,7 @@
         <v>153</v>
       </c>
       <c r="U19" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q19,$R19,$S19,$T19)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V19" s="231"/>
@@ -21061,7 +21104,7 @@
         <v>SEK1S3S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>8.02</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="R20" s="46">
         <v>0</v>
@@ -21073,8 +21116,8 @@
         <v>0</v>
       </c>
       <c r="U20" s="46">
-        <f>_xll.qlMidEquivalent($Q20,$R20,$S20,$T20)</f>
-        <v>8.02</v>
+        <f t="shared" si="2"/>
+        <v>8.0299999999999994</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -21082,7 +21125,7 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>8.02</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
@@ -21146,7 +21189,7 @@
         <v>153</v>
       </c>
       <c r="U21" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q21,$R21,$S21,$T21)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V21" s="231"/>
@@ -21219,7 +21262,7 @@
         <v>153</v>
       </c>
       <c r="U22" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q22,$R22,$S22,$T22)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V22" s="231"/>
@@ -21292,7 +21335,7 @@
         <v>153</v>
       </c>
       <c r="U23" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q23,$R23,$S23,$T23)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V23" s="231"/>
@@ -21365,7 +21408,7 @@
         <v>153</v>
       </c>
       <c r="U24" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q24,$R24,$S24,$T24)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V24" s="231"/>
@@ -21438,7 +21481,7 @@
         <v>153</v>
       </c>
       <c r="U25" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q25,$R25,$S25,$T25)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V25" s="231"/>
@@ -21511,7 +21554,7 @@
         <v>153</v>
       </c>
       <c r="U26" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q26,$R26,$S26,$T26)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V26" s="231"/>
@@ -21584,7 +21627,7 @@
         <v>153</v>
       </c>
       <c r="U27" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q27,$R27,$S27,$T27)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V27" s="231"/>
@@ -21658,7 +21701,7 @@
         <v>153</v>
       </c>
       <c r="U28" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q28,$R28,$S28,$T28)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V28" s="231"/>
@@ -21731,7 +21774,7 @@
         <v>153</v>
       </c>
       <c r="U29" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q29,$R29,$S29,$T29)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V29" s="231"/>
@@ -21804,7 +21847,7 @@
         <v>153</v>
       </c>
       <c r="U30" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q30,$R30,$S30,$T30)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V30" s="231"/>
@@ -21877,7 +21920,7 @@
         <v>153</v>
       </c>
       <c r="U31" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q31,$R31,$S31,$T31)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V31" s="231"/>
@@ -21938,7 +21981,7 @@
         <v>SEK1S3S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>9.26</v>
+        <v>9.27</v>
       </c>
       <c r="R32" s="46">
         <v>0</v>
@@ -21950,8 +21993,8 @@
         <v>0</v>
       </c>
       <c r="U32" s="46">
-        <f>_xll.qlMidEquivalent($Q32,$R32,$S32,$T32)</f>
-        <v>9.26</v>
+        <f t="shared" si="2"/>
+        <v>9.27</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -21959,7 +22002,7 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>9.26</v>
+        <v>9.27</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
@@ -22023,7 +22066,7 @@
         <v>153</v>
       </c>
       <c r="U33" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q33,$R33,$S33,$T33)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V33" s="231"/>
@@ -22096,7 +22139,7 @@
         <v>153</v>
       </c>
       <c r="U34" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q34,$R34,$S34,$T34)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V34" s="231"/>
@@ -22169,7 +22212,7 @@
         <v>153</v>
       </c>
       <c r="U35" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q35,$R35,$S35,$T35)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V35" s="231"/>
@@ -22242,7 +22285,7 @@
         <v>0</v>
       </c>
       <c r="U36" s="46">
-        <f>_xll.qlMidEquivalent($Q36,$R36,$S36,$T36)</f>
+        <f t="shared" si="2"/>
         <v>9.83</v>
       </c>
       <c r="V36" s="231"/>
@@ -22315,7 +22358,7 @@
         <v>153</v>
       </c>
       <c r="U37" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q37,$R37,$S37,$T37)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V37" s="231"/>
@@ -22388,7 +22431,7 @@
         <v>153</v>
       </c>
       <c r="U38" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q38,$R38,$S38,$T38)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V38" s="231"/>
@@ -22461,7 +22504,7 @@
         <v>153</v>
       </c>
       <c r="U39" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q39,$R39,$S39,$T39)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V39" s="231"/>
@@ -22534,7 +22577,7 @@
         <v>0</v>
       </c>
       <c r="U40" s="46">
-        <f>_xll.qlMidEquivalent($Q40,$R40,$S40,$T40)</f>
+        <f t="shared" si="2"/>
         <v>10.1</v>
       </c>
       <c r="V40" s="231"/>
@@ -22607,7 +22650,7 @@
         <v>153</v>
       </c>
       <c r="U41" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q41,$R41,$S41,$T41)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V41" s="231"/>
@@ -22680,7 +22723,7 @@
         <v>153</v>
       </c>
       <c r="U42" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q42,$R42,$S42,$T42)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V42" s="231"/>
@@ -22753,7 +22796,7 @@
         <v>153</v>
       </c>
       <c r="U43" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q43,$R43,$S43,$T43)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V43" s="231"/>
@@ -22826,7 +22869,7 @@
         <v>0</v>
       </c>
       <c r="U44" s="46">
-        <f>_xll.qlMidEquivalent($Q44,$R44,$S44,$T44)</f>
+        <f t="shared" si="2"/>
         <v>10.15</v>
       </c>
       <c r="V44" s="231"/>
@@ -22899,7 +22942,7 @@
         <v>0</v>
       </c>
       <c r="U45" s="46">
-        <f>_xll.qlMidEquivalent($Q45,$R45,$S45,$T45)</f>
+        <f t="shared" si="2"/>
         <v>10.17</v>
       </c>
       <c r="V45" s="231"/>
@@ -22972,7 +23015,7 @@
         <v>0</v>
       </c>
       <c r="U46" s="46">
-        <f>_xll.qlMidEquivalent($Q46,$R46,$S46,$T46)</f>
+        <f t="shared" si="2"/>
         <v>10.18</v>
       </c>
       <c r="V46" s="231"/>
@@ -23045,7 +23088,7 @@
         <v>0</v>
       </c>
       <c r="U47" s="46">
-        <f>_xll.qlMidEquivalent($Q47,$R47,$S47,$T47)</f>
+        <f t="shared" si="2"/>
         <v>10.17</v>
       </c>
       <c r="V47" s="231"/>
@@ -23058,7 +23101,7 @@
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>-1.0000000000001327E-6</v>
+        <v>0</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -23118,7 +23161,7 @@
         <v>0</v>
       </c>
       <c r="U48" s="46">
-        <f>_xll.qlMidEquivalent($Q48,$R48,$S48,$T48)</f>
+        <f t="shared" si="2"/>
         <v>10.17</v>
       </c>
       <c r="V48" s="231"/>
@@ -23191,7 +23234,7 @@
         <v>0</v>
       </c>
       <c r="U49" s="46">
-        <f>_xll.qlMidEquivalent($Q49,$R49,$S49,$T49)</f>
+        <f t="shared" si="2"/>
         <v>10.16</v>
       </c>
       <c r="V49" s="231"/>
@@ -23264,7 +23307,7 @@
         <v>0</v>
       </c>
       <c r="U50" s="46">
-        <f>_xll.qlMidEquivalent($Q50,$R50,$S50,$T50)</f>
+        <f t="shared" si="2"/>
         <v>10.14</v>
       </c>
       <c r="V50" s="231"/>
@@ -23337,7 +23380,7 @@
         <v>0</v>
       </c>
       <c r="U51" s="46">
-        <f>_xll.qlMidEquivalent($Q51,$R51,$S51,$T51)</f>
+        <f t="shared" si="2"/>
         <v>9.92</v>
       </c>
       <c r="V51" s="231"/>
@@ -23410,7 +23453,7 @@
         <v>0</v>
       </c>
       <c r="U52" s="46">
-        <f>_xll.qlMidEquivalent($Q52,$R52,$S52,$T52)</f>
+        <f t="shared" si="2"/>
         <v>9.3800000000000008</v>
       </c>
       <c r="V52" s="231"/>
@@ -23483,7 +23526,7 @@
         <v>0</v>
       </c>
       <c r="U53" s="46">
-        <f>_xll.qlMidEquivalent($Q53,$R53,$S53,$T53)</f>
+        <f t="shared" si="2"/>
         <v>8.9600000000000009</v>
       </c>
       <c r="V53" s="231"/>
@@ -23556,7 +23599,7 @@
         <v>153</v>
       </c>
       <c r="U54" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q54,$R54,$S54,$T54)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V54" s="231"/>
@@ -23629,7 +23672,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="46">
-        <f>_xll.qlMidEquivalent($Q55,$R55,$S55,$T55)</f>
+        <f t="shared" si="2"/>
         <v>8.68</v>
       </c>
       <c r="V55" s="231"/>
@@ -23702,7 +23745,7 @@
         <v>153</v>
       </c>
       <c r="U56" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q56,$R56,$S56,$T56)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V56" s="231"/>
@@ -23775,7 +23818,7 @@
         <v>153</v>
       </c>
       <c r="U57" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q57,$R57,$S57,$T57)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V57" s="231"/>
@@ -23848,7 +23891,7 @@
         <v>153</v>
       </c>
       <c r="U58" s="46" t="e">
-        <f>_xll.qlMidEquivalent($Q58,$R58,$S58,$T58)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V58" s="231"/>
@@ -23921,7 +23964,7 @@
         <v>153</v>
       </c>
       <c r="U59" s="53" t="e">
-        <f>_xll.qlMidEquivalent($Q59,$R59,$S59,$T59)</f>
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
       <c r="V59" s="231"/>

</xml_diff>

<commit_message>
SEK Market: fixed average OIS calculation, ask is not quoted
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
@@ -1791,45 +1791,45 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
         <stp/>
-        <stp>{B51EDCFF-A915-49AB-AAF4-837E709DDFD5}</stp>
+        <stp>{5C479A66-51EF-4C0A-8CB8-8610CB59C58D}</stp>
+        <tr r="P5" s="69"/>
+      </tp>
+      <tp t="s">
+        <v>Paused at 09:35:04</v>
+        <stp/>
+        <stp>{952C35EB-8489-495D-9960-0343A44CD2A5}</stp>
+        <tr r="S3" s="64"/>
+      </tp>
+      <tp t="s">
+        <v>Paused at 09:35:04</v>
+        <stp/>
+        <stp>{B39BE39A-CB49-4FA6-9F99-8009615693B9}</stp>
+        <tr r="O6" s="22"/>
+      </tp>
+      <tp t="s">
+        <v>Paused at 09:35:04</v>
+        <stp/>
+        <stp>{E02D3973-DEF8-49F8-BB78-F76D57FD2040}</stp>
         <tr r="P5" s="66"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
         <stp/>
-        <stp>{1D3416D1-5DA5-4A84-A20C-DF84ADE45C57}</stp>
-        <tr r="O6" s="22"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:25:07</v>
-        <stp/>
-        <stp>{DD259B0A-751E-4597-BC2C-6D4A4E8445A4}</stp>
+        <stp>{6A58075F-0492-4CB4-A3A3-4E6DC1027E8A}</stp>
         <tr r="N5" s="16"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
         <stp/>
-        <stp>{FB0569B8-6AC8-4782-897B-C360AD203C3B}</stp>
-        <tr r="P5" s="69"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:25:07</v>
-        <stp/>
-        <stp>{2F48653C-77B6-41ED-B8E4-065BC0D2314F}</stp>
-        <tr r="S3" s="64"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:25:07</v>
-        <stp/>
-        <stp>{7DA82CC9-E1FE-4A63-BF8B-C15F488B9368}</stp>
+        <stp>{C76AEC19-8564-47C9-B0A1-F98121FBF20A}</stp>
         <tr r="P5" s="67"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
         <stp/>
-        <stp>{97700A76-B804-4895-A845-C4B8145E523B}</stp>
+        <stp>{AC385E6E-2FDE-4835-B2D0-4BD1349054F7}</stp>
         <tr r="K5" s="15"/>
       </tp>
     </main>
@@ -2128,7 +2128,7 @@
   <dimension ref="B1:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2146,7 +2146,7 @@
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="72" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov  4 2014 09:24:39</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Dec 24 2014 09:17:06</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -2154,14 +2154,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="75">
-        <v>42044.391979166663</v>
+        <v>42088.391377314816</v>
       </c>
       <c r="H3" s="114" t="s">
         <v>132</v>
       </c>
       <c r="I3" s="77">
         <f>_xll.ohTrigger(Deposits!S4,FRA3M!X4,OIS!Y5,Swaps3M!Z4,BasisSwap3M6M!Z4,BasisSwap1M3M!Z4)</f>
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="D8" s="85">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42044</v>
+        <v>42088</v>
       </c>
       <c r="E8" s="105"/>
       <c r="G8" s="97"/>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="S3" s="183" t="str">
         <f>_xll.RData(S4:S10,T3:U3,"RTFEED:IDN",,,T4)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="T3" s="177" t="s">
         <v>137</v>
@@ -2756,10 +2756,10 @@
         <v>STISEKTNDFI=</v>
       </c>
       <c r="T5" s="178">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U5" s="187">
-        <v>3.6000000000000004E-2</v>
+        <v>-0.123</v>
       </c>
       <c r="V5" s="178" t="b">
         <f>IF(AND(ISNUMBER($U5),$U5&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2830,10 +2830,10 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="T6" s="178">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U6" s="187">
-        <v>4.1000000000000002E-2</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="V6" s="178" t="b">
         <f>IF(AND(ISNUMBER($U6),$U6&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="X6" s="181">
         <f>_xll.qlQuoteValue(L6)</f>
-        <v>3.7000000000000005E-4</v>
+        <v>4.0999999999999999E-4</v>
       </c>
       <c r="Y6" s="8"/>
     </row>
@@ -2907,10 +2907,10 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="T7" s="178">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U7" s="187">
-        <v>-1.1000000000000001E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="V7" s="178" t="b">
         <f t="shared" ref="V7:V10" si="5">IF(AND(ISNUMBER($U7),$U7&lt;&gt;0%),TRUE,FALSE)</f>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="X7" s="181">
         <f>_xll.qlQuoteValue(L7)</f>
-        <v>1.1000000000000002E-4</v>
+        <v>-1.1000000000000002E-4</v>
       </c>
       <c r="Y7" s="8"/>
     </row>
@@ -2981,10 +2981,10 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="T8" s="178">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U8" s="187">
-        <v>7.0000000000000001E-3</v>
+        <v>-6.9999999999999993E-2</v>
       </c>
       <c r="V8" s="178" t="b">
         <f t="shared" si="5"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="X8" s="181">
         <f>_xll.qlQuoteValue(L8)</f>
-        <v>1.2E-4</v>
+        <v>7.0000000000000007E-5</v>
       </c>
       <c r="Y8" s="8"/>
     </row>
@@ -3058,10 +3058,10 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="T9" s="178">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U9" s="187">
-        <v>4.7E-2</v>
+        <v>-5.5000000000000007E-2</v>
       </c>
       <c r="V9" s="178" t="b">
         <f t="shared" si="5"/>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="X9" s="181">
         <f>_xll.qlQuoteValue(L9)</f>
-        <v>5.4000000000000001E-4</v>
+        <v>4.6999999999999999E-4</v>
       </c>
       <c r="Y9" s="8"/>
     </row>
@@ -3135,10 +3135,10 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="T10" s="179">
-        <v>42041</v>
+        <v>42087</v>
       </c>
       <c r="U10" s="187">
-        <v>0.129</v>
+        <v>-2.7000000000000003E-2</v>
       </c>
       <c r="V10" s="179" t="b">
         <f t="shared" si="5"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="X10" s="182">
         <f>_xll.qlQuoteValue(L10)</f>
-        <v>1.33E-3</v>
+        <v>1.2900000000000001E-3</v>
       </c>
       <c r="Y10" s="8"/>
     </row>
@@ -4547,7 +4547,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="33">
         <f>_xll.ohTrigger(S6:S23)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="T4" s="34"/>
     </row>
@@ -4569,7 +4569,7 @@
       <c r="J5" s="166"/>
       <c r="K5" s="176" t="str">
         <f>_xll.RData(K7:K23,L5:M5,,ReutersRtMode,,L7)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="L5" s="167" t="s">
         <v>106</v>
@@ -4670,14 +4670,14 @@
         <v>STISEKTNDFI=</v>
       </c>
       <c r="L7" s="153">
-        <v>3.6000000000000004E-2</v>
+        <v>-0.123</v>
       </c>
       <c r="M7" s="153">
         <v>0</v>
       </c>
       <c r="N7" s="46">
         <f t="shared" ref="N7:N23" si="1">IF(ISNUMBER(L7),L7,#NUM!)</f>
-        <v>3.6000000000000004E-2</v>
+        <v>-0.123</v>
       </c>
       <c r="O7" s="32" t="s">
         <v>154</v>
@@ -4687,11 +4687,11 @@
       </c>
       <c r="Q7" s="32"/>
       <c r="R7" s="46">
-        <v>3.6000000000000004E-2</v>
+        <v>-0.123</v>
       </c>
       <c r="S7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E7,R7/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.5900000000000001E-3</v>
       </c>
       <c r="T7" s="34"/>
     </row>
@@ -4772,14 +4772,14 @@
         <v>STISEK1WDFI=</v>
       </c>
       <c r="L9" s="153">
-        <v>4.1000000000000002E-2</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="M9" s="153">
         <v>0</v>
       </c>
       <c r="N9" s="46">
         <f t="shared" si="1"/>
-        <v>4.1000000000000002E-2</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="O9" s="32" t="s">
         <v>154</v>
@@ -4789,11 +4789,11 @@
       </c>
       <c r="Q9" s="32"/>
       <c r="R9" s="46">
-        <v>4.1000000000000002E-2</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="S9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E9,R9/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.7600000000000001E-3</v>
       </c>
       <c r="T9" s="34"/>
     </row>
@@ -4925,14 +4925,14 @@
         <v>STISEK1MDFI=</v>
       </c>
       <c r="L12" s="153">
-        <v>-1.1000000000000001E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="M12" s="153">
         <v>0</v>
       </c>
       <c r="N12" s="46">
         <f t="shared" si="1"/>
-        <v>-1.1000000000000001E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="O12" s="32" t="s">
         <v>154</v>
@@ -4942,11 +4942,11 @@
       </c>
       <c r="Q12" s="32"/>
       <c r="R12" s="46">
-        <v>-1.1000000000000001E-2</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="S12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E12,R12/100,Trigger)</f>
-        <v>0</v>
+        <v>-6.4999999999999997E-4</v>
       </c>
       <c r="T12" s="34"/>
     </row>
@@ -4976,14 +4976,14 @@
         <v>STISEK2MDFI=</v>
       </c>
       <c r="L13" s="153">
-        <v>7.0000000000000001E-3</v>
+        <v>-6.9999999999999993E-2</v>
       </c>
       <c r="M13" s="153">
         <v>0</v>
       </c>
       <c r="N13" s="46">
         <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+        <v>-6.9999999999999993E-2</v>
       </c>
       <c r="O13" s="32" t="s">
         <v>154</v>
@@ -4993,11 +4993,11 @@
       </c>
       <c r="Q13" s="32"/>
       <c r="R13" s="46">
-        <v>7.0000000000000001E-3</v>
+        <v>-6.9999999999999993E-2</v>
       </c>
       <c r="S13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E13,R13/100,Trigger)</f>
-        <v>0</v>
+        <v>-7.6999999999999985E-4</v>
       </c>
       <c r="T13" s="34"/>
     </row>
@@ -5027,14 +5027,14 @@
         <v>STISEK3MDFI=</v>
       </c>
       <c r="L14" s="153">
-        <v>4.7E-2</v>
+        <v>-5.5000000000000007E-2</v>
       </c>
       <c r="M14" s="153">
         <v>0</v>
       </c>
       <c r="N14" s="46">
         <f t="shared" si="1"/>
-        <v>4.7E-2</v>
+        <v>-5.5000000000000007E-2</v>
       </c>
       <c r="O14" s="32" t="s">
         <v>154</v>
@@ -5044,11 +5044,11 @@
       </c>
       <c r="Q14" s="32"/>
       <c r="R14" s="46">
-        <v>4.7E-2</v>
+        <v>-5.5000000000000007E-2</v>
       </c>
       <c r="S14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E14,R14/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.0200000000000001E-3</v>
       </c>
       <c r="T14" s="34"/>
     </row>
@@ -5180,14 +5180,14 @@
         <v>STISEK6MDFI=</v>
       </c>
       <c r="L17" s="153">
-        <v>0.129</v>
+        <v>-2.7000000000000003E-2</v>
       </c>
       <c r="M17" s="153">
         <v>0</v>
       </c>
       <c r="N17" s="46">
         <f t="shared" si="1"/>
-        <v>0.129</v>
+        <v>-2.7000000000000003E-2</v>
       </c>
       <c r="O17" s="32" t="s">
         <v>154</v>
@@ -5197,11 +5197,11 @@
       </c>
       <c r="Q17" s="32"/>
       <c r="R17" s="46">
-        <v>0.129</v>
+        <v>-2.7000000000000003E-2</v>
       </c>
       <c r="S17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E17,R17/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.5600000000000002E-3</v>
       </c>
       <c r="T17" s="34"/>
     </row>
@@ -5690,7 +5690,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="33">
         <f>_xll.ohTrigger(X6:X20)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="34"/>
       <c r="AA4" s="28"/>
@@ -5721,7 +5721,7 @@
       <c r="M5" s="175"/>
       <c r="N5" s="176" t="str">
         <f>_xll.RData(N6:N20,O5:R5,"RTFEED:IDN",ReutersRtMode,,O6)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="O5" s="168" t="s">
         <v>106</v>
@@ -5804,10 +5804,10 @@
         <v>SEK3F1=HBCO</v>
       </c>
       <c r="O6" s="39">
-        <v>5.2500000000000005E-2</v>
+        <v>-0.10500000000000001</v>
       </c>
       <c r="P6" s="39">
-        <v>7.2500000000000009E-2</v>
+        <v>-8.4999999999999992E-2</v>
       </c>
       <c r="Q6" s="37">
         <v>0</v>
@@ -5817,7 +5817,7 @@
       </c>
       <c r="S6" s="39">
         <f>IF(ISERROR(AVERAGE(O6,P6)),#NUM!,AVERAGE(O6,P6))</f>
-        <v>6.25E-2</v>
+        <v>-9.5000000000000001E-2</v>
       </c>
       <c r="T6" s="32"/>
       <c r="U6" s="40">
@@ -5826,11 +5826,11 @@
       <c r="V6" s="32"/>
       <c r="W6" s="40">
         <f t="array" ref="W6:W20">QuoteLive</f>
-        <v>6.25E-2</v>
+        <v>-9.5000000000000001E-2</v>
       </c>
       <c r="X6" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/100,Trigger)</f>
-        <v>-2.4999999999999957E-5</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="AA6" s="28"/>
@@ -5844,11 +5844,11 @@
       </c>
       <c r="AD6" s="199">
         <f>100-W6</f>
-        <v>99.9375</v>
+        <v>100.095</v>
       </c>
       <c r="AE6" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC6,AD6,Trigger)</f>
-        <v>2.4999999999977263E-3</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="59"/>
     </row>
@@ -5890,10 +5890,10 @@
         <v>SEK3F2=HBCO</v>
       </c>
       <c r="O7" s="46">
-        <v>2.5000000000000001E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="P7" s="46">
-        <v>4.5000000000000005E-2</v>
+        <v>-0.10500000000000001</v>
       </c>
       <c r="Q7" s="44">
         <v>0</v>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="S7" s="46">
         <f t="shared" ref="S7:S20" si="4">IF(ISERROR(AVERAGE(O7,P7)),#NUM!,AVERAGE(O7,P7))</f>
-        <v>3.5000000000000003E-2</v>
+        <v>-0.115</v>
       </c>
       <c r="T7" s="32"/>
       <c r="U7" s="47">
@@ -5911,11 +5911,11 @@
       </c>
       <c r="V7" s="32"/>
       <c r="W7" s="47">
-        <v>3.5000000000000003E-2</v>
+        <v>-0.115</v>
       </c>
       <c r="X7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F7,W7/100,Trigger)</f>
-        <v>-4.9999999999999969E-5</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="34"/>
       <c r="AA7" s="28"/>
@@ -5929,11 +5929,11 @@
       </c>
       <c r="AD7" s="200">
         <f t="shared" ref="AD7:AD20" si="6">100-W7</f>
-        <v>99.965000000000003</v>
+        <v>100.11499999999999</v>
       </c>
       <c r="AE7" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC7,AD7,Trigger)</f>
-        <v>5.0000000000096634E-3</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="59"/>
     </row>
@@ -5975,10 +5975,10 @@
         <v>SEK3F3=HBCO</v>
       </c>
       <c r="O8" s="46">
-        <v>2.5000000000000001E-2</v>
+        <v>-0.13</v>
       </c>
       <c r="P8" s="46">
-        <v>4.5000000000000005E-2</v>
+        <v>-0.11000000000000001</v>
       </c>
       <c r="Q8" s="44">
         <v>0</v>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="S8" s="46">
         <f t="shared" si="4"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-0.12000000000000001</v>
       </c>
       <c r="T8" s="32"/>
       <c r="U8" s="47">
@@ -5996,11 +5996,11 @@
       </c>
       <c r="V8" s="32"/>
       <c r="W8" s="47">
-        <v>3.5000000000000003E-2</v>
+        <v>-0.12000000000000001</v>
       </c>
       <c r="X8" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F8,W8/100,Trigger)</f>
-        <v>-4.9999999999999969E-5</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="34"/>
       <c r="AA8" s="28"/>
@@ -6014,11 +6014,11 @@
       </c>
       <c r="AD8" s="200">
         <f t="shared" si="6"/>
-        <v>99.965000000000003</v>
+        <v>100.12</v>
       </c>
       <c r="AE8" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC8,AD8,Trigger)</f>
-        <v>5.0000000000096634E-3</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="59"/>
     </row>
@@ -6060,10 +6060,10 @@
         <v>SEK3F4=HBCO</v>
       </c>
       <c r="O9" s="46">
-        <v>3.5000000000000003E-2</v>
+        <v>-9.7500000000000003E-2</v>
       </c>
       <c r="P9" s="46">
-        <v>5.5E-2</v>
+        <v>-7.7499999999999999E-2</v>
       </c>
       <c r="Q9" s="44">
         <v>0</v>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="S9" s="46">
         <f t="shared" si="4"/>
-        <v>4.4999999999999998E-2</v>
+        <v>-8.7499999999999994E-2</v>
       </c>
       <c r="T9" s="32"/>
       <c r="U9" s="47">
@@ -6081,11 +6081,11 @@
       </c>
       <c r="V9" s="32"/>
       <c r="W9" s="47">
-        <v>4.4999999999999998E-2</v>
+        <v>-8.7499999999999994E-2</v>
       </c>
       <c r="X9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F9,W9/100,Trigger)</f>
-        <v>-1.0000000000000005E-4</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="34"/>
       <c r="AA9" s="28"/>
@@ -6099,11 +6099,11 @@
       </c>
       <c r="AD9" s="200">
         <f t="shared" si="6"/>
-        <v>99.954999999999998</v>
+        <v>100.08750000000001</v>
       </c>
       <c r="AE9" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC9,AD9,Trigger)</f>
-        <v>1.0000000000005116E-2</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="59"/>
     </row>
@@ -6145,10 +6145,10 @@
         <v>SEK3F5=HBCO</v>
       </c>
       <c r="O10" s="46">
-        <v>6.0000000000000005E-2</v>
+        <v>-5.7499999999999996E-2</v>
       </c>
       <c r="P10" s="46">
-        <v>9.0000000000000011E-2</v>
+        <v>-2.7500000000000004E-2</v>
       </c>
       <c r="Q10" s="44">
         <v>0</v>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="S10" s="46">
         <f t="shared" si="4"/>
-        <v>7.5000000000000011E-2</v>
+        <v>-4.2499999999999996E-2</v>
       </c>
       <c r="T10" s="32"/>
       <c r="U10" s="47">
@@ -6166,11 +6166,11 @@
       </c>
       <c r="V10" s="32"/>
       <c r="W10" s="47">
-        <v>7.5000000000000011E-2</v>
+        <v>-4.2499999999999996E-2</v>
       </c>
       <c r="X10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/100,Trigger)</f>
-        <v>-7.4999999999999871E-5</v>
+        <v>-2.4999999999999903E-5</v>
       </c>
       <c r="Y10" s="34"/>
       <c r="AA10" s="28"/>
@@ -6184,11 +6184,11 @@
       </c>
       <c r="AD10" s="200">
         <f t="shared" si="6"/>
-        <v>99.924999999999997</v>
+        <v>100.0425</v>
       </c>
       <c r="AE10" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC10,AD10,Trigger)</f>
-        <v>7.4999999999931788E-3</v>
+        <v>2.4999999999977263E-3</v>
       </c>
       <c r="AF10" s="59"/>
     </row>
@@ -6230,10 +6230,10 @@
         <v>SEK3F6=HBCO</v>
       </c>
       <c r="O11" s="46">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="P11" s="46">
-        <v>0.13</v>
+        <v>0.04</v>
       </c>
       <c r="Q11" s="44">
         <v>0</v>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="S11" s="46">
         <f t="shared" si="4"/>
-        <v>0.115</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="T11" s="32"/>
       <c r="U11" s="47">
@@ -6251,11 +6251,11 @@
       </c>
       <c r="V11" s="32"/>
       <c r="W11" s="47">
-        <v>0.115</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="X11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/100,Trigger)</f>
-        <v>-5.0000000000000131E-5</v>
+        <v>-2.4999999999999957E-5</v>
       </c>
       <c r="Y11" s="34"/>
       <c r="AA11" s="28"/>
@@ -6269,11 +6269,11 @@
       </c>
       <c r="AD11" s="200">
         <f t="shared" si="6"/>
-        <v>99.885000000000005</v>
+        <v>99.974999999999994</v>
       </c>
       <c r="AE11" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC11,AD11,Trigger)</f>
-        <v>5.0000000000096634E-3</v>
+        <v>2.4999999999977263E-3</v>
       </c>
       <c r="AF11" s="59"/>
     </row>
@@ -6315,10 +6315,10 @@
         <v>SEK3F7=HBCO</v>
       </c>
       <c r="O12" s="46">
-        <v>0.155</v>
+        <v>0.09</v>
       </c>
       <c r="P12" s="46">
-        <v>0.185</v>
+        <v>0.12</v>
       </c>
       <c r="Q12" s="44">
         <v>0</v>
@@ -6328,7 +6328,7 @@
       </c>
       <c r="S12" s="46">
         <f t="shared" si="4"/>
-        <v>0.16999999999999998</v>
+        <v>0.105</v>
       </c>
       <c r="T12" s="32"/>
       <c r="U12" s="47">
@@ -6336,7 +6336,7 @@
       </c>
       <c r="V12" s="32"/>
       <c r="W12" s="47">
-        <v>0.16999999999999998</v>
+        <v>0.105</v>
       </c>
       <c r="X12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/100,Trigger)</f>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="AD12" s="200">
         <f t="shared" si="6"/>
-        <v>99.83</v>
+        <v>99.894999999999996</v>
       </c>
       <c r="AE12" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC12,AD12,Trigger)</f>
@@ -6400,10 +6400,10 @@
         <v>SEK3F8=HBCO</v>
       </c>
       <c r="O13" s="46">
-        <v>0.22</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P13" s="46">
-        <v>0.25</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="Q13" s="44">
         <v>0</v>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="S13" s="46">
         <f t="shared" si="4"/>
-        <v>0.23499999999999999</v>
+        <v>0.19</v>
       </c>
       <c r="T13" s="32"/>
       <c r="U13" s="47">
@@ -6421,11 +6421,11 @@
       </c>
       <c r="V13" s="32"/>
       <c r="W13" s="47">
-        <v>0.23499999999999999</v>
+        <v>0.19</v>
       </c>
       <c r="X13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/100,Trigger)</f>
-        <v>4.9999999999999697E-5</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="34"/>
       <c r="AA13" s="28"/>
@@ -6439,11 +6439,11 @@
       </c>
       <c r="AD13" s="200">
         <f t="shared" si="6"/>
-        <v>99.765000000000001</v>
+        <v>99.81</v>
       </c>
       <c r="AE13" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC13,AD13,Trigger)</f>
-        <v>-4.9999999999954525E-3</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="59"/>
     </row>
@@ -6485,10 +6485,10 @@
         <v>SEK3F9=HBCO</v>
       </c>
       <c r="O14" s="46">
-        <v>0.28000000000000003</v>
+        <v>0.255</v>
       </c>
       <c r="P14" s="46">
-        <v>0.32</v>
+        <v>0.29500000000000004</v>
       </c>
       <c r="Q14" s="44">
         <v>0</v>
@@ -6498,7 +6498,7 @@
       </c>
       <c r="S14" s="46">
         <f t="shared" si="4"/>
-        <v>0.30000000000000004</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="T14" s="32"/>
       <c r="U14" s="47">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="V14" s="32"/>
       <c r="W14" s="47">
-        <v>0.30000000000000004</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="X14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,W14/100,Trigger)</f>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="AD14" s="200">
         <f t="shared" si="6"/>
-        <v>99.7</v>
+        <v>99.724999999999994</v>
       </c>
       <c r="AE14" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC14,AD14,Trigger)</f>
@@ -6570,10 +6570,10 @@
         <v>SEK3F10=HBCO</v>
       </c>
       <c r="O15" s="46">
-        <v>0.35000000000000003</v>
+        <v>0.34249999999999997</v>
       </c>
       <c r="P15" s="46">
-        <v>0.39</v>
+        <v>0.38250000000000001</v>
       </c>
       <c r="Q15" s="44">
         <v>0</v>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="S15" s="46">
         <f t="shared" si="4"/>
-        <v>0.37</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="T15" s="32"/>
       <c r="U15" s="47">
@@ -6591,11 +6591,11 @@
       </c>
       <c r="V15" s="32"/>
       <c r="W15" s="47">
-        <v>0.37</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="X15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/100,Trigger)</f>
-        <v>-7.5000000000000414E-5</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="34"/>
       <c r="AA15" s="28"/>
@@ -6609,11 +6609,11 @@
       </c>
       <c r="AD15" s="200">
         <f t="shared" si="6"/>
-        <v>99.63</v>
+        <v>99.637500000000003</v>
       </c>
       <c r="AE15" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC15,AD15,Trigger)</f>
-        <v>7.4999999999931788E-3</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="59"/>
     </row>
@@ -6655,10 +6655,10 @@
         <v>SEK3F11=HBCO</v>
       </c>
       <c r="O16" s="46">
-        <v>0.42500000000000004</v>
+        <v>0.43</v>
       </c>
       <c r="P16" s="46">
-        <v>0.46500000000000002</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="Q16" s="44">
         <v>0</v>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="S16" s="46">
         <f t="shared" si="4"/>
-        <v>0.44500000000000006</v>
+        <v>0.45</v>
       </c>
       <c r="T16" s="32"/>
       <c r="U16" s="47">
@@ -6676,11 +6676,11 @@
       </c>
       <c r="V16" s="32"/>
       <c r="W16" s="47">
-        <v>0.44500000000000006</v>
+        <v>0.45</v>
       </c>
       <c r="X16" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F16,W16/100,Trigger)</f>
-        <v>-1.2499999999999924E-4</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="34"/>
       <c r="AA16" s="28"/>
@@ -6694,11 +6694,11 @@
       </c>
       <c r="AD16" s="200">
         <f t="shared" si="6"/>
-        <v>99.555000000000007</v>
+        <v>99.55</v>
       </c>
       <c r="AE16" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC16,AD16,Trigger)</f>
-        <v>1.2500000000002842E-2</v>
+        <v>0</v>
       </c>
       <c r="AF16" s="59"/>
     </row>
@@ -6740,10 +6740,10 @@
         <v>SEK3F12=HBCO</v>
       </c>
       <c r="O17" s="46">
-        <v>0.5</v>
+        <v>0.51749999999999996</v>
       </c>
       <c r="P17" s="46">
-        <v>0.54</v>
+        <v>0.5575</v>
       </c>
       <c r="Q17" s="44">
         <v>0</v>
@@ -6753,7 +6753,7 @@
       </c>
       <c r="S17" s="46">
         <f t="shared" si="4"/>
-        <v>0.52</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="T17" s="32"/>
       <c r="U17" s="47">
@@ -6761,11 +6761,11 @@
       </c>
       <c r="V17" s="32"/>
       <c r="W17" s="47">
-        <v>0.52</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="X17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F17,W17/100,Trigger)</f>
-        <v>-1.7500000000000154E-4</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="AA17" s="28"/>
@@ -6779,11 +6779,11 @@
       </c>
       <c r="AD17" s="200">
         <f t="shared" si="6"/>
-        <v>99.48</v>
+        <v>99.462500000000006</v>
       </c>
       <c r="AE17" s="61">
         <f>_xll.qlSimpleQuoteSetValue(AC17,AD17,Trigger)</f>
-        <v>1.7499999999998295E-2</v>
+        <v>0</v>
       </c>
       <c r="AF17" s="59"/>
     </row>
@@ -7099,7 +7099,7 @@
   <dimension ref="B1:AC99"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -7224,7 +7224,10 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="7" t="b">
+        <f t="array" ref="Q5">AND(_xll.ohFilter($Q$22:$Q$61,NOT($Q$22:$Q$61="The record could not be found"))=0)</f>
+        <v>1</v>
+      </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -7234,7 +7237,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="33">
         <f>_xll.ohTrigger(Y7:Y61)</f>
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="Z5" s="34"/>
     </row>
@@ -7260,7 +7263,7 @@
       <c r="N6" s="234"/>
       <c r="O6" s="235" t="str">
         <f>_xll.RData(O7:O61,P6:S6,"RTFEED:IDN",ReutersRtMode,,P7)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="P6" s="190" t="s">
         <v>106</v>
@@ -7543,10 +7546,10 @@
         <v>SEKAMTNS1M=HBCO</v>
       </c>
       <c r="P10" s="46">
-        <v>-1.0999999999999999E-2</v>
+        <v>-0.22799999999999998</v>
       </c>
       <c r="Q10" s="46">
-        <v>1.9E-2</v>
+        <v>-0.19800000000000001</v>
       </c>
       <c r="R10" s="46">
         <v>0</v>
@@ -7556,7 +7559,7 @@
       </c>
       <c r="T10" s="46">
         <f t="shared" si="2"/>
-        <v>4.0000000000000001E-3</v>
+        <v>-0.21299999999999999</v>
       </c>
       <c r="U10" s="231"/>
       <c r="V10" s="233">
@@ -7564,11 +7567,11 @@
       </c>
       <c r="W10" s="231"/>
       <c r="X10" s="46">
-        <v>4.0000000000000001E-3</v>
+        <v>-0.21299999999999999</v>
       </c>
       <c r="Y10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,X10/100,Trigger)</f>
-        <v>-4.0000000000000003E-5</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="34"/>
       <c r="AB10" s="237"/>
@@ -7614,10 +7617,10 @@
         <v>SEKAMTNS2M=HBCO</v>
       </c>
       <c r="P11" s="46">
-        <v>-2.4E-2</v>
+        <v>-0.23900000000000002</v>
       </c>
       <c r="Q11" s="46">
-        <v>6.0000000000000001E-3</v>
+        <v>-0.20899999999999999</v>
       </c>
       <c r="R11" s="46">
         <v>0</v>
@@ -7627,7 +7630,7 @@
       </c>
       <c r="T11" s="46">
         <f t="shared" si="2"/>
-        <v>-9.0000000000000011E-3</v>
+        <v>-0.224</v>
       </c>
       <c r="U11" s="231"/>
       <c r="V11" s="233">
@@ -7635,11 +7638,11 @@
       </c>
       <c r="W11" s="231"/>
       <c r="X11" s="46">
-        <v>-9.0000000000000011E-3</v>
+        <v>-0.224</v>
       </c>
       <c r="Y11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
-        <v>-2.0000000000000012E-5</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="34"/>
     </row>
@@ -7684,10 +7687,10 @@
         <v>SEKAMTNS3M=HBCO</v>
       </c>
       <c r="P12" s="46">
-        <v>-2.9000000000000001E-2</v>
+        <v>-0.24700000000000003</v>
       </c>
       <c r="Q12" s="46">
-        <v>1E-3</v>
+        <v>-0.217</v>
       </c>
       <c r="R12" s="46">
         <v>0</v>
@@ -7697,7 +7700,7 @@
       </c>
       <c r="T12" s="46">
         <f t="shared" si="2"/>
-        <v>-1.4E-2</v>
+        <v>-0.23200000000000001</v>
       </c>
       <c r="U12" s="231"/>
       <c r="V12" s="233">
@@ -7705,11 +7708,11 @@
       </c>
       <c r="W12" s="231"/>
       <c r="X12" s="46">
-        <v>-1.4E-2</v>
+        <v>-0.23200000000000001</v>
       </c>
       <c r="Y12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
-        <v>-9.9999999999999991E-6</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="34"/>
     </row>
@@ -7754,10 +7757,10 @@
         <v>SEKAMTNS4M=HBCO</v>
       </c>
       <c r="P13" s="46">
-        <v>-3.9E-2</v>
+        <v>-0.252</v>
       </c>
       <c r="Q13" s="46">
-        <v>-9.0000000000000011E-3</v>
+        <v>-0.22200000000000003</v>
       </c>
       <c r="R13" s="46">
         <v>0</v>
@@ -7767,7 +7770,7 @@
       </c>
       <c r="T13" s="46">
         <f t="shared" si="2"/>
-        <v>-2.4E-2</v>
+        <v>-0.23700000000000002</v>
       </c>
       <c r="U13" s="231"/>
       <c r="V13" s="233">
@@ -7775,11 +7778,11 @@
       </c>
       <c r="W13" s="231"/>
       <c r="X13" s="46">
-        <v>-2.4E-2</v>
+        <v>-0.23700000000000002</v>
       </c>
       <c r="Y13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,X13/100,Trigger)</f>
-        <v>-2.0000000000000025E-5</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="34"/>
     </row>
@@ -7824,10 +7827,10 @@
         <v>SEKAMTNS5M=HBCO</v>
       </c>
       <c r="P14" s="46">
-        <v>-4.4999999999999998E-2</v>
+        <v>-0.255</v>
       </c>
       <c r="Q14" s="46">
-        <v>-1.4999999999999999E-2</v>
+        <v>-0.22500000000000001</v>
       </c>
       <c r="R14" s="46">
         <v>0</v>
@@ -7837,7 +7840,7 @@
       </c>
       <c r="T14" s="46">
         <f t="shared" si="2"/>
-        <v>-0.03</v>
+        <v>-0.24</v>
       </c>
       <c r="U14" s="231"/>
       <c r="V14" s="233">
@@ -7845,11 +7848,11 @@
       </c>
       <c r="W14" s="231"/>
       <c r="X14" s="46">
-        <v>-0.03</v>
+        <v>-0.24</v>
       </c>
       <c r="Y14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,X14/100,Trigger)</f>
-        <v>-1.9999999999999944E-5</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="34"/>
     </row>
@@ -7894,10 +7897,10 @@
         <v>SEKAMTNS6M=HBCO</v>
       </c>
       <c r="P15" s="46">
-        <v>-5.1000000000000004E-2</v>
+        <v>-0.25800000000000001</v>
       </c>
       <c r="Q15" s="46">
-        <v>-2.1000000000000001E-2</v>
+        <v>-0.22799999999999998</v>
       </c>
       <c r="R15" s="46">
         <v>0</v>
@@ -7907,7 +7910,7 @@
       </c>
       <c r="T15" s="46">
         <f t="shared" si="2"/>
-        <v>-3.6000000000000004E-2</v>
+        <v>-0.24299999999999999</v>
       </c>
       <c r="U15" s="231"/>
       <c r="V15" s="233">
@@ -7915,11 +7918,11 @@
       </c>
       <c r="W15" s="231"/>
       <c r="X15" s="46">
-        <v>-3.6000000000000004E-2</v>
+        <v>-0.24299999999999999</v>
       </c>
       <c r="Y15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,X15/100,Trigger)</f>
-        <v>-3.0000000000000024E-5</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="34"/>
     </row>
@@ -8105,10 +8108,10 @@
         <v>SEKAMTNS9M=HBCO</v>
       </c>
       <c r="P18" s="46">
-        <v>-0.06</v>
+        <v>-0.26100000000000001</v>
       </c>
       <c r="Q18" s="46">
-        <v>-0.03</v>
+        <v>-0.23100000000000001</v>
       </c>
       <c r="R18" s="46">
         <v>0</v>
@@ -8118,7 +8121,7 @@
       </c>
       <c r="T18" s="46">
         <f t="shared" si="2"/>
-        <v>-4.4999999999999998E-2</v>
+        <v>-0.246</v>
       </c>
       <c r="U18" s="231"/>
       <c r="V18" s="233">
@@ -8126,11 +8129,11 @@
       </c>
       <c r="W18" s="231"/>
       <c r="X18" s="46">
-        <v>-4.4999999999999998E-2</v>
+        <v>-0.246</v>
       </c>
       <c r="Y18" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F18,X18/100,Trigger)</f>
-        <v>-2.999999999999997E-5</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="34"/>
       <c r="AC18" s="237"/>
@@ -8316,10 +8319,10 @@
         <v>SEKAMTNS12M=HBCO</v>
       </c>
       <c r="P21" s="46">
-        <v>-6.6000000000000003E-2</v>
+        <v>-0.254</v>
       </c>
       <c r="Q21" s="46">
-        <v>-3.6000000000000004E-2</v>
+        <v>-0.22400000000000003</v>
       </c>
       <c r="R21" s="46">
         <v>0</v>
@@ -8329,7 +8332,7 @@
       </c>
       <c r="T21" s="46">
         <f t="shared" si="2"/>
-        <v>-5.1000000000000004E-2</v>
+        <v>-0.23900000000000002</v>
       </c>
       <c r="U21" s="231"/>
       <c r="V21" s="233">
@@ -8337,11 +8340,11 @@
       </c>
       <c r="W21" s="231"/>
       <c r="X21" s="46">
-        <v>-5.1000000000000004E-2</v>
+        <v>-0.23900000000000002</v>
       </c>
       <c r="Y21" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F21,X21/100,Trigger)</f>
-        <v>-5.0000000000000023E-5</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="34"/>
     </row>
@@ -8385,7 +8388,7 @@
         <v>SEKAMTNS1Y=ICAP</v>
       </c>
       <c r="P22" s="39">
-        <v>-0.05</v>
+        <v>-0.24</v>
       </c>
       <c r="Q22" s="39">
         <v>0</v>
@@ -8397,8 +8400,8 @@
         <v>0</v>
       </c>
       <c r="T22" s="39">
-        <f t="shared" si="2"/>
-        <v>-2.5000000000000001E-2</v>
+        <f>IF(ISERROR(AVERAGE(P22,Q22)),#NUM!,IF($Q$5,P22,AVERAGE(P22,Q22)))</f>
+        <v>-0.24</v>
       </c>
       <c r="U22" s="231"/>
       <c r="V22" s="232">
@@ -8406,11 +8409,11 @@
       </c>
       <c r="W22" s="231"/>
       <c r="X22" s="39">
-        <v>-2.5000000000000001E-2</v>
+        <v>-0.24</v>
       </c>
       <c r="Y22" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F22,X22/100,Trigger)</f>
-        <v>-2.4999999999999984E-5</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="Z22" s="34"/>
     </row>
@@ -8467,7 +8470,7 @@
         <v>153</v>
       </c>
       <c r="T23" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T23:T61" si="3">IF(ISERROR(AVERAGE(P23,Q23)),#NUM!,IF($Q$5,P23,AVERAGE(P23,Q23)))</f>
         <v>#NUM!</v>
       </c>
       <c r="U23" s="231"/>
@@ -8537,7 +8540,7 @@
         <v>153</v>
       </c>
       <c r="T24" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U24" s="231"/>
@@ -8607,7 +8610,7 @@
         <v>153</v>
       </c>
       <c r="T25" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U25" s="231"/>
@@ -8677,7 +8680,7 @@
         <v>153</v>
       </c>
       <c r="T26" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U26" s="231"/>
@@ -8747,7 +8750,7 @@
         <v>153</v>
       </c>
       <c r="T27" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U27" s="231"/>
@@ -8817,7 +8820,7 @@
         <v>153</v>
       </c>
       <c r="T28" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U28" s="231"/>
@@ -8887,7 +8890,7 @@
         <v>153</v>
       </c>
       <c r="T29" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U29" s="231"/>
@@ -8958,7 +8961,7 @@
         <v>153</v>
       </c>
       <c r="T30" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U30" s="231"/>
@@ -9028,7 +9031,7 @@
         <v>153</v>
       </c>
       <c r="T31" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U31" s="231"/>
@@ -9098,7 +9101,7 @@
         <v>153</v>
       </c>
       <c r="T32" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U32" s="231"/>
@@ -9168,7 +9171,7 @@
         <v>153</v>
       </c>
       <c r="T33" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U33" s="231"/>
@@ -9226,7 +9229,7 @@
         <v>SEKAMTNS2Y=ICAP</v>
       </c>
       <c r="P34" s="46">
-        <v>-0.125</v>
+        <v>-0.1925</v>
       </c>
       <c r="Q34" s="46">
         <v>0</v>
@@ -9238,8 +9241,8 @@
         <v>0</v>
       </c>
       <c r="T34" s="46">
-        <f t="shared" si="2"/>
-        <v>-6.25E-2</v>
+        <f t="shared" si="3"/>
+        <v>-0.1925</v>
       </c>
       <c r="U34" s="231"/>
       <c r="V34" s="233">
@@ -9247,11 +9250,11 @@
       </c>
       <c r="W34" s="231"/>
       <c r="X34" s="46">
-        <v>-6.25E-2</v>
+        <v>-0.1925</v>
       </c>
       <c r="Y34" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F34,X34/100,Trigger)</f>
-        <v>0</v>
+        <v>-5.9625000000000008E-3</v>
       </c>
       <c r="Z34" s="34"/>
     </row>
@@ -9308,7 +9311,7 @@
         <v>153</v>
       </c>
       <c r="T35" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U35" s="231"/>
@@ -9378,7 +9381,7 @@
         <v>153</v>
       </c>
       <c r="T36" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U36" s="231"/>
@@ -9448,7 +9451,7 @@
         <v>153</v>
       </c>
       <c r="T37" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U37" s="231"/>
@@ -9506,7 +9509,7 @@
         <v>SEKAMTNS3Y=ICAP</v>
       </c>
       <c r="P38" s="46">
-        <v>-3.0000000000000002E-2</v>
+        <v>-7.7499999999999999E-2</v>
       </c>
       <c r="Q38" s="46">
         <v>0</v>
@@ -9518,8 +9521,8 @@
         <v>0</v>
       </c>
       <c r="T38" s="46">
-        <f t="shared" si="2"/>
-        <v>-1.5000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>-7.7499999999999999E-2</v>
       </c>
       <c r="U38" s="231"/>
       <c r="V38" s="233">
@@ -9527,11 +9530,11 @@
       </c>
       <c r="W38" s="231"/>
       <c r="X38" s="46">
-        <v>-1.5000000000000001E-2</v>
+        <v>-7.7499999999999999E-2</v>
       </c>
       <c r="Y38" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F38,X38/100,Trigger)</f>
-        <v>-1.2500000000000006E-5</v>
+        <v>-3.8749999999999999E-4</v>
       </c>
       <c r="Z38" s="34"/>
     </row>
@@ -9588,7 +9591,7 @@
         <v>153</v>
       </c>
       <c r="T39" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U39" s="231"/>
@@ -9614,7 +9617,7 @@
         <v>91</v>
       </c>
       <c r="E40" s="42" t="str">
-        <f t="shared" ref="E40:E61" si="3">Currency&amp;$C40&amp;$D40&amp;QuoteSuffix</f>
+        <f t="shared" ref="E40:E61" si="4">Currency&amp;$C40&amp;$D40&amp;QuoteSuffix</f>
         <v>SEKOIS42M_Quote</v>
       </c>
       <c r="F40" s="42" t="str">
@@ -9639,7 +9642,7 @@
         <v>164</v>
       </c>
       <c r="N40" s="228" t="str">
-        <f t="shared" ref="N40:N61" si="4">Currency&amp;L40&amp;M40&amp;K40</f>
+        <f t="shared" ref="N40:N61" si="5">Currency&amp;L40&amp;M40&amp;K40</f>
         <v>SEKAMTNS42M</v>
       </c>
       <c r="O40" s="228" t="str">
@@ -9658,7 +9661,7 @@
         <v>153</v>
       </c>
       <c r="T40" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U40" s="231"/>
@@ -9684,7 +9687,7 @@
         <v>90</v>
       </c>
       <c r="E41" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS45M_Quote</v>
       </c>
       <c r="F41" s="42" t="str">
@@ -9709,7 +9712,7 @@
         <v>164</v>
       </c>
       <c r="N41" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS45M</v>
       </c>
       <c r="O41" s="228" t="str">
@@ -9728,7 +9731,7 @@
         <v>153</v>
       </c>
       <c r="T41" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U41" s="231"/>
@@ -9754,7 +9757,7 @@
         <v>56</v>
       </c>
       <c r="E42" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS4Y_Quote</v>
       </c>
       <c r="F42" s="42" t="str">
@@ -9779,14 +9782,14 @@
         <v>164</v>
       </c>
       <c r="N42" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS4Y</v>
       </c>
       <c r="O42" s="228" t="str">
         <v>SEKAMTNS4Y=ICAP</v>
       </c>
       <c r="P42" s="46">
-        <v>0.08</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Q42" s="46">
         <v>0</v>
@@ -9798,8 +9801,8 @@
         <v>0</v>
       </c>
       <c r="T42" s="46">
-        <f t="shared" si="2"/>
-        <v>0.04</v>
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
       </c>
       <c r="U42" s="231"/>
       <c r="V42" s="233">
@@ -9807,11 +9810,11 @@
       </c>
       <c r="W42" s="231"/>
       <c r="X42" s="46">
-        <v>0.04</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Y42" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F42,X42/100,Trigger)</f>
-        <v>-1.2499999999999979E-5</v>
+        <v>3.1250000000000001E-4</v>
       </c>
       <c r="Z42" s="34"/>
     </row>
@@ -9824,7 +9827,7 @@
         <v>89</v>
       </c>
       <c r="E43" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS51M_Quote</v>
       </c>
       <c r="F43" s="42" t="str">
@@ -9849,7 +9852,7 @@
         <v>164</v>
       </c>
       <c r="N43" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS51M</v>
       </c>
       <c r="O43" s="228" t="str">
@@ -9868,7 +9871,7 @@
         <v>153</v>
       </c>
       <c r="T43" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U43" s="231"/>
@@ -9894,7 +9897,7 @@
         <v>88</v>
       </c>
       <c r="E44" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS54M_Quote</v>
       </c>
       <c r="F44" s="42" t="str">
@@ -9919,7 +9922,7 @@
         <v>164</v>
       </c>
       <c r="N44" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS54M</v>
       </c>
       <c r="O44" s="228" t="str">
@@ -9938,7 +9941,7 @@
         <v>153</v>
       </c>
       <c r="T44" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U44" s="231"/>
@@ -9964,7 +9967,7 @@
         <v>87</v>
       </c>
       <c r="E45" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS57M_Quote</v>
       </c>
       <c r="F45" s="42" t="str">
@@ -9989,7 +9992,7 @@
         <v>164</v>
       </c>
       <c r="N45" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS57M</v>
       </c>
       <c r="O45" s="228" t="str">
@@ -10008,7 +10011,7 @@
         <v>153</v>
       </c>
       <c r="T45" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U45" s="231"/>
@@ -10034,7 +10037,7 @@
         <v>55</v>
       </c>
       <c r="E46" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS5Y_Quote</v>
       </c>
       <c r="F46" s="42" t="str">
@@ -10059,14 +10062,14 @@
         <v>164</v>
       </c>
       <c r="N46" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS5Y</v>
       </c>
       <c r="O46" s="228" t="str">
         <v>SEKAMTNS5Y=ICAP</v>
       </c>
       <c r="P46" s="46">
-        <v>0.20750000000000002</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="Q46" s="46">
         <v>0</v>
@@ -10078,8 +10081,8 @@
         <v>0</v>
       </c>
       <c r="T46" s="46">
-        <f t="shared" si="2"/>
-        <v>0.10375000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.20499999999999999</v>
       </c>
       <c r="U46" s="231"/>
       <c r="V46" s="233">
@@ -10087,11 +10090,11 @@
       </c>
       <c r="W46" s="231"/>
       <c r="X46" s="46">
-        <v>0.10375000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="Y46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>-2.5000000000000066E-5</v>
+        <v>1.0249999999999999E-3</v>
       </c>
       <c r="Z46" s="34"/>
     </row>
@@ -10104,7 +10107,7 @@
         <v>54</v>
       </c>
       <c r="E47" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS6Y_Quote</v>
       </c>
       <c r="F47" s="42" t="str">
@@ -10129,14 +10132,14 @@
         <v>164</v>
       </c>
       <c r="N47" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS6Y</v>
       </c>
       <c r="O47" s="228" t="str">
         <v>SEKAMTNS6Y=ICAP</v>
       </c>
       <c r="P47" s="46">
-        <v>0.34250000000000003</v>
+        <v>0.34249999999999997</v>
       </c>
       <c r="Q47" s="46">
         <v>0</v>
@@ -10148,8 +10151,8 @@
         <v>0</v>
       </c>
       <c r="T47" s="46">
-        <f t="shared" si="2"/>
-        <v>0.17125000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.34249999999999997</v>
       </c>
       <c r="U47" s="231"/>
       <c r="V47" s="233">
@@ -10157,11 +10160,11 @@
       </c>
       <c r="W47" s="231"/>
       <c r="X47" s="46">
-        <v>0.17125000000000001</v>
+        <v>0.34249999999999997</v>
       </c>
       <c r="Y47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>-1.2500000000000141E-5</v>
+        <v>1.7124999999999998E-3</v>
       </c>
       <c r="Z47" s="34"/>
     </row>
@@ -10174,7 +10177,7 @@
         <v>53</v>
       </c>
       <c r="E48" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS7Y_Quote</v>
       </c>
       <c r="F48" s="42" t="str">
@@ -10199,14 +10202,14 @@
         <v>164</v>
       </c>
       <c r="N48" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS7Y</v>
       </c>
       <c r="O48" s="228" t="str">
         <v>SEKAMTNS7Y=ICAP</v>
       </c>
       <c r="P48" s="46">
-        <v>0.47000000000000003</v>
+        <v>0.46749999999999997</v>
       </c>
       <c r="Q48" s="46">
         <v>0</v>
@@ -10218,8 +10221,8 @@
         <v>0</v>
       </c>
       <c r="T48" s="46">
-        <f t="shared" si="2"/>
-        <v>0.23500000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.46749999999999997</v>
       </c>
       <c r="U48" s="231"/>
       <c r="V48" s="233">
@@ -10227,11 +10230,11 @@
       </c>
       <c r="W48" s="231"/>
       <c r="X48" s="46">
-        <v>0.23500000000000001</v>
+        <v>0.46749999999999997</v>
       </c>
       <c r="Y48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>-1.2499999999999924E-5</v>
+        <v>2.3374999999999997E-3</v>
       </c>
       <c r="Z48" s="34"/>
     </row>
@@ -10244,7 +10247,7 @@
         <v>52</v>
       </c>
       <c r="E49" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS8Y_Quote</v>
       </c>
       <c r="F49" s="42" t="str">
@@ -10269,14 +10272,14 @@
         <v>164</v>
       </c>
       <c r="N49" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS8Y</v>
       </c>
       <c r="O49" s="228" t="str">
         <v>SEKAMTNS8Y=ICAP</v>
       </c>
       <c r="P49" s="46">
-        <v>0.58500000000000008</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="Q49" s="46">
         <v>0</v>
@@ -10288,8 +10291,8 @@
         <v>0</v>
       </c>
       <c r="T49" s="46">
-        <f t="shared" si="2"/>
-        <v>0.29250000000000004</v>
+        <f t="shared" si="3"/>
+        <v>0.57499999999999996</v>
       </c>
       <c r="U49" s="231"/>
       <c r="V49" s="233">
@@ -10297,11 +10300,11 @@
       </c>
       <c r="W49" s="231"/>
       <c r="X49" s="46">
-        <v>0.29250000000000004</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="Y49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>-1.2499999999999491E-5</v>
+        <v>2.875E-3</v>
       </c>
       <c r="Z49" s="34"/>
     </row>
@@ -10314,7 +10317,7 @@
         <v>51</v>
       </c>
       <c r="E50" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS9Y_Quote</v>
       </c>
       <c r="F50" s="42" t="str">
@@ -10339,14 +10342,14 @@
         <v>164</v>
       </c>
       <c r="N50" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS9Y</v>
       </c>
       <c r="O50" s="228" t="str">
         <v>SEKAMTNS9Y=ICAP</v>
       </c>
       <c r="P50" s="46">
-        <v>0.68500000000000005</v>
+        <v>0.66249999999999998</v>
       </c>
       <c r="Q50" s="46">
         <v>0</v>
@@ -10358,8 +10361,8 @@
         <v>0</v>
       </c>
       <c r="T50" s="46">
-        <f t="shared" si="2"/>
-        <v>0.34250000000000003</v>
+        <f t="shared" si="3"/>
+        <v>0.66249999999999998</v>
       </c>
       <c r="U50" s="231"/>
       <c r="V50" s="233">
@@ -10367,11 +10370,11 @@
       </c>
       <c r="W50" s="231"/>
       <c r="X50" s="46">
-        <v>0.34250000000000003</v>
+        <v>0.66249999999999998</v>
       </c>
       <c r="Y50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>0</v>
+        <v>3.3124999999999999E-3</v>
       </c>
       <c r="Z50" s="34"/>
     </row>
@@ -10384,7 +10387,7 @@
         <v>50</v>
       </c>
       <c r="E51" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS10Y_Quote</v>
       </c>
       <c r="F51" s="42" t="str">
@@ -10409,14 +10412,14 @@
         <v>164</v>
       </c>
       <c r="N51" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS10Y</v>
       </c>
       <c r="O51" s="228" t="str">
         <v>SEKAMTNS10Y=ICAP</v>
       </c>
       <c r="P51" s="46">
-        <v>0.76500000000000001</v>
+        <v>0.73250000000000004</v>
       </c>
       <c r="Q51" s="46">
         <v>0</v>
@@ -10428,8 +10431,8 @@
         <v>0</v>
       </c>
       <c r="T51" s="46">
-        <f t="shared" si="2"/>
-        <v>0.38250000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.73250000000000004</v>
       </c>
       <c r="U51" s="231"/>
       <c r="V51" s="233">
@@ -10437,11 +10440,11 @@
       </c>
       <c r="W51" s="231"/>
       <c r="X51" s="46">
-        <v>0.38250000000000001</v>
+        <v>0.73250000000000004</v>
       </c>
       <c r="Y51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>-1.2499999999999924E-5</v>
+        <v>3.6625000000000004E-3</v>
       </c>
       <c r="Z51" s="34"/>
     </row>
@@ -10454,7 +10457,7 @@
         <v>48</v>
       </c>
       <c r="E52" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS12Y_Quote</v>
       </c>
       <c r="F52" s="42" t="str">
@@ -10479,14 +10482,14 @@
         <v>164</v>
       </c>
       <c r="N52" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS12Y</v>
       </c>
       <c r="O52" s="228" t="str">
         <v>SEKAMTNS12Y=ICAP</v>
       </c>
       <c r="P52" s="46">
-        <v>0.90750000000000008</v>
+        <v>0.85749999999999993</v>
       </c>
       <c r="Q52" s="46">
         <v>0</v>
@@ -10498,8 +10501,8 @@
         <v>0</v>
       </c>
       <c r="T52" s="46">
-        <f t="shared" si="2"/>
-        <v>0.45375000000000004</v>
+        <f t="shared" si="3"/>
+        <v>0.85749999999999993</v>
       </c>
       <c r="U52" s="231"/>
       <c r="V52" s="233">
@@ -10507,11 +10510,11 @@
       </c>
       <c r="W52" s="231"/>
       <c r="X52" s="46">
-        <v>0.45375000000000004</v>
+        <v>0.85749999999999993</v>
       </c>
       <c r="Y52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>-1.2499999999999491E-5</v>
+        <v>4.2874999999999996E-3</v>
       </c>
       <c r="Z52" s="34"/>
     </row>
@@ -10524,7 +10527,7 @@
         <v>45</v>
       </c>
       <c r="E53" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS15Y_Quote</v>
       </c>
       <c r="F53" s="42" t="str">
@@ -10549,14 +10552,14 @@
         <v>164</v>
       </c>
       <c r="N53" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS15Y</v>
       </c>
       <c r="O53" s="228" t="str">
         <v>SEKAMTNS15Y=ICAP</v>
       </c>
       <c r="P53" s="46">
-        <v>1.075</v>
+        <v>0.99749999999999994</v>
       </c>
       <c r="Q53" s="46">
         <v>0</v>
@@ -10568,8 +10571,8 @@
         <v>0</v>
       </c>
       <c r="T53" s="46">
-        <f t="shared" si="2"/>
-        <v>0.53749999999999998</v>
+        <f t="shared" si="3"/>
+        <v>0.99749999999999994</v>
       </c>
       <c r="U53" s="231"/>
       <c r="V53" s="233">
@@ -10577,11 +10580,11 @@
       </c>
       <c r="W53" s="231"/>
       <c r="X53" s="46">
-        <v>0.53749999999999998</v>
+        <v>0.99749999999999994</v>
       </c>
       <c r="Y53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F53,X53/100,Trigger)</f>
-        <v>-1.2500000000001225E-5</v>
+        <v>4.9874999999999997E-3</v>
       </c>
       <c r="Z53" s="34"/>
     </row>
@@ -10594,7 +10597,7 @@
         <v>40</v>
       </c>
       <c r="E54" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS20Y_Quote</v>
       </c>
       <c r="F54" s="42" t="str">
@@ -10619,14 +10622,14 @@
         <v>164</v>
       </c>
       <c r="N54" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS20Y</v>
       </c>
       <c r="O54" s="228" t="str">
         <v>SEKAMTNS20Y=ICAP</v>
       </c>
       <c r="P54" s="46">
-        <v>1.2650000000000001</v>
+        <v>1.1675</v>
       </c>
       <c r="Q54" s="46">
         <v>0</v>
@@ -10638,8 +10641,8 @@
         <v>0</v>
       </c>
       <c r="T54" s="46">
-        <f t="shared" si="2"/>
-        <v>0.63250000000000006</v>
+        <f t="shared" si="3"/>
+        <v>1.1675</v>
       </c>
       <c r="U54" s="231"/>
       <c r="V54" s="233">
@@ -10647,11 +10650,11 @@
       </c>
       <c r="W54" s="231"/>
       <c r="X54" s="46">
-        <v>0.63250000000000006</v>
+        <v>1.1675</v>
       </c>
       <c r="Y54" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>0</v>
+        <v>5.8374999999999998E-3</v>
       </c>
       <c r="Z54" s="34"/>
     </row>
@@ -10664,7 +10667,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS25Y_Quote</v>
       </c>
       <c r="F55" s="42" t="str">
@@ -10689,14 +10692,14 @@
         <v>164</v>
       </c>
       <c r="N55" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS25Y</v>
       </c>
       <c r="O55" s="228" t="str">
         <v>SEKAMTNS25Y=ICAP</v>
       </c>
       <c r="P55" s="46">
-        <v>1.34</v>
+        <v>1.2575000000000001</v>
       </c>
       <c r="Q55" s="46">
         <v>0</v>
@@ -10708,8 +10711,8 @@
         <v>0</v>
       </c>
       <c r="T55" s="46">
-        <f t="shared" si="2"/>
-        <v>0.67</v>
+        <f t="shared" si="3"/>
+        <v>1.2575000000000001</v>
       </c>
       <c r="U55" s="231"/>
       <c r="V55" s="233">
@@ -10717,11 +10720,11 @@
       </c>
       <c r="W55" s="231"/>
       <c r="X55" s="46">
-        <v>0.67</v>
+        <v>1.2575000000000001</v>
       </c>
       <c r="Y55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F55,X55/100,Trigger)</f>
-        <v>-1.2499999999999491E-5</v>
+        <v>6.2875000000000006E-3</v>
       </c>
       <c r="Z55" s="34"/>
     </row>
@@ -10734,7 +10737,7 @@
         <v>33</v>
       </c>
       <c r="E56" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS27Y_Quote</v>
       </c>
       <c r="F56" s="42" t="str">
@@ -10759,7 +10762,7 @@
         <v>164</v>
       </c>
       <c r="N56" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS27Y</v>
       </c>
       <c r="O56" s="228" t="str">
@@ -10778,7 +10781,7 @@
         <v>153</v>
       </c>
       <c r="T56" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U56" s="231"/>
@@ -10804,7 +10807,7 @@
         <v>30</v>
       </c>
       <c r="E57" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS30Y_Quote</v>
       </c>
       <c r="F57" s="42" t="str">
@@ -10829,14 +10832,14 @@
         <v>164</v>
       </c>
       <c r="N57" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS30Y</v>
       </c>
       <c r="O57" s="228" t="str">
         <v>SEKAMTNS30Y=ICAP</v>
       </c>
       <c r="P57" s="46">
-        <v>1.365</v>
+        <v>1.2925</v>
       </c>
       <c r="Q57" s="46">
         <v>0</v>
@@ -10848,8 +10851,8 @@
         <v>0</v>
       </c>
       <c r="T57" s="46">
-        <f t="shared" si="2"/>
-        <v>0.6825</v>
+        <f t="shared" si="3"/>
+        <v>1.2925</v>
       </c>
       <c r="U57" s="231"/>
       <c r="V57" s="233">
@@ -10857,11 +10860,11 @@
       </c>
       <c r="W57" s="231"/>
       <c r="X57" s="46">
-        <v>0.6825</v>
+        <v>1.2925</v>
       </c>
       <c r="Y57" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F57,X57/100,Trigger)</f>
-        <v>-1.2500000000000358E-5</v>
+        <v>6.4624999999999995E-3</v>
       </c>
       <c r="Z57" s="34"/>
     </row>
@@ -10874,7 +10877,7 @@
         <v>29</v>
       </c>
       <c r="E58" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS35Y_Quote</v>
       </c>
       <c r="F58" s="42" t="str">
@@ -10899,7 +10902,7 @@
         <v>164</v>
       </c>
       <c r="N58" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS35Y</v>
       </c>
       <c r="O58" s="228" t="str">
@@ -10918,7 +10921,7 @@
         <v>153</v>
       </c>
       <c r="T58" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U58" s="231"/>
@@ -10944,7 +10947,7 @@
         <v>28</v>
       </c>
       <c r="E59" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS40Y_Quote</v>
       </c>
       <c r="F59" s="42" t="str">
@@ -10969,7 +10972,7 @@
         <v>164</v>
       </c>
       <c r="N59" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS40Y</v>
       </c>
       <c r="O59" s="228" t="str">
@@ -10988,7 +10991,7 @@
         <v>153</v>
       </c>
       <c r="T59" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U59" s="231"/>
@@ -11014,7 +11017,7 @@
         <v>27</v>
       </c>
       <c r="E60" s="42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS45Y_Quote</v>
       </c>
       <c r="F60" s="42" t="str">
@@ -11039,7 +11042,7 @@
         <v>164</v>
       </c>
       <c r="N60" s="228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS45Y</v>
       </c>
       <c r="O60" s="228" t="str">
@@ -11058,7 +11061,7 @@
         <v>153</v>
       </c>
       <c r="T60" s="46" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U60" s="231"/>
@@ -11084,7 +11087,7 @@
         <v>26</v>
       </c>
       <c r="E61" s="49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>SEKOIS50Y_Quote</v>
       </c>
       <c r="F61" s="49" t="str">
@@ -11109,7 +11112,7 @@
         <v>164</v>
       </c>
       <c r="N61" s="229" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SEKAMTNS50Y</v>
       </c>
       <c r="O61" s="229" t="str">
@@ -11128,7 +11131,7 @@
         <v>153</v>
       </c>
       <c r="T61" s="53" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
       <c r="U61" s="231"/>
@@ -11445,7 +11448,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -12546,10 +12549,10 @@
         <v>SEKAB3S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>0.02</v>
+        <v>-0.12250000000000001</v>
       </c>
       <c r="R20" s="46">
-        <v>7.0000000000000007E-2</v>
+        <v>-7.2499999999999995E-2</v>
       </c>
       <c r="S20" s="46">
         <v>0</v>
@@ -12559,7 +12562,7 @@
       </c>
       <c r="U20" s="46">
         <f t="shared" si="2"/>
-        <v>4.5000000000000005E-2</v>
+        <v>-9.7500000000000003E-2</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -12567,11 +12570,11 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>4.5000000000000005E-2</v>
+        <v>-9.7500000000000003E-2</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/100,Trigger)</f>
-        <v>2.5000000000000011E-5</v>
+        <v>-1.4250000000000001E-3</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -13423,10 +13426,10 @@
         <v>SEKAB3S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>6.0000000000000005E-2</v>
+        <v>-6.7500000000000004E-2</v>
       </c>
       <c r="R32" s="46">
-        <v>0.11</v>
+        <v>-1.7499999999999998E-2</v>
       </c>
       <c r="S32" s="46">
         <v>0</v>
@@ -13436,7 +13439,7 @@
       </c>
       <c r="U32" s="46">
         <f t="shared" si="2"/>
-        <v>8.5000000000000006E-2</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -13444,11 +13447,11 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>8.5000000000000006E-2</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/100,Trigger)</f>
-        <v>0</v>
+        <v>-1.2750000000000001E-3</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -13715,10 +13718,10 @@
         <v>SEKAB3S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>0.155</v>
+        <v>5.7499999999999996E-2</v>
       </c>
       <c r="R36" s="46">
-        <v>0.20500000000000002</v>
+        <v>0.1075</v>
       </c>
       <c r="S36" s="46">
         <v>0</v>
@@ -13728,7 +13731,7 @@
       </c>
       <c r="U36" s="46">
         <f t="shared" si="2"/>
-        <v>0.18</v>
+        <v>8.249999999999999E-2</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -13736,11 +13739,11 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>0.18</v>
+        <v>8.249999999999999E-2</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/100,Trigger)</f>
-        <v>-2.5000000000000066E-5</v>
+        <v>-9.7500000000000006E-4</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -14007,10 +14010,10 @@
         <v>SEKAB3S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>0.27750000000000002</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="R40" s="46">
-        <v>0.32750000000000001</v>
+        <v>0.255</v>
       </c>
       <c r="S40" s="46">
         <v>0</v>
@@ -14020,7 +14023,7 @@
       </c>
       <c r="U40" s="46">
         <f t="shared" si="2"/>
-        <v>0.30249999999999999</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -14028,11 +14031,11 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>0.30249999999999999</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-7.2499999999999995E-4</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -14299,10 +14302,10 @@
         <v>SEKAB3S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>0.41250000000000003</v>
+        <v>0.35249999999999998</v>
       </c>
       <c r="R44" s="46">
-        <v>0.46250000000000002</v>
+        <v>0.40250000000000002</v>
       </c>
       <c r="S44" s="46">
         <v>0</v>
@@ -14312,7 +14315,7 @@
       </c>
       <c r="U44" s="46">
         <f t="shared" si="2"/>
-        <v>0.4375</v>
+        <v>0.3775</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -14320,11 +14323,11 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>0.4375</v>
+        <v>0.3775</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/100,Trigger)</f>
-        <v>-2.4999999999999849E-5</v>
+        <v>-6.0000000000000027E-4</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -14372,10 +14375,10 @@
         <v>SEKAB3S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
+        <v>0.495</v>
+      </c>
+      <c r="R45" s="46">
         <v>0.54500000000000004</v>
-      </c>
-      <c r="R45" s="46">
-        <v>0.59499999999999997</v>
       </c>
       <c r="S45" s="46">
         <v>0</v>
@@ -14385,7 +14388,7 @@
       </c>
       <c r="U45" s="46">
         <f t="shared" si="2"/>
-        <v>0.57000000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -14393,11 +14396,11 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>0.57000000000000006</v>
+        <v>0.52</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/100,Trigger)</f>
-        <v>-2.4999999999999849E-5</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -14445,10 +14448,10 @@
         <v>SEKAB3S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>0.67500000000000004</v>
+        <v>0.62</v>
       </c>
       <c r="R46" s="46">
-        <v>0.72500000000000009</v>
+        <v>0.67</v>
       </c>
       <c r="S46" s="46">
         <v>0</v>
@@ -14458,7 +14461,7 @@
       </c>
       <c r="U46" s="46">
         <f t="shared" si="2"/>
-        <v>0.70000000000000007</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -14466,11 +14469,11 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>0.70000000000000007</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/100,Trigger)</f>
-        <v>-2.4999999999998981E-5</v>
+        <v>-5.5000000000000101E-4</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -14518,10 +14521,10 @@
         <v>SEKAB3S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>0.79</v>
+        <v>0.72750000000000004</v>
       </c>
       <c r="R47" s="46">
-        <v>0.84000000000000008</v>
+        <v>0.77750000000000008</v>
       </c>
       <c r="S47" s="46">
         <v>0</v>
@@ -14531,7 +14534,7 @@
       </c>
       <c r="U47" s="46">
         <f t="shared" si="2"/>
-        <v>0.81500000000000006</v>
+        <v>0.75250000000000006</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -14539,11 +14542,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>0.81500000000000006</v>
+        <v>0.75250000000000006</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-6.2500000000000056E-4</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -14591,10 +14594,10 @@
         <v>SEKAB3S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>0.88750000000000007</v>
+        <v>0.81500000000000006</v>
       </c>
       <c r="R48" s="46">
-        <v>0.9375</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="S48" s="46">
         <v>0</v>
@@ -14604,7 +14607,7 @@
       </c>
       <c r="U48" s="46">
         <f t="shared" si="2"/>
-        <v>0.91250000000000009</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -14612,11 +14615,11 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>0.91250000000000009</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/100,Trigger)</f>
-        <v>-2.4999999999998981E-5</v>
+        <v>-7.2499999999999995E-4</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -14664,10 +14667,10 @@
         <v>SEKAB3S10Y=ICAP</v>
       </c>
       <c r="Q49" s="46">
-        <v>0.97000000000000008</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="R49" s="46">
-        <v>1.02</v>
+        <v>0.93499999999999994</v>
       </c>
       <c r="S49" s="46">
         <v>0</v>
@@ -14677,7 +14680,7 @@
       </c>
       <c r="U49" s="46">
         <f t="shared" si="2"/>
-        <v>0.99500000000000011</v>
+        <v>0.90999999999999992</v>
       </c>
       <c r="V49" s="231"/>
       <c r="W49" s="233">
@@ -14685,11 +14688,11 @@
       </c>
       <c r="X49" s="231"/>
       <c r="Y49" s="46">
-        <v>0.99500000000000011</v>
+        <v>0.90999999999999992</v>
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-8.500000000000018E-4</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -14737,10 +14740,10 @@
         <v>SEKAB3S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>1.105</v>
+        <v>1.0024999999999999</v>
       </c>
       <c r="R50" s="46">
-        <v>1.165</v>
+        <v>1.0625</v>
       </c>
       <c r="S50" s="46">
         <v>0</v>
@@ -14750,7 +14753,7 @@
       </c>
       <c r="U50" s="46">
         <f t="shared" si="2"/>
-        <v>1.135</v>
+        <v>1.0325</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -14758,11 +14761,11 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>1.135</v>
+        <v>1.0325</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-1.0250000000000016E-3</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -14810,10 +14813,10 @@
         <v>SEKAB3S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>1.27</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="R51" s="46">
-        <v>1.33</v>
+        <v>1.2</v>
       </c>
       <c r="S51" s="46">
         <v>0</v>
@@ -14823,7 +14826,7 @@
       </c>
       <c r="U51" s="46">
         <f t="shared" si="2"/>
-        <v>1.3</v>
+        <v>1.17</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -14831,11 +14834,11 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>1.3</v>
+        <v>1.17</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/100,Trigger)</f>
-        <v>-2.4999999999998981E-5</v>
+        <v>-1.3000000000000025E-3</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -14883,10 +14886,10 @@
         <v>SEKAB3S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>1.4450000000000001</v>
+        <v>1.2850000000000001</v>
       </c>
       <c r="R52" s="46">
-        <v>1.5250000000000001</v>
+        <v>1.365</v>
       </c>
       <c r="S52" s="46">
         <v>0</v>
@@ -14896,7 +14899,7 @@
       </c>
       <c r="U52" s="46">
         <f t="shared" si="2"/>
-        <v>1.4850000000000001</v>
+        <v>1.3250000000000002</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -14904,11 +14907,11 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>1.4850000000000001</v>
+        <v>1.3250000000000002</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-1.599999999999999E-3</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -14956,10 +14959,10 @@
         <v>SEKAB3S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>1.5150000000000001</v>
+        <v>1.3599999999999999</v>
       </c>
       <c r="R53" s="46">
-        <v>1.595</v>
+        <v>1.44</v>
       </c>
       <c r="S53" s="46">
         <v>0</v>
@@ -14969,7 +14972,7 @@
       </c>
       <c r="U53" s="46">
         <f t="shared" si="2"/>
-        <v>1.5550000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -14977,11 +14980,11 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>1.5550000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/100,Trigger)</f>
-        <v>-2.4999999999998981E-5</v>
+        <v>-1.5500000000000028E-3</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -15102,10 +15105,10 @@
         <v>SEKAB3S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>1.5250000000000001</v>
+        <v>1.375</v>
       </c>
       <c r="R55" s="46">
-        <v>1.625</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="S55" s="46">
         <v>0</v>
@@ -15115,7 +15118,7 @@
       </c>
       <c r="U55" s="46">
         <f t="shared" si="2"/>
-        <v>1.5750000000000002</v>
+        <v>1.425</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -15123,11 +15126,11 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>1.5750000000000002</v>
+        <v>1.425</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/100,Trigger)</f>
-        <v>-2.5000000000000716E-5</v>
+        <v>-1.4999999999999996E-3</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -15697,7 +15700,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -15724,7 +15727,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -16825,7 +16828,7 @@
         <v>SEK3S6S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>8.57</v>
+        <v>6.91</v>
       </c>
       <c r="R20" s="46">
         <v>0</v>
@@ -16838,7 +16841,7 @@
       </c>
       <c r="U20" s="46">
         <f t="shared" si="2"/>
-        <v>8.57</v>
+        <v>6.91</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -16846,11 +16849,11 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>8.57</v>
+        <v>6.91</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.6600000000000002E-4</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -17702,7 +17705,7 @@
         <v>SEK3S6S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>9.2799999999999994</v>
+        <v>8.44</v>
       </c>
       <c r="R32" s="46">
         <v>0</v>
@@ -17715,7 +17718,7 @@
       </c>
       <c r="U32" s="46">
         <f t="shared" si="2"/>
-        <v>9.2799999999999994</v>
+        <v>8.44</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -17723,11 +17726,11 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>9.2799999999999994</v>
+        <v>8.44</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
-        <v>0</v>
+        <v>-8.3999999999999982E-5</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -17994,7 +17997,7 @@
         <v>SEK3S6S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>9.51</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="R36" s="46">
         <v>0</v>
@@ -18007,7 +18010,7 @@
       </c>
       <c r="U36" s="46">
         <f t="shared" si="2"/>
-        <v>9.51</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -18015,11 +18018,11 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>9.51</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/10000,Trigger)</f>
-        <v>0</v>
+        <v>-5.600000000000006E-5</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -18286,7 +18289,7 @@
         <v>SEK3S6S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>9.61</v>
+        <v>9.19</v>
       </c>
       <c r="R40" s="46">
         <v>0</v>
@@ -18299,7 +18302,7 @@
       </c>
       <c r="U40" s="46">
         <f t="shared" si="2"/>
-        <v>9.61</v>
+        <v>9.19</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -18307,11 +18310,11 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>9.61</v>
+        <v>9.19</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
-        <v>0</v>
+        <v>-4.1999999999999937E-5</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -18578,7 +18581,7 @@
         <v>SEK3S6S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>9.66</v>
+        <v>9.32</v>
       </c>
       <c r="R44" s="46">
         <v>0</v>
@@ -18591,7 +18594,7 @@
       </c>
       <c r="U44" s="46">
         <f t="shared" si="2"/>
-        <v>9.66</v>
+        <v>9.32</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -18599,11 +18602,11 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>9.66</v>
+        <v>9.32</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
-        <v>0</v>
+        <v>-3.4000000000000067E-5</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -18651,7 +18654,7 @@
         <v>SEK3S6S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>9.68</v>
+        <v>9.39</v>
       </c>
       <c r="R45" s="46">
         <v>0</v>
@@ -18664,7 +18667,7 @@
       </c>
       <c r="U45" s="46">
         <f t="shared" si="2"/>
-        <v>9.68</v>
+        <v>9.39</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -18672,11 +18675,11 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>9.68</v>
+        <v>9.39</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.8999999999999946E-5</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -18724,7 +18727,7 @@
         <v>SEK3S6S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>9.69</v>
+        <v>9.44</v>
       </c>
       <c r="R46" s="46">
         <v>0</v>
@@ -18737,7 +18740,7 @@
       </c>
       <c r="U46" s="46">
         <f t="shared" si="2"/>
-        <v>9.69</v>
+        <v>9.44</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -18745,11 +18748,11 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>9.69</v>
+        <v>9.44</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.4999999999999957E-5</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -18797,7 +18800,7 @@
         <v>SEK3S6S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>9.69</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="R47" s="46">
         <v>0</v>
@@ -18810,7 +18813,7 @@
       </c>
       <c r="U47" s="46">
         <f t="shared" si="2"/>
-        <v>9.69</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -18818,11 +18821,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>9.69</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.1999999999999884E-5</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -18870,7 +18873,7 @@
         <v>SEK3S6S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>9.68</v>
+        <v>9.49</v>
       </c>
       <c r="R48" s="46">
         <v>0</v>
@@ -18883,7 +18886,7 @@
       </c>
       <c r="U48" s="46">
         <f t="shared" si="2"/>
-        <v>9.68</v>
+        <v>9.49</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -18891,11 +18894,11 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>9.68</v>
+        <v>9.49</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.9000000000000028E-5</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -18943,7 +18946,7 @@
         <v>SEK3S6S10Y=ICAP</v>
       </c>
       <c r="Q49" s="46">
-        <v>9.6300000000000008</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -18956,7 +18959,7 @@
       </c>
       <c r="U49" s="46">
         <f t="shared" si="2"/>
-        <v>9.6300000000000008</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="V49" s="231"/>
       <c r="W49" s="233">
@@ -18964,11 +18967,11 @@
       </c>
       <c r="X49" s="231"/>
       <c r="Y49" s="46">
-        <v>9.6300000000000008</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.699999999999998E-5</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -19016,7 +19019,7 @@
         <v>SEK3S6S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>9.370000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="R50" s="46">
         <v>0</v>
@@ -19029,7 +19032,7 @@
       </c>
       <c r="U50" s="46">
         <f t="shared" si="2"/>
-        <v>9.370000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -19037,11 +19040,11 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>9.370000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.4000000000000123E-5</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -19089,7 +19092,7 @@
         <v>SEK3S6S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>8.68</v>
+        <v>8.58</v>
       </c>
       <c r="R51" s="46">
         <v>0</v>
@@ -19102,7 +19105,7 @@
       </c>
       <c r="U51" s="46">
         <f t="shared" si="2"/>
-        <v>8.68</v>
+        <v>8.58</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -19110,11 +19113,11 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>8.68</v>
+        <v>8.58</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.9999999999999178E-6</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -19162,7 +19165,7 @@
         <v>SEK3S6S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>7.65</v>
+        <v>7.57</v>
       </c>
       <c r="R52" s="46">
         <v>0</v>
@@ -19175,7 +19178,7 @@
       </c>
       <c r="U52" s="46">
         <f t="shared" si="2"/>
-        <v>7.65</v>
+        <v>7.57</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -19183,11 +19186,11 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>7.65</v>
+        <v>7.57</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/10000,Trigger)</f>
-        <v>0</v>
+        <v>-7.9999999999999776E-6</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -19235,7 +19238,7 @@
         <v>SEK3S6S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>6.92</v>
+        <v>6.83</v>
       </c>
       <c r="R53" s="46">
         <v>0</v>
@@ -19248,7 +19251,7 @@
       </c>
       <c r="U53" s="46">
         <f t="shared" si="2"/>
-        <v>6.92</v>
+        <v>6.83</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -19256,11 +19259,11 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>6.92</v>
+        <v>6.83</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.0000000000000019E-6</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -19381,7 +19384,7 @@
         <v>SEK3S6S30Y=ICAP</v>
       </c>
       <c r="Q55" s="46">
-        <v>6.32</v>
+        <v>6.23</v>
       </c>
       <c r="R55" s="46">
         <v>0</v>
@@ -19394,7 +19397,7 @@
       </c>
       <c r="U55" s="46">
         <f t="shared" si="2"/>
-        <v>6.32</v>
+        <v>6.23</v>
       </c>
       <c r="V55" s="231"/>
       <c r="W55" s="233">
@@ -19402,11 +19405,11 @@
       </c>
       <c r="X55" s="231"/>
       <c r="Y55" s="46">
-        <v>6.32</v>
+        <v>6.23</v>
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.0000000000000019E-6</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -19976,7 +19979,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -20003,7 +20006,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 09:25:07</v>
+        <v>Paused at 09:35:04</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -21104,7 +21107,7 @@
         <v>SEK1S3S1Y=ICAP</v>
       </c>
       <c r="Q20" s="46">
-        <v>8.0299999999999994</v>
+        <v>7.98</v>
       </c>
       <c r="R20" s="46">
         <v>0</v>
@@ -21117,7 +21120,7 @@
       </c>
       <c r="U20" s="46">
         <f t="shared" si="2"/>
-        <v>8.0299999999999994</v>
+        <v>7.98</v>
       </c>
       <c r="V20" s="231"/>
       <c r="W20" s="233">
@@ -21125,11 +21128,11 @@
       </c>
       <c r="X20" s="231"/>
       <c r="Y20" s="46">
-        <v>8.0299999999999994</v>
+        <v>7.98</v>
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
-        <v>0</v>
+        <v>-4.9999999999999047E-6</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -21981,7 +21984,7 @@
         <v>SEK1S3S2Y=ICAP</v>
       </c>
       <c r="Q32" s="46">
-        <v>9.27</v>
+        <v>9.23</v>
       </c>
       <c r="R32" s="46">
         <v>0</v>
@@ -21994,7 +21997,7 @@
       </c>
       <c r="U32" s="46">
         <f t="shared" si="2"/>
-        <v>9.27</v>
+        <v>9.23</v>
       </c>
       <c r="V32" s="231"/>
       <c r="W32" s="233">
@@ -22002,11 +22005,11 @@
       </c>
       <c r="X32" s="231"/>
       <c r="Y32" s="46">
-        <v>9.27</v>
+        <v>9.23</v>
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
-        <v>0</v>
+        <v>-3.9999999999999888E-6</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -22273,7 +22276,7 @@
         <v>SEK1S3S3Y=ICAP</v>
       </c>
       <c r="Q36" s="46">
-        <v>9.83</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="R36" s="46">
         <v>0</v>
@@ -22286,7 +22289,7 @@
       </c>
       <c r="U36" s="46">
         <f t="shared" si="2"/>
-        <v>9.83</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="V36" s="231"/>
       <c r="W36" s="233">
@@ -22294,11 +22297,11 @@
       </c>
       <c r="X36" s="231"/>
       <c r="Y36" s="46">
-        <v>9.83</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.9999999999999645E-6</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -22565,7 +22568,7 @@
         <v>SEK1S3S4Y=ICAP</v>
       </c>
       <c r="Q40" s="46">
-        <v>10.1</v>
+        <v>10.08</v>
       </c>
       <c r="R40" s="46">
         <v>0</v>
@@ -22578,7 +22581,7 @@
       </c>
       <c r="U40" s="46">
         <f t="shared" si="2"/>
-        <v>10.1</v>
+        <v>10.08</v>
       </c>
       <c r="V40" s="231"/>
       <c r="W40" s="233">
@@ -22586,11 +22589,11 @@
       </c>
       <c r="X40" s="231"/>
       <c r="Y40" s="46">
-        <v>10.1</v>
+        <v>10.08</v>
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.0000000000000486E-6</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -22857,7 +22860,7 @@
         <v>SEK1S3S5Y=ICAP</v>
       </c>
       <c r="Q44" s="46">
-        <v>10.15</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="R44" s="46">
         <v>0</v>
@@ -22870,7 +22873,7 @@
       </c>
       <c r="U44" s="46">
         <f t="shared" si="2"/>
-        <v>10.15</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="V44" s="231"/>
       <c r="W44" s="233">
@@ -22878,11 +22881,11 @@
       </c>
       <c r="X44" s="231"/>
       <c r="Y44" s="46">
-        <v>10.15</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.0000000000000486E-6</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -22930,7 +22933,7 @@
         <v>SEK1S3S6Y=ICAP</v>
       </c>
       <c r="Q45" s="46">
-        <v>10.17</v>
+        <v>10.15</v>
       </c>
       <c r="R45" s="46">
         <v>0</v>
@@ -22943,7 +22946,7 @@
       </c>
       <c r="U45" s="46">
         <f t="shared" si="2"/>
-        <v>10.17</v>
+        <v>10.15</v>
       </c>
       <c r="V45" s="231"/>
       <c r="W45" s="233">
@@ -22951,11 +22954,11 @@
       </c>
       <c r="X45" s="231"/>
       <c r="Y45" s="46">
-        <v>10.17</v>
+        <v>10.15</v>
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
-        <v>0</v>
+        <v>-1.9999999999998318E-6</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -23003,7 +23006,7 @@
         <v>SEK1S3S7Y=ICAP</v>
       </c>
       <c r="Q46" s="46">
-        <v>10.18</v>
+        <v>10.16</v>
       </c>
       <c r="R46" s="46">
         <v>0</v>
@@ -23016,7 +23019,7 @@
       </c>
       <c r="U46" s="46">
         <f t="shared" si="2"/>
-        <v>10.18</v>
+        <v>10.16</v>
       </c>
       <c r="V46" s="231"/>
       <c r="W46" s="233">
@@ -23024,11 +23027,11 @@
       </c>
       <c r="X46" s="231"/>
       <c r="Y46" s="46">
-        <v>10.18</v>
+        <v>10.16</v>
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/10000,Trigger)</f>
-        <v>0</v>
+        <v>-2.0000000000000486E-6</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -23076,7 +23079,7 @@
         <v>SEK1S3S8Y=ICAP</v>
       </c>
       <c r="Q47" s="46">
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="R47" s="46">
         <v>0</v>
@@ -23089,7 +23092,7 @@
       </c>
       <c r="U47" s="46">
         <f t="shared" si="2"/>
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="V47" s="231"/>
       <c r="W47" s="233">
@@ -23097,11 +23100,11 @@
       </c>
       <c r="X47" s="231"/>
       <c r="Y47" s="46">
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.9999999999991589E-7</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -23149,7 +23152,7 @@
         <v>SEK1S3S9Y=ICAP</v>
       </c>
       <c r="Q48" s="46">
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="R48" s="46">
         <v>0</v>
@@ -23162,7 +23165,7 @@
       </c>
       <c r="U48" s="46">
         <f t="shared" si="2"/>
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="V48" s="231"/>
       <c r="W48" s="233">
@@ -23170,11 +23173,11 @@
       </c>
       <c r="X48" s="231"/>
       <c r="Y48" s="46">
-        <v>10.17</v>
+        <v>10.16</v>
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>0</v>
+        <v>-9.9999999999991589E-7</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -23295,7 +23298,7 @@
         <v>SEK1S3S12Y=ICAP</v>
       </c>
       <c r="Q50" s="46">
-        <v>10.14</v>
+        <v>10.15</v>
       </c>
       <c r="R50" s="46">
         <v>0</v>
@@ -23308,7 +23311,7 @@
       </c>
       <c r="U50" s="46">
         <f t="shared" si="2"/>
-        <v>10.14</v>
+        <v>10.15</v>
       </c>
       <c r="V50" s="231"/>
       <c r="W50" s="233">
@@ -23316,11 +23319,11 @@
       </c>
       <c r="X50" s="231"/>
       <c r="Y50" s="46">
-        <v>10.14</v>
+        <v>10.15</v>
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/10000,Trigger)</f>
-        <v>0</v>
+        <v>9.9999999999991589E-7</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -23368,7 +23371,7 @@
         <v>SEK1S3S15Y=ICAP</v>
       </c>
       <c r="Q51" s="46">
-        <v>9.92</v>
+        <v>9.94</v>
       </c>
       <c r="R51" s="46">
         <v>0</v>
@@ -23381,7 +23384,7 @@
       </c>
       <c r="U51" s="46">
         <f t="shared" si="2"/>
-        <v>9.92</v>
+        <v>9.94</v>
       </c>
       <c r="V51" s="231"/>
       <c r="W51" s="233">
@@ -23389,11 +23392,11 @@
       </c>
       <c r="X51" s="231"/>
       <c r="Y51" s="46">
-        <v>9.92</v>
+        <v>9.94</v>
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
-        <v>0</v>
+        <v>1.9999999999998318E-6</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -23441,7 +23444,7 @@
         <v>SEK1S3S20Y=ICAP</v>
       </c>
       <c r="Q52" s="46">
-        <v>9.3800000000000008</v>
+        <v>9.42</v>
       </c>
       <c r="R52" s="46">
         <v>0</v>
@@ -23454,7 +23457,7 @@
       </c>
       <c r="U52" s="46">
         <f t="shared" si="2"/>
-        <v>9.3800000000000008</v>
+        <v>9.42</v>
       </c>
       <c r="V52" s="231"/>
       <c r="W52" s="233">
@@ -23462,11 +23465,11 @@
       </c>
       <c r="X52" s="231"/>
       <c r="Y52" s="46">
-        <v>9.3800000000000008</v>
+        <v>9.42</v>
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/10000,Trigger)</f>
-        <v>0</v>
+        <v>3.9999999999999888E-6</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -23514,7 +23517,7 @@
         <v>SEK1S3S25Y=ICAP</v>
       </c>
       <c r="Q53" s="46">
-        <v>8.9600000000000009</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="R53" s="46">
         <v>0</v>
@@ -23527,7 +23530,7 @@
       </c>
       <c r="U53" s="46">
         <f t="shared" si="2"/>
-        <v>8.9600000000000009</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="V53" s="231"/>
       <c r="W53" s="233">
@@ -23535,11 +23538,11 @@
       </c>
       <c r="X53" s="231"/>
       <c r="Y53" s="46">
-        <v>8.9600000000000009</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
-        <v>0</v>
+        <v>9.9999999999991589E-7</v>
       </c>
       <c r="AA53" s="34"/>
     </row>

</xml_diff>

<commit_message>
IMM Fut with ObjectOverwrite
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK/SEK_Market.xlsx
@@ -1791,54 +1791,46 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
         <stp/>
-        <stp>{0B068006-DE2A-48BB-99DB-D2C3030141A1}</stp>
-        <tr r="P5" s="67"/>
+        <stp>{90BFE4FF-5062-49D3-AB2B-617393EF964C}</stp>
+        <tr r="O6" s="22"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
         <stp/>
-        <stp>{62FAD510-4DC8-4CDD-8C88-A2E390529DA8}</stp>
+        <stp>{0FEDD04E-DD1F-4E0F-BD35-18B552146D7D}</stp>
+        <tr r="N5" s="16"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 16:46:14</v>
+        <stp/>
+        <stp>{184CB3D7-3011-41FA-A180-E9A26CD0C306}</stp>
+        <tr r="S3" s="64"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 16:46:14</v>
+        <stp/>
+        <stp>{6C600682-3ACD-4E2B-9D0C-C096165B89CF}</stp>
         <tr r="P5" s="69"/>
       </tp>
       <tp t="s">
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
         <stp/>
-        <stp>{925B370A-5BCB-4FEE-A44B-17C8EDAC0FA6}</stp>
-        <tr r="O6" s="22"/>
+        <stp>{EF7F85B9-FA7A-4622-AA69-215DFCA8786F}</stp>
+        <tr r="P5" s="66"/>
       </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
         <stp/>
-        <stp>{510AE85C-FFE4-4B71-AF1C-80B4944EA17A}</stp>
-        <tr r="N5" s="16"/>
-      </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 13:02:50</v>
-        <stp/>
-        <stp>{4098CE5D-4FCE-4A5C-B09C-E86753C28D08}</stp>
-        <tr r="S3" s="64"/>
-      </tp>
-    </main>
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 13:02:50</v>
-        <stp/>
-        <stp>{A84EBA7D-07C5-48AA-AB4A-671BB6859644}</stp>
+        <stp>{CA679186-9101-48F6-B635-6B9FE6F6B892}</stp>
         <tr r="K5" s="15"/>
       </tp>
       <tp t="s">
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
         <stp/>
-        <stp>{7EAD2D43-0F7F-4F2C-B1AE-C59E8AE6ADBA}</stp>
-        <tr r="P5" s="66"/>
+        <stp>{59F4C388-DE63-42EB-B0B4-C2932D9849C1}</stp>
+        <tr r="P5" s="67"/>
       </tp>
     </main>
   </volType>
@@ -2162,14 +2154,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="75">
-        <v>42137.543564814812</v>
+        <v>42137.697928240741</v>
       </c>
       <c r="H3" s="114" t="s">
         <v>132</v>
       </c>
       <c r="I3" s="77">
         <f>_xll.ohTrigger(Deposits!S4,FRA3M!X4,OIS!Y5,Swaps3M!Z4,BasisSwap3M6M!Z4,BasisSwap1M3M!Z4)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2178,7 +2170,7 @@
       </c>
       <c r="I4" s="78">
         <f>_xll.ohTrigger(Stibor!W5:W10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -2648,7 +2640,7 @@
       </c>
       <c r="S3" s="183" t="str">
         <f>_xll.RData(S4:S10,T3:U3,"RTFEED:IDN",,,T4)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="T3" s="177" t="s">
         <v>137</v>
@@ -2734,15 +2726,15 @@
       </c>
       <c r="J5" s="123" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C5,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKON#0001</v>
+        <v>SEKON#0000</v>
       </c>
       <c r="K5" s="123" t="str">
         <f>_xll.qlOvernightIndex(I5,,D5,Currency,Calendar,H5,J5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborON#0001</v>
+        <v>SekiborON#0000</v>
       </c>
       <c r="L5" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C5&amp;"LastFixing_Quote",K5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborONLastFixing_Quote#0001</v>
+        <v>SekiborONLastFixing_Quote#0000</v>
       </c>
       <c r="M5" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K5)</f>
@@ -2757,7 +2749,7 @@
       </c>
       <c r="R5" s="21" t="str">
         <f>K5</f>
-        <v>SekiborON#0001</v>
+        <v>SekiborON#0000</v>
       </c>
       <c r="S5" s="178" t="str">
         <f t="shared" ref="S5:S10" si="2">"STI"&amp;Currency&amp;Q5&amp;"DFI="</f>
@@ -2811,11 +2803,11 @@
       <c r="J6" s="123"/>
       <c r="K6" s="123" t="str">
         <f>_xll.qlIborIndex(I6,FamilyName,C6,D6,Currency,E6,F6,G6,H6,J6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor1W#0001</v>
+        <v>Sekibor1W#0000</v>
       </c>
       <c r="L6" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C6&amp;"LastFixing_Quote",K6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor1WLastFixing_Quote#0001</v>
+        <v>Sekibor1WLastFixing_Quote#0000</v>
       </c>
       <c r="M6" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K6)</f>
@@ -2831,7 +2823,7 @@
       </c>
       <c r="R6" s="21" t="str">
         <f>K6</f>
-        <v>Sekibor1W#0001</v>
+        <v>Sekibor1W#0000</v>
       </c>
       <c r="S6" s="178" t="str">
         <f t="shared" si="2"/>
@@ -2884,15 +2876,15 @@
       </c>
       <c r="J7" s="123" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C7,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK1M#0001</v>
+        <v>SEK1M#0000</v>
       </c>
       <c r="K7" s="123" t="str">
         <f>_xll.qlIborIndex(I7,FamilyName,C7,D7,Currency,E7,F7,G7,H7,J7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor1M#0001</v>
+        <v>Sekibor1M#0000</v>
       </c>
       <c r="L7" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C7&amp;"LastFixing_Quote",K7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor1MLastFixing_Quote#0001</v>
+        <v>Sekibor1MLastFixing_Quote#0000</v>
       </c>
       <c r="M7" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K7)</f>
@@ -2908,7 +2900,7 @@
       </c>
       <c r="R7" s="21" t="str">
         <f t="shared" ref="R7:R10" si="4">K7</f>
-        <v>Sekibor1M#0001</v>
+        <v>Sekibor1M#0000</v>
       </c>
       <c r="S7" s="178" t="str">
         <f t="shared" si="2"/>
@@ -2962,11 +2954,11 @@
       <c r="J8" s="123"/>
       <c r="K8" s="123" t="str">
         <f>_xll.qlIborIndex(I8,FamilyName,C8,D8,Currency,E8,F8,G8,H8,J8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor2M#0001</v>
+        <v>Sekibor2M#0000</v>
       </c>
       <c r="L8" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C8&amp;"LastFixing_Quote",K8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor2MLastFixing_Quote#0001</v>
+        <v>Sekibor2MLastFixing_Quote#0000</v>
       </c>
       <c r="M8" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K8)</f>
@@ -2982,7 +2974,7 @@
       </c>
       <c r="R8" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>Sekibor2M#0001</v>
+        <v>Sekibor2M#0000</v>
       </c>
       <c r="S8" s="178" t="str">
         <f t="shared" si="2"/>
@@ -3035,15 +3027,15 @@
       </c>
       <c r="J9" s="123" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C9,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3M#0001</v>
+        <v>SEK3M#0000</v>
       </c>
       <c r="K9" s="123" t="str">
         <f>_xll.qlIborIndex(I9,FamilyName,C9,D9,Currency,E9,F9,G9,H9,J9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor3M#0001</v>
+        <v>Sekibor3M#0000</v>
       </c>
       <c r="L9" s="123" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C9&amp;"LastFixing_Quote",K9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor3MLastFixing_Quote#0001</v>
+        <v>Sekibor3MLastFixing_Quote#0000</v>
       </c>
       <c r="M9" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(K9)</f>
@@ -3059,7 +3051,7 @@
       </c>
       <c r="R9" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>Sekibor3M#0001</v>
+        <v>Sekibor3M#0000</v>
       </c>
       <c r="S9" s="178" t="str">
         <f t="shared" si="2"/>
@@ -3112,15 +3104,15 @@
       </c>
       <c r="J10" s="125" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C10,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK6M#0001</v>
+        <v>SEK6M#0000</v>
       </c>
       <c r="K10" s="125" t="str">
         <f>_xll.qlIborIndex(I10,FamilyName,C10,D10,Currency,E10,F10,G10,H10,J10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor6M#0001</v>
+        <v>Sekibor6M#0000</v>
       </c>
       <c r="L10" s="125" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C10&amp;"LastFixing_Quote",K10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>Sekibor6MLastFixing_Quote#0001</v>
+        <v>Sekibor6MLastFixing_Quote#0000</v>
       </c>
       <c r="M10" s="134" t="str">
         <f>_xll.ohRangeRetrieveError(K10)</f>
@@ -3136,7 +3128,7 @@
       </c>
       <c r="R10" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>Sekibor6M#0001</v>
+        <v>Sekibor6M#0000</v>
       </c>
       <c r="S10" s="179" t="str">
         <f t="shared" si="2"/>
@@ -3175,7 +3167,7 @@
       <c r="I11" s="117"/>
       <c r="J11" s="118" t="str">
         <f>_xll.qlRelinkableHandleYieldTermStructure(Currency&amp;C11,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKSTD#0001</v>
+        <v>SEKSTD#0000</v>
       </c>
       <c r="K11" s="117"/>
       <c r="L11" s="117"/>
@@ -3309,7 +3301,7 @@
       </c>
       <c r="F4" s="140" t="str">
         <f>_xll.qlSwapIndex($E4,FixingType,C4,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc3M#0001</v>
+        <v>SekiborSwapForBasisCalc3M#0000</v>
       </c>
       <c r="G4" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -3331,7 +3323,7 @@
       </c>
       <c r="F5" s="143" t="str">
         <f>_xll.qlSwapIndex($E5,FixingType,C5,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc6M#0001</v>
+        <v>SekiborSwapForBasisCalc6M#0000</v>
       </c>
       <c r="G5" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -3353,7 +3345,7 @@
       </c>
       <c r="F6" s="143" t="str">
         <f>_xll.qlSwapIndex($E6,FixingType,C6,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc9M#0001</v>
+        <v>SekiborSwapForBasisCalc9M#0000</v>
       </c>
       <c r="G6" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -3375,7 +3367,7 @@
       </c>
       <c r="F7" s="143" t="str">
         <f>_xll.qlSwapIndex($E7,FixingType,C7,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc1Y#0001</v>
+        <v>SekiborSwapForBasisCalc1Y#0000</v>
       </c>
       <c r="G7" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -3397,7 +3389,7 @@
       </c>
       <c r="F8" s="143" t="str">
         <f>_xll.qlSwapIndex($E8,FixingType,C8,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc15M#0001</v>
+        <v>SekiborSwapForBasisCalc15M#0000</v>
       </c>
       <c r="G8" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -3419,7 +3411,7 @@
       </c>
       <c r="F9" s="143" t="str">
         <f>_xll.qlSwapIndex($E9,FixingType,C9,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc18M#0001</v>
+        <v>SekiborSwapForBasisCalc18M#0000</v>
       </c>
       <c r="G9" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -3441,7 +3433,7 @@
       </c>
       <c r="F10" s="143" t="str">
         <f>_xll.qlSwapIndex($E10,FixingType,C10,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc2Y#0001</v>
+        <v>SekiborSwapForBasisCalc2Y#0000</v>
       </c>
       <c r="G10" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -3463,7 +3455,7 @@
       </c>
       <c r="F11" s="143" t="str">
         <f>_xll.qlSwapIndex($E11,FixingType,C11,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc3Y#0001</v>
+        <v>SekiborSwapForBasisCalc3Y#0000</v>
       </c>
       <c r="G11" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -3485,7 +3477,7 @@
       </c>
       <c r="F12" s="143" t="str">
         <f>_xll.qlSwapIndex($E12,FixingType,C12,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc4Y#0001</v>
+        <v>SekiborSwapForBasisCalc4Y#0000</v>
       </c>
       <c r="G12" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -3507,7 +3499,7 @@
       </c>
       <c r="F13" s="143" t="str">
         <f>_xll.qlSwapIndex($E13,FixingType,C13,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc5Y#0001</v>
+        <v>SekiborSwapForBasisCalc5Y#0000</v>
       </c>
       <c r="G13" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -3529,7 +3521,7 @@
       </c>
       <c r="F14" s="143" t="str">
         <f>_xll.qlSwapIndex($E14,FixingType,C14,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc6Y#0001</v>
+        <v>SekiborSwapForBasisCalc6Y#0000</v>
       </c>
       <c r="G14" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -3551,7 +3543,7 @@
       </c>
       <c r="F15" s="143" t="str">
         <f>_xll.qlSwapIndex($E15,FixingType,C15,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc7Y#0001</v>
+        <v>SekiborSwapForBasisCalc7Y#0000</v>
       </c>
       <c r="G15" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -3573,7 +3565,7 @@
       </c>
       <c r="F16" s="143" t="str">
         <f>_xll.qlSwapIndex($E16,FixingType,C16,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc8Y#0001</v>
+        <v>SekiborSwapForBasisCalc8Y#0000</v>
       </c>
       <c r="G16" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -3595,7 +3587,7 @@
       </c>
       <c r="F17" s="143" t="str">
         <f>_xll.qlSwapIndex($E17,FixingType,C17,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc9Y#0001</v>
+        <v>SekiborSwapForBasisCalc9Y#0000</v>
       </c>
       <c r="G17" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -3617,7 +3609,7 @@
       </c>
       <c r="F18" s="143" t="str">
         <f>_xll.qlSwapIndex($E18,FixingType,C18,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc10Y#0001</v>
+        <v>SekiborSwapForBasisCalc10Y#0000</v>
       </c>
       <c r="G18" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -3639,7 +3631,7 @@
       </c>
       <c r="F19" s="143" t="str">
         <f>_xll.qlSwapIndex($E19,FixingType,C19,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc11Y#0001</v>
+        <v>SekiborSwapForBasisCalc11Y#0000</v>
       </c>
       <c r="G19" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F19)</f>
@@ -3661,7 +3653,7 @@
       </c>
       <c r="F20" s="143" t="str">
         <f>_xll.qlSwapIndex($E20,FixingType,C20,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc12Y#0001</v>
+        <v>SekiborSwapForBasisCalc12Y#0000</v>
       </c>
       <c r="G20" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F20)</f>
@@ -3683,7 +3675,7 @@
       </c>
       <c r="F21" s="143" t="str">
         <f>_xll.qlSwapIndex($E21,FixingType,C21,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc13Y#0001</v>
+        <v>SekiborSwapForBasisCalc13Y#0000</v>
       </c>
       <c r="G21" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F21)</f>
@@ -3705,7 +3697,7 @@
       </c>
       <c r="F22" s="143" t="str">
         <f>_xll.qlSwapIndex($E22,FixingType,C22,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc14Y#0001</v>
+        <v>SekiborSwapForBasisCalc14Y#0000</v>
       </c>
       <c r="G22" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F22)</f>
@@ -3727,7 +3719,7 @@
       </c>
       <c r="F23" s="143" t="str">
         <f>_xll.qlSwapIndex($E23,FixingType,C23,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc15Y#0001</v>
+        <v>SekiborSwapForBasisCalc15Y#0000</v>
       </c>
       <c r="G23" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F23)</f>
@@ -3749,7 +3741,7 @@
       </c>
       <c r="F24" s="143" t="str">
         <f>_xll.qlSwapIndex($E24,FixingType,C24,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc16Y#0001</v>
+        <v>SekiborSwapForBasisCalc16Y#0000</v>
       </c>
       <c r="G24" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F24)</f>
@@ -3771,7 +3763,7 @@
       </c>
       <c r="F25" s="143" t="str">
         <f>_xll.qlSwapIndex($E25,FixingType,C25,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc17Y#0001</v>
+        <v>SekiborSwapForBasisCalc17Y#0000</v>
       </c>
       <c r="G25" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F25)</f>
@@ -3793,7 +3785,7 @@
       </c>
       <c r="F26" s="143" t="str">
         <f>_xll.qlSwapIndex($E26,FixingType,C26,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc18Y#0001</v>
+        <v>SekiborSwapForBasisCalc18Y#0000</v>
       </c>
       <c r="G26" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F26)</f>
@@ -3815,7 +3807,7 @@
       </c>
       <c r="F27" s="143" t="str">
         <f>_xll.qlSwapIndex($E27,FixingType,C27,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc19Y#0001</v>
+        <v>SekiborSwapForBasisCalc19Y#0000</v>
       </c>
       <c r="G27" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F27)</f>
@@ -3837,7 +3829,7 @@
       </c>
       <c r="F28" s="143" t="str">
         <f>_xll.qlSwapIndex($E28,FixingType,C28,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc20Y#0001</v>
+        <v>SekiborSwapForBasisCalc20Y#0000</v>
       </c>
       <c r="G28" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F28)</f>
@@ -3859,7 +3851,7 @@
       </c>
       <c r="F29" s="143" t="str">
         <f>_xll.qlSwapIndex($E29,FixingType,C29,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc21Y#0001</v>
+        <v>SekiborSwapForBasisCalc21Y#0000</v>
       </c>
       <c r="G29" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F29)</f>
@@ -3881,7 +3873,7 @@
       </c>
       <c r="F30" s="143" t="str">
         <f>_xll.qlSwapIndex($E30,FixingType,C30,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc22Y#0001</v>
+        <v>SekiborSwapForBasisCalc22Y#0000</v>
       </c>
       <c r="G30" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F30)</f>
@@ -3903,7 +3895,7 @@
       </c>
       <c r="F31" s="143" t="str">
         <f>_xll.qlSwapIndex($E31,FixingType,C31,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc23Y#0001</v>
+        <v>SekiborSwapForBasisCalc23Y#0000</v>
       </c>
       <c r="G31" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F31)</f>
@@ -3925,7 +3917,7 @@
       </c>
       <c r="F32" s="143" t="str">
         <f>_xll.qlSwapIndex($E32,FixingType,C32,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc24Y#0001</v>
+        <v>SekiborSwapForBasisCalc24Y#0000</v>
       </c>
       <c r="G32" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F32)</f>
@@ -3947,7 +3939,7 @@
       </c>
       <c r="F33" s="143" t="str">
         <f>_xll.qlSwapIndex($E33,FixingType,C33,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc25Y#0001</v>
+        <v>SekiborSwapForBasisCalc25Y#0000</v>
       </c>
       <c r="G33" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F33)</f>
@@ -3969,7 +3961,7 @@
       </c>
       <c r="F34" s="143" t="str">
         <f>_xll.qlSwapIndex($E34,FixingType,C34,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc26Y#0001</v>
+        <v>SekiborSwapForBasisCalc26Y#0000</v>
       </c>
       <c r="G34" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F34)</f>
@@ -3991,7 +3983,7 @@
       </c>
       <c r="F35" s="143" t="str">
         <f>_xll.qlSwapIndex($E35,FixingType,C35,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc27Y#0001</v>
+        <v>SekiborSwapForBasisCalc27Y#0000</v>
       </c>
       <c r="G35" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F35)</f>
@@ -4013,7 +4005,7 @@
       </c>
       <c r="F36" s="143" t="str">
         <f>_xll.qlSwapIndex($E36,FixingType,C36,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc28Y#0001</v>
+        <v>SekiborSwapForBasisCalc28Y#0000</v>
       </c>
       <c r="G36" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F36)</f>
@@ -4035,7 +4027,7 @@
       </c>
       <c r="F37" s="143" t="str">
         <f>_xll.qlSwapIndex($E37,FixingType,C37,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc29Y#0001</v>
+        <v>SekiborSwapForBasisCalc29Y#0000</v>
       </c>
       <c r="G37" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F37)</f>
@@ -4057,7 +4049,7 @@
       </c>
       <c r="F38" s="143" t="str">
         <f>_xll.qlSwapIndex($E38,FixingType,C38,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc30Y#0001</v>
+        <v>SekiborSwapForBasisCalc30Y#0000</v>
       </c>
       <c r="G38" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F38)</f>
@@ -4079,7 +4071,7 @@
       </c>
       <c r="F39" s="143" t="str">
         <f>_xll.qlSwapIndex($E39,FixingType,C39,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc35Y#0001</v>
+        <v>SekiborSwapForBasisCalc35Y#0000</v>
       </c>
       <c r="G39" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F39)</f>
@@ -4101,7 +4093,7 @@
       </c>
       <c r="F40" s="143" t="str">
         <f>_xll.qlSwapIndex($E40,FixingType,C40,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc40Y#0001</v>
+        <v>SekiborSwapForBasisCalc40Y#0000</v>
       </c>
       <c r="G40" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F40)</f>
@@ -4123,7 +4115,7 @@
       </c>
       <c r="F41" s="143" t="str">
         <f>_xll.qlSwapIndex($E41,FixingType,C41,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc50Y#0001</v>
+        <v>SekiborSwapForBasisCalc50Y#0000</v>
       </c>
       <c r="G41" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(F41)</f>
@@ -4145,7 +4137,7 @@
       </c>
       <c r="F42" s="146" t="str">
         <f>_xll.qlSwapIndex($E42,FixingType,C42,2,Currency,Calendar,"1Y","mf","30/360 (Bond Basis)",Stibor!$K$9,Discounting,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SekiborSwapForBasisCalc60Y#0001</v>
+        <v>SekiborSwapForBasisCalc60Y#0000</v>
       </c>
       <c r="G42" s="146" t="str">
         <f>_xll.ohRangeRetrieveError(F42)</f>
@@ -4555,7 +4547,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="33">
         <f>_xll.ohTrigger(S6:S23)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="T4" s="34"/>
     </row>
@@ -4577,7 +4569,7 @@
       <c r="J5" s="166"/>
       <c r="K5" s="176" t="str">
         <f>_xll.RData(K7:K23,L5:M5,,ReutersRtMode,,L7)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="L5" s="167" t="s">
         <v>106</v>
@@ -4614,7 +4606,7 @@
       </c>
       <c r="E6" s="36" t="str">
         <f>_xll.qlSimpleQuote(D6,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOND_Quote#0001</v>
+        <v>SEKOND_Quote#0000</v>
       </c>
       <c r="F6" s="159" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -4663,7 +4655,7 @@
       </c>
       <c r="E7" s="43" t="str">
         <f>_xll.qlSimpleQuote(D7,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKTND_Quote#0001</v>
+        <v>SEKTND_Quote#0000</v>
       </c>
       <c r="F7" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -4699,7 +4691,7 @@
       </c>
       <c r="S7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E7,R7/100,Trigger)</f>
-        <v>-5.9000000000000003E-4</v>
+        <v>0</v>
       </c>
       <c r="T7" s="34"/>
     </row>
@@ -4714,7 +4706,7 @@
       </c>
       <c r="E8" s="43" t="str">
         <f>_xll.qlSimpleQuote(D8,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKSND_Quote#0001</v>
+        <v>SEKSND_Quote#0000</v>
       </c>
       <c r="F8" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -4765,7 +4757,7 @@
       </c>
       <c r="E9" s="43" t="str">
         <f>_xll.qlSimpleQuote(D9,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKSWD_Quote#0001</v>
+        <v>SEKSWD_Quote#0000</v>
       </c>
       <c r="F9" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -4801,7 +4793,7 @@
       </c>
       <c r="S9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E9,R9/100,Trigger)</f>
-        <v>-1.31E-3</v>
+        <v>0</v>
       </c>
       <c r="T9" s="34"/>
     </row>
@@ -4816,7 +4808,7 @@
       </c>
       <c r="E10" s="43" t="str">
         <f>_xll.qlSimpleQuote(D10,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK2WD_Quote#0001</v>
+        <v>SEK2WD_Quote#0000</v>
       </c>
       <c r="F10" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -4867,7 +4859,7 @@
       </c>
       <c r="E11" s="43" t="str">
         <f>_xll.qlSimpleQuote(D11,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3WD_Quote#0001</v>
+        <v>SEK3WD_Quote#0000</v>
       </c>
       <c r="F11" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -4918,7 +4910,7 @@
       </c>
       <c r="E12" s="43" t="str">
         <f>_xll.qlSimpleQuote(D12,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK1MD_Quote#0001</v>
+        <v>SEK1MD_Quote#0000</v>
       </c>
       <c r="F12" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E12)</f>
@@ -4954,7 +4946,7 @@
       </c>
       <c r="S12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E12,R12/100,Trigger)</f>
-        <v>-1.8800000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="T12" s="34"/>
     </row>
@@ -4969,7 +4961,7 @@
       </c>
       <c r="E13" s="43" t="str">
         <f>_xll.qlSimpleQuote(D13,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK2MD_Quote#0001</v>
+        <v>SEK2MD_Quote#0000</v>
       </c>
       <c r="F13" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E13)</f>
@@ -5005,7 +4997,7 @@
       </c>
       <c r="S13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E13,R13/100,Trigger)</f>
-        <v>-1.7300000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="T13" s="34"/>
     </row>
@@ -5020,7 +5012,7 @@
       </c>
       <c r="E14" s="43" t="str">
         <f>_xll.qlSimpleQuote(D14,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3MD_Quote#0001</v>
+        <v>SEK3MD_Quote#0000</v>
       </c>
       <c r="F14" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E14)</f>
@@ -5056,7 +5048,7 @@
       </c>
       <c r="S14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E14,R14/100,Trigger)</f>
-        <v>-1.5300000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="T14" s="34"/>
     </row>
@@ -5071,7 +5063,7 @@
       </c>
       <c r="E15" s="43" t="str">
         <f>_xll.qlSimpleQuote(D15,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK4MD_Quote#0001</v>
+        <v>SEK4MD_Quote#0000</v>
       </c>
       <c r="F15" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E15)</f>
@@ -5122,7 +5114,7 @@
       </c>
       <c r="E16" s="43" t="str">
         <f>_xll.qlSimpleQuote(D16,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK5MD_Quote#0001</v>
+        <v>SEK5MD_Quote#0000</v>
       </c>
       <c r="F16" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E16)</f>
@@ -5173,7 +5165,7 @@
       </c>
       <c r="E17" s="43" t="str">
         <f>_xll.qlSimpleQuote(D17,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK6MD_Quote#0001</v>
+        <v>SEK6MD_Quote#0000</v>
       </c>
       <c r="F17" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E17)</f>
@@ -5209,7 +5201,7 @@
       </c>
       <c r="S17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(E17,R17/100,Trigger)</f>
-        <v>-1.2799999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="T17" s="34"/>
     </row>
@@ -5224,7 +5216,7 @@
       </c>
       <c r="E18" s="43" t="str">
         <f>_xll.qlSimpleQuote(D18,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK7MD_Quote#0001</v>
+        <v>SEK7MD_Quote#0000</v>
       </c>
       <c r="F18" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E18)</f>
@@ -5275,7 +5267,7 @@
       </c>
       <c r="E19" s="43" t="str">
         <f>_xll.qlSimpleQuote(D19,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK8MD_Quote#0001</v>
+        <v>SEK8MD_Quote#0000</v>
       </c>
       <c r="F19" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E19)</f>
@@ -5326,7 +5318,7 @@
       </c>
       <c r="E20" s="43" t="str">
         <f>_xll.qlSimpleQuote(D20,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK9MD_Quote#0001</v>
+        <v>SEK9MD_Quote#0000</v>
       </c>
       <c r="F20" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E20)</f>
@@ -5377,7 +5369,7 @@
       </c>
       <c r="E21" s="43" t="str">
         <f>_xll.qlSimpleQuote(D21,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK10MD_Quote#0001</v>
+        <v>SEK10MD_Quote#0000</v>
       </c>
       <c r="F21" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E21)</f>
@@ -5428,7 +5420,7 @@
       </c>
       <c r="E22" s="43" t="str">
         <f>_xll.qlSimpleQuote(D22,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK11MD_Quote#0001</v>
+        <v>SEK11MD_Quote#0000</v>
       </c>
       <c r="F22" s="160" t="str">
         <f>_xll.ohRangeRetrieveError(E22)</f>
@@ -5479,7 +5471,7 @@
       </c>
       <c r="E23" s="50" t="str">
         <f>_xll.qlSimpleQuote(D23,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK1YD_Quote#0001</v>
+        <v>SEK1YD_Quote#0000</v>
       </c>
       <c r="F23" s="161" t="str">
         <f>_xll.ohRangeRetrieveError(E23)</f>
@@ -5698,7 +5690,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="33">
         <f>_xll.ohTrigger(X6:X20)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Y4" s="34"/>
       <c r="AA4" s="28"/>
@@ -5729,7 +5721,7 @@
       <c r="M5" s="175"/>
       <c r="N5" s="176" t="str">
         <f>_xll.RData(N6:N20,O5:R5,"RTFEED:IDN",ReutersRtMode,,O6)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="O5" s="168" t="s">
         <v>106</v>
@@ -5787,7 +5779,7 @@
       </c>
       <c r="F6" s="36" t="str">
         <f>_xll.qlSimpleQuote(E6,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F1_Quote#0001</v>
+        <v>SEK3F1_Quote#0000</v>
       </c>
       <c r="G6" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -5838,7 +5830,7 @@
       </c>
       <c r="X6" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F6,W6/100,Trigger)</f>
-        <v>-1.4499999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="AA6" s="28"/>
@@ -5847,16 +5839,16 @@
         <v>FUTSEK3F1_Quote</v>
       </c>
       <c r="AC6" s="36" t="str">
-        <f>_xll.qlSimpleQuote(AB6,,,,Trigger)</f>
-        <v>FUTSEK3F1_Quote#0001</v>
+        <f>_xll.qlSimpleQuote(AB6,,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>FUTSEK3F1_Quote#0010</v>
       </c>
       <c r="AD6" s="199">
         <f>100-W6</f>
         <v>100.24</v>
       </c>
-      <c r="AE6" s="61">
+      <c r="AE6" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC6,AD6,Trigger)</f>
-        <v>0.14499999999999602</v>
+        <v>#N/A</v>
       </c>
       <c r="AF6" s="59"/>
     </row>
@@ -5874,7 +5866,7 @@
       </c>
       <c r="F7" s="43" t="str">
         <f>_xll.qlSimpleQuote(E7,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F2_Quote#0001</v>
+        <v>SEK3F2_Quote#0000</v>
       </c>
       <c r="G7" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -5923,7 +5915,7 @@
       </c>
       <c r="X7" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F7,W7/100,Trigger)</f>
-        <v>-1.4499999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="34"/>
       <c r="AA7" s="28"/>
@@ -5932,16 +5924,16 @@
         <v>FUTSEK3F2_Quote</v>
       </c>
       <c r="AC7" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB7,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB7,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F2_Quote#0001</v>
       </c>
       <c r="AD7" s="200">
         <f t="shared" ref="AD7:AD20" si="6">100-W7</f>
         <v>100.26</v>
       </c>
-      <c r="AE7" s="61">
+      <c r="AE7" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC7,AD7,Trigger)</f>
-        <v>0.14500000000001023</v>
+        <v>#N/A</v>
       </c>
       <c r="AF7" s="59"/>
     </row>
@@ -5959,7 +5951,7 @@
       </c>
       <c r="F8" s="43" t="str">
         <f>_xll.qlSimpleQuote(E8,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F3_Quote#0001</v>
+        <v>SEK3F3_Quote#0000</v>
       </c>
       <c r="G8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -6008,7 +6000,7 @@
       </c>
       <c r="X8" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F8,W8/100,Trigger)</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="34"/>
       <c r="AA8" s="28"/>
@@ -6017,16 +6009,16 @@
         <v>FUTSEK3F3_Quote</v>
       </c>
       <c r="AC8" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB8,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB8,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F3_Quote#0001</v>
       </c>
       <c r="AD8" s="200">
         <f t="shared" si="6"/>
         <v>100.25</v>
       </c>
-      <c r="AE8" s="61">
+      <c r="AE8" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC8,AD8,Trigger)</f>
-        <v>0.12999999999999545</v>
+        <v>#N/A</v>
       </c>
       <c r="AF8" s="59"/>
     </row>
@@ -6044,7 +6036,7 @@
       </c>
       <c r="F9" s="43" t="str">
         <f>_xll.qlSimpleQuote(E9,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F4_Quote#0001</v>
+        <v>SEK3F4_Quote#0000</v>
       </c>
       <c r="G9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -6093,7 +6085,7 @@
       </c>
       <c r="X9" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F9,W9/100,Trigger)</f>
-        <v>-1.2750000000000005E-3</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="34"/>
       <c r="AA9" s="28"/>
@@ -6102,16 +6094,16 @@
         <v>FUTSEK3F4_Quote</v>
       </c>
       <c r="AC9" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB9,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB9,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F4_Quote#0001</v>
       </c>
       <c r="AD9" s="200">
         <f t="shared" si="6"/>
         <v>100.215</v>
       </c>
-      <c r="AE9" s="61">
+      <c r="AE9" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC9,AD9,Trigger)</f>
-        <v>0.12749999999999773</v>
+        <v>#N/A</v>
       </c>
       <c r="AF9" s="59"/>
     </row>
@@ -6129,7 +6121,7 @@
       </c>
       <c r="F10" s="43" t="str">
         <f>_xll.qlSimpleQuote(E10,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F5_Quote#0001</v>
+        <v>SEK3F5_Quote#0000</v>
       </c>
       <c r="G10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -6178,7 +6170,7 @@
       </c>
       <c r="X10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,W10/100,Trigger)</f>
-        <v>-1.0500000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="34"/>
       <c r="AA10" s="28"/>
@@ -6187,16 +6179,16 @@
         <v>FUTSEK3F5_Quote</v>
       </c>
       <c r="AC10" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB10,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB10,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F5_Quote#0001</v>
       </c>
       <c r="AD10" s="200">
         <f t="shared" si="6"/>
         <v>100.14749999999999</v>
       </c>
-      <c r="AE10" s="61">
+      <c r="AE10" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC10,AD10,Trigger)</f>
-        <v>0.10499999999998977</v>
+        <v>#N/A</v>
       </c>
       <c r="AF10" s="59"/>
     </row>
@@ -6214,7 +6206,7 @@
       </c>
       <c r="F11" s="43" t="str">
         <f>_xll.qlSimpleQuote(E11,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F6_Quote#0001</v>
+        <v>SEK3F6_Quote#0000</v>
       </c>
       <c r="G11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -6263,7 +6255,7 @@
       </c>
       <c r="X11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,W11/100,Trigger)</f>
-        <v>-8.0000000000000004E-4</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="34"/>
       <c r="AA11" s="28"/>
@@ -6272,16 +6264,16 @@
         <v>FUTSEK3F6_Quote</v>
       </c>
       <c r="AC11" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB11,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB11,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F6_Quote#0001</v>
       </c>
       <c r="AD11" s="200">
         <f t="shared" si="6"/>
         <v>100.05500000000001</v>
       </c>
-      <c r="AE11" s="61">
+      <c r="AE11" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC11,AD11,Trigger)</f>
-        <v>8.0000000000012506E-2</v>
+        <v>#N/A</v>
       </c>
       <c r="AF11" s="59"/>
     </row>
@@ -6299,7 +6291,7 @@
       </c>
       <c r="F12" s="43" t="str">
         <f>_xll.qlSimpleQuote(E12,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F7_Quote#0001</v>
+        <v>SEK3F7_Quote#0000</v>
       </c>
       <c r="G12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -6348,7 +6340,7 @@
       </c>
       <c r="X12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,W12/100,Trigger)</f>
-        <v>-3.4999999999999983E-4</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="34"/>
       <c r="AA12" s="28"/>
@@ -6357,16 +6349,16 @@
         <v>FUTSEK3F7_Quote</v>
       </c>
       <c r="AC12" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB12,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB12,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F7_Quote#0001</v>
       </c>
       <c r="AD12" s="200">
         <f t="shared" si="6"/>
         <v>99.93</v>
       </c>
-      <c r="AE12" s="61">
+      <c r="AE12" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC12,AD12,Trigger)</f>
-        <v>3.50000000000108E-2</v>
+        <v>#N/A</v>
       </c>
       <c r="AF12" s="59"/>
     </row>
@@ -6384,7 +6376,7 @@
       </c>
       <c r="F13" s="43" t="str">
         <f>_xll.qlSimpleQuote(E13,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F8_Quote#0001</v>
+        <v>SEK3F8_Quote#0000</v>
       </c>
       <c r="G13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -6433,7 +6425,7 @@
       </c>
       <c r="X13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,W13/100,Trigger)</f>
-        <v>7.5000000000000197E-5</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="34"/>
       <c r="AA13" s="28"/>
@@ -6442,16 +6434,16 @@
         <v>FUTSEK3F8_Quote</v>
       </c>
       <c r="AC13" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB13,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB13,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F8_Quote#0001</v>
       </c>
       <c r="AD13" s="200">
         <f t="shared" si="6"/>
         <v>99.802499999999995</v>
       </c>
-      <c r="AE13" s="61">
+      <c r="AE13" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC13,AD13,Trigger)</f>
-        <v>-7.5000000000073896E-3</v>
+        <v>#N/A</v>
       </c>
       <c r="AF13" s="59"/>
     </row>
@@ -6469,7 +6461,7 @@
       </c>
       <c r="F14" s="43" t="str">
         <f>_xll.qlSimpleQuote(E14,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F9_Quote#0001</v>
+        <v>SEK3F9_Quote#0000</v>
       </c>
       <c r="G14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -6518,7 +6510,7 @@
       </c>
       <c r="X14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,W14/100,Trigger)</f>
-        <v>5.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="34"/>
       <c r="AA14" s="28"/>
@@ -6527,16 +6519,16 @@
         <v>FUTSEK3F9_Quote</v>
       </c>
       <c r="AC14" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB14,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB14,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F9_Quote#0001</v>
       </c>
       <c r="AD14" s="200">
         <f t="shared" si="6"/>
         <v>99.674999999999997</v>
       </c>
-      <c r="AE14" s="61">
+      <c r="AE14" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC14,AD14,Trigger)</f>
-        <v>-4.9999999999997158E-2</v>
+        <v>#N/A</v>
       </c>
       <c r="AF14" s="59"/>
     </row>
@@ -6554,7 +6546,7 @@
       </c>
       <c r="F15" s="43" t="str">
         <f>_xll.qlSimpleQuote(E15,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F10_Quote#0001</v>
+        <v>SEK3F10_Quote#0000</v>
       </c>
       <c r="G15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -6603,7 +6595,7 @@
       </c>
       <c r="X15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,W15/100,Trigger)</f>
-        <v>9.7500000000000017E-4</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="34"/>
       <c r="AA15" s="28"/>
@@ -6612,16 +6604,16 @@
         <v>FUTSEK3F10_Quote</v>
       </c>
       <c r="AC15" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB15,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB15,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F10_Quote#0001</v>
       </c>
       <c r="AD15" s="200">
         <f t="shared" si="6"/>
         <v>99.54</v>
       </c>
-      <c r="AE15" s="61">
+      <c r="AE15" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC15,AD15,Trigger)</f>
-        <v>-9.7499999999996589E-2</v>
+        <v>#N/A</v>
       </c>
       <c r="AF15" s="59"/>
     </row>
@@ -6639,7 +6631,7 @@
       </c>
       <c r="F16" s="43" t="str">
         <f>_xll.qlSimpleQuote(E16,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F11_Quote#0001</v>
+        <v>SEK3F11_Quote#0000</v>
       </c>
       <c r="G16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -6688,7 +6680,7 @@
       </c>
       <c r="X16" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F16,W16/100,Trigger)</f>
-        <v>1.449999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="34"/>
       <c r="AA16" s="28"/>
@@ -6697,16 +6689,16 @@
         <v>FUTSEK3F11_Quote</v>
       </c>
       <c r="AC16" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB16,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB16,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F11_Quote#0001</v>
       </c>
       <c r="AD16" s="200">
         <f t="shared" si="6"/>
         <v>99.405000000000001</v>
       </c>
-      <c r="AE16" s="61">
+      <c r="AE16" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC16,AD16,Trigger)</f>
-        <v>-0.14499999999999602</v>
+        <v>#N/A</v>
       </c>
       <c r="AF16" s="59"/>
     </row>
@@ -6724,7 +6716,7 @@
       </c>
       <c r="F17" s="43" t="str">
         <f>_xll.qlSimpleQuote(E17,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F12_Quote#0001</v>
+        <v>SEK3F12_Quote#0000</v>
       </c>
       <c r="G17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -6773,7 +6765,7 @@
       </c>
       <c r="X17" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F17,W17/100,Trigger)</f>
-        <v>1.9250000000000005E-3</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="AA17" s="28"/>
@@ -6782,16 +6774,16 @@
         <v>FUTSEK3F12_Quote</v>
       </c>
       <c r="AC17" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB17,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB17,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F12_Quote#0001</v>
       </c>
       <c r="AD17" s="200">
         <f t="shared" si="6"/>
         <v>99.27</v>
       </c>
-      <c r="AE17" s="61">
+      <c r="AE17" s="61" t="e">
         <f>_xll.qlSimpleQuoteSetValue(AC17,AD17,Trigger)</f>
-        <v>-0.19250000000000966</v>
+        <v>#N/A</v>
       </c>
       <c r="AF17" s="59"/>
     </row>
@@ -6809,7 +6801,7 @@
       </c>
       <c r="F18" s="43" t="str">
         <f>_xll.qlSimpleQuote(E18,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F13_Quote#0001</v>
+        <v>SEK3F13_Quote#0000</v>
       </c>
       <c r="G18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -6867,7 +6859,7 @@
         <v>FUTSEK3F13_Quote</v>
       </c>
       <c r="AC18" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB18,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB18,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F13_Quote#0001</v>
       </c>
       <c r="AD18" s="200" t="e">
@@ -6894,7 +6886,7 @@
       </c>
       <c r="F19" s="43" t="str">
         <f>_xll.qlSimpleQuote(E19,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F14_Quote#0001</v>
+        <v>SEK3F14_Quote#0000</v>
       </c>
       <c r="G19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F19)</f>
@@ -6952,7 +6944,7 @@
         <v>FUTSEK3F14_Quote</v>
       </c>
       <c r="AC19" s="43" t="str">
-        <f>_xll.qlSimpleQuote(AB19,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB19,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F14_Quote#0001</v>
       </c>
       <c r="AD19" s="200" t="e">
@@ -6979,7 +6971,7 @@
       </c>
       <c r="F20" s="50" t="str">
         <f>_xll.qlSimpleQuote(E20,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEK3F15_Quote#0001</v>
+        <v>SEK3F15_Quote#0000</v>
       </c>
       <c r="G20" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(F20)</f>
@@ -7037,7 +7029,7 @@
         <v>FUTSEK3F15_Quote</v>
       </c>
       <c r="AC20" s="50" t="str">
-        <f>_xll.qlSimpleQuote(AB20,,,,Trigger)</f>
+        <f>_xll.qlSimpleQuote(AB20,,,Permanent,Trigger,ObjectOverwrite)</f>
         <v>FUTSEK3F15_Quote#0001</v>
       </c>
       <c r="AD20" s="201" t="e">
@@ -7245,7 +7237,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="33">
         <f>_xll.ohTrigger(Y7:Y61)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Z5" s="34"/>
     </row>
@@ -7271,7 +7263,7 @@
       <c r="N6" s="234"/>
       <c r="O6" s="235" t="str">
         <f>_xll.RData(O7:O61,P6:S6,"RTFEED:IDN",ReutersRtMode,,P7)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="P6" s="190" t="s">
         <v>106</v>
@@ -7315,7 +7307,7 @@
       </c>
       <c r="F7" s="35" t="str">
         <f>_xll.qlSimpleQuote(E7,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOISSW_Quote#0001</v>
+        <v>SEKOISSW_Quote#0000</v>
       </c>
       <c r="G7" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -7387,7 +7379,7 @@
       </c>
       <c r="F8" s="42" t="str">
         <f>_xll.qlSimpleQuote(E8,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS2W_Quote#0001</v>
+        <v>SEKOIS2W_Quote#0000</v>
       </c>
       <c r="G8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -7457,7 +7449,7 @@
       </c>
       <c r="F9" s="42" t="str">
         <f>_xll.qlSimpleQuote(E9,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS3W_Quote#0001</v>
+        <v>SEKOIS3W_Quote#0000</v>
       </c>
       <c r="G9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -7527,7 +7519,7 @@
       </c>
       <c r="F10" s="42" t="str">
         <f>_xll.qlSimpleQuote(E10,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS1M_Quote#0001</v>
+        <v>SEKOIS1M_Quote#0000</v>
       </c>
       <c r="G10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -7579,7 +7571,7 @@
       </c>
       <c r="Y10" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F10,X10/100,Trigger)</f>
-        <v>-8.4000000000000047E-4</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="34"/>
       <c r="AB10" s="237"/>
@@ -7598,7 +7590,7 @@
       </c>
       <c r="F11" s="42" t="str">
         <f>_xll.qlSimpleQuote(E11,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS2M_Quote#0001</v>
+        <v>SEKOIS2M_Quote#0000</v>
       </c>
       <c r="G11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -7650,7 +7642,7 @@
       </c>
       <c r="Y11" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F11,X11/100,Trigger)</f>
-        <v>-8.8999999999999973E-4</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="34"/>
     </row>
@@ -7668,7 +7660,7 @@
       </c>
       <c r="F12" s="42" t="str">
         <f>_xll.qlSimpleQuote(E12,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS3M_Quote#0001</v>
+        <v>SEKOIS3M_Quote#0000</v>
       </c>
       <c r="G12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -7720,7 +7712,7 @@
       </c>
       <c r="Y12" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F12,X12/100,Trigger)</f>
-        <v>-1.0200000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="34"/>
     </row>
@@ -7738,7 +7730,7 @@
       </c>
       <c r="F13" s="42" t="str">
         <f>_xll.qlSimpleQuote(E13,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS4M_Quote#0001</v>
+        <v>SEKOIS4M_Quote#0000</v>
       </c>
       <c r="G13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -7790,7 +7782,7 @@
       </c>
       <c r="Y13" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F13,X13/100,Trigger)</f>
-        <v>-1.0699999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="34"/>
     </row>
@@ -7808,7 +7800,7 @@
       </c>
       <c r="F14" s="42" t="str">
         <f>_xll.qlSimpleQuote(E14,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS5M_Quote#0001</v>
+        <v>SEKOIS5M_Quote#0000</v>
       </c>
       <c r="G14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -7860,7 +7852,7 @@
       </c>
       <c r="Y14" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F14,X14/100,Trigger)</f>
-        <v>-1.0599999999999997E-3</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="34"/>
     </row>
@@ -7878,7 +7870,7 @@
       </c>
       <c r="F15" s="42" t="str">
         <f>_xll.qlSimpleQuote(E15,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS6M_Quote#0001</v>
+        <v>SEKOIS6M_Quote#0000</v>
       </c>
       <c r="G15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -7930,7 +7922,7 @@
       </c>
       <c r="Y15" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F15,X15/100,Trigger)</f>
-        <v>-1.0899999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="34"/>
     </row>
@@ -7948,7 +7940,7 @@
       </c>
       <c r="F16" s="42" t="str">
         <f>_xll.qlSimpleQuote(E16,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS7M_Quote#0001</v>
+        <v>SEKOIS7M_Quote#0000</v>
       </c>
       <c r="G16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -8019,7 +8011,7 @@
       </c>
       <c r="F17" s="42" t="str">
         <f>_xll.qlSimpleQuote(E17,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS8M_Quote#0001</v>
+        <v>SEKOIS8M_Quote#0000</v>
       </c>
       <c r="G17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -8089,7 +8081,7 @@
       </c>
       <c r="F18" s="42" t="str">
         <f>_xll.qlSimpleQuote(E18,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS9M_Quote#0001</v>
+        <v>SEKOIS9M_Quote#0000</v>
       </c>
       <c r="G18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -8141,7 +8133,7 @@
       </c>
       <c r="Y18" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F18,X18/100,Trigger)</f>
-        <v>-1.0699999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="34"/>
       <c r="AC18" s="237"/>
@@ -8160,7 +8152,7 @@
       </c>
       <c r="F19" s="42" t="str">
         <f>_xll.qlSimpleQuote(E19,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS10M_Quote#0001</v>
+        <v>SEKOIS10M_Quote#0000</v>
       </c>
       <c r="G19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F19)</f>
@@ -8230,7 +8222,7 @@
       </c>
       <c r="F20" s="42" t="str">
         <f>_xll.qlSimpleQuote(E20,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS11M_Quote#0001</v>
+        <v>SEKOIS11M_Quote#0000</v>
       </c>
       <c r="G20" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F20)</f>
@@ -8300,7 +8292,7 @@
       </c>
       <c r="F21" s="42" t="str">
         <f>_xll.qlSimpleQuote(E21,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS12M_Quote#0001</v>
+        <v>SEKOIS12M_Quote#0000</v>
       </c>
       <c r="G21" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F21)</f>
@@ -8352,7 +8344,7 @@
       </c>
       <c r="Y21" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F21,X21/100,Trigger)</f>
-        <v>-1.1299999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="34"/>
     </row>
@@ -8370,7 +8362,7 @@
       </c>
       <c r="F22" s="35" t="str">
         <f>_xll.qlSimpleQuote(E22,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS1Y_Quote#0001</v>
+        <v>SEKOIS1Y_Quote#0000</v>
       </c>
       <c r="G22" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(F22)</f>
@@ -8421,7 +8413,7 @@
       </c>
       <c r="Y22" s="41">
         <f>_xll.qlSimpleQuoteSetValue(F22,X22/100,Trigger)</f>
-        <v>-8.7500000000000034E-4</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="34"/>
     </row>
@@ -8439,7 +8431,7 @@
       </c>
       <c r="F23" s="42" t="str">
         <f>_xll.qlSimpleQuote(E23,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS13M_Quote#0001</v>
+        <v>SEKOIS13M_Quote#0000</v>
       </c>
       <c r="G23" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F23)</f>
@@ -8509,7 +8501,7 @@
       </c>
       <c r="F24" s="42" t="str">
         <f>_xll.qlSimpleQuote(E24,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS14M_Quote#0001</v>
+        <v>SEKOIS14M_Quote#0000</v>
       </c>
       <c r="G24" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F24)</f>
@@ -8579,7 +8571,7 @@
       </c>
       <c r="F25" s="42" t="str">
         <f>_xll.qlSimpleQuote(E25,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS15M_Quote#0001</v>
+        <v>SEKOIS15M_Quote#0000</v>
       </c>
       <c r="G25" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F25)</f>
@@ -8649,7 +8641,7 @@
       </c>
       <c r="F26" s="42" t="str">
         <f>_xll.qlSimpleQuote(E26,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS16M_Quote#0001</v>
+        <v>SEKOIS16M_Quote#0000</v>
       </c>
       <c r="G26" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F26)</f>
@@ -8719,7 +8711,7 @@
       </c>
       <c r="F27" s="42" t="str">
         <f>_xll.qlSimpleQuote(E27,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS17M_Quote#0001</v>
+        <v>SEKOIS17M_Quote#0000</v>
       </c>
       <c r="G27" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F27)</f>
@@ -8789,7 +8781,7 @@
       </c>
       <c r="F28" s="42" t="str">
         <f>_xll.qlSimpleQuote(E28,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS18M_Quote#0001</v>
+        <v>SEKOIS18M_Quote#0000</v>
       </c>
       <c r="G28" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F28)</f>
@@ -8859,7 +8851,7 @@
       </c>
       <c r="F29" s="42" t="str">
         <f>_xll.qlSimpleQuote(E29,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS19M_Quote#0001</v>
+        <v>SEKOIS19M_Quote#0000</v>
       </c>
       <c r="G29" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F29)</f>
@@ -8930,7 +8922,7 @@
       </c>
       <c r="F30" s="42" t="str">
         <f>_xll.qlSimpleQuote(E30,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS20M_Quote#0001</v>
+        <v>SEKOIS20M_Quote#0000</v>
       </c>
       <c r="G30" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F30)</f>
@@ -9000,7 +8992,7 @@
       </c>
       <c r="F31" s="42" t="str">
         <f>_xll.qlSimpleQuote(E31,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS21M_Quote#0001</v>
+        <v>SEKOIS21M_Quote#0000</v>
       </c>
       <c r="G31" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F31)</f>
@@ -9070,7 +9062,7 @@
       </c>
       <c r="F32" s="42" t="str">
         <f>_xll.qlSimpleQuote(E32,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS22M_Quote#0001</v>
+        <v>SEKOIS22M_Quote#0000</v>
       </c>
       <c r="G32" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F32)</f>
@@ -9140,7 +9132,7 @@
       </c>
       <c r="F33" s="42" t="str">
         <f>_xll.qlSimpleQuote(E33,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS23M_Quote#0001</v>
+        <v>SEKOIS23M_Quote#0000</v>
       </c>
       <c r="G33" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F33)</f>
@@ -9210,7 +9202,7 @@
       </c>
       <c r="F34" s="42" t="str">
         <f>_xll.qlSimpleQuote(E34,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS2Y_Quote#0001</v>
+        <v>SEKOIS2Y_Quote#0000</v>
       </c>
       <c r="G34" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F34)</f>
@@ -9262,7 +9254,7 @@
       </c>
       <c r="Y34" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F34,X34/100,Trigger)</f>
-        <v>-5.5000000000000014E-4</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="34"/>
     </row>
@@ -9280,7 +9272,7 @@
       </c>
       <c r="F35" s="42" t="str">
         <f>_xll.qlSimpleQuote(E35,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS27M_Quote#0001</v>
+        <v>SEKOIS27M_Quote#0000</v>
       </c>
       <c r="G35" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F35)</f>
@@ -9350,7 +9342,7 @@
       </c>
       <c r="F36" s="42" t="str">
         <f>_xll.qlSimpleQuote(E36,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS30M_Quote#0001</v>
+        <v>SEKOIS30M_Quote#0000</v>
       </c>
       <c r="G36" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F36)</f>
@@ -9420,7 +9412,7 @@
       </c>
       <c r="F37" s="42" t="str">
         <f>_xll.qlSimpleQuote(E37,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS33M_Quote#0001</v>
+        <v>SEKOIS33M_Quote#0000</v>
       </c>
       <c r="G37" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F37)</f>
@@ -9490,7 +9482,7 @@
       </c>
       <c r="F38" s="42" t="str">
         <f>_xll.qlSimpleQuote(E38,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS3Y_Quote#0001</v>
+        <v>SEKOIS3Y_Quote#0000</v>
       </c>
       <c r="G38" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F38)</f>
@@ -9542,7 +9534,7 @@
       </c>
       <c r="Y38" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F38,X38/100,Trigger)</f>
-        <v>1.7499999999999992E-4</v>
+        <v>0</v>
       </c>
       <c r="Z38" s="34"/>
     </row>
@@ -9560,7 +9552,7 @@
       </c>
       <c r="F39" s="42" t="str">
         <f>_xll.qlSimpleQuote(E39,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS39M_Quote#0001</v>
+        <v>SEKOIS39M_Quote#0000</v>
       </c>
       <c r="G39" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F39)</f>
@@ -9630,7 +9622,7 @@
       </c>
       <c r="F40" s="42" t="str">
         <f>_xll.qlSimpleQuote(E40,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS42M_Quote#0001</v>
+        <v>SEKOIS42M_Quote#0000</v>
       </c>
       <c r="G40" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F40)</f>
@@ -9700,7 +9692,7 @@
       </c>
       <c r="F41" s="42" t="str">
         <f>_xll.qlSimpleQuote(E41,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS45M_Quote#0001</v>
+        <v>SEKOIS45M_Quote#0000</v>
       </c>
       <c r="G41" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F41)</f>
@@ -9770,7 +9762,7 @@
       </c>
       <c r="F42" s="42" t="str">
         <f>_xll.qlSimpleQuote(E42,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS4Y_Quote#0001</v>
+        <v>SEKOIS4Y_Quote#0000</v>
       </c>
       <c r="G42" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F42)</f>
@@ -9822,7 +9814,7 @@
       </c>
       <c r="Y42" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F42,X42/100,Trigger)</f>
-        <v>8.7500000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="Z42" s="34"/>
     </row>
@@ -9840,7 +9832,7 @@
       </c>
       <c r="F43" s="42" t="str">
         <f>_xll.qlSimpleQuote(E43,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS51M_Quote#0001</v>
+        <v>SEKOIS51M_Quote#0000</v>
       </c>
       <c r="G43" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F43)</f>
@@ -9910,7 +9902,7 @@
       </c>
       <c r="F44" s="42" t="str">
         <f>_xll.qlSimpleQuote(E44,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS54M_Quote#0001</v>
+        <v>SEKOIS54M_Quote#0000</v>
       </c>
       <c r="G44" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F44)</f>
@@ -9980,7 +9972,7 @@
       </c>
       <c r="F45" s="42" t="str">
         <f>_xll.qlSimpleQuote(E45,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS57M_Quote#0001</v>
+        <v>SEKOIS57M_Quote#0000</v>
       </c>
       <c r="G45" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F45)</f>
@@ -10050,7 +10042,7 @@
       </c>
       <c r="F46" s="42" t="str">
         <f>_xll.qlSimpleQuote(E46,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS5Y_Quote#0001</v>
+        <v>SEKOIS5Y_Quote#0000</v>
       </c>
       <c r="G46" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F46)</f>
@@ -10102,7 +10094,7 @@
       </c>
       <c r="Y46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F46,X46/100,Trigger)</f>
-        <v>1.7250000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="Z46" s="34"/>
     </row>
@@ -10120,7 +10112,7 @@
       </c>
       <c r="F47" s="42" t="str">
         <f>_xll.qlSimpleQuote(E47,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS6Y_Quote#0001</v>
+        <v>SEKOIS6Y_Quote#0000</v>
       </c>
       <c r="G47" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F47)</f>
@@ -10172,7 +10164,7 @@
       </c>
       <c r="Y47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F47,X47/100,Trigger)</f>
-        <v>2.4500000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="34"/>
     </row>
@@ -10190,7 +10182,7 @@
       </c>
       <c r="F48" s="42" t="str">
         <f>_xll.qlSimpleQuote(E48,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS7Y_Quote#0001</v>
+        <v>SEKOIS7Y_Quote#0000</v>
       </c>
       <c r="G48" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F48)</f>
@@ -10242,7 +10234,7 @@
       </c>
       <c r="Y48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F48,X48/100,Trigger)</f>
-        <v>3.1000000000000012E-3</v>
+        <v>0</v>
       </c>
       <c r="Z48" s="34"/>
     </row>
@@ -10260,7 +10252,7 @@
       </c>
       <c r="F49" s="42" t="str">
         <f>_xll.qlSimpleQuote(E49,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS8Y_Quote#0001</v>
+        <v>SEKOIS8Y_Quote#0000</v>
       </c>
       <c r="G49" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F49)</f>
@@ -10312,7 +10304,7 @@
       </c>
       <c r="Y49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F49,X49/100,Trigger)</f>
-        <v>3.6000000000000008E-3</v>
+        <v>0</v>
       </c>
       <c r="Z49" s="34"/>
     </row>
@@ -10330,7 +10322,7 @@
       </c>
       <c r="F50" s="42" t="str">
         <f>_xll.qlSimpleQuote(E50,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS9Y_Quote#0001</v>
+        <v>SEKOIS9Y_Quote#0000</v>
       </c>
       <c r="G50" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F50)</f>
@@ -10382,7 +10374,7 @@
       </c>
       <c r="Y50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F50,X50/100,Trigger)</f>
-        <v>4.000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="34"/>
     </row>
@@ -10400,7 +10392,7 @@
       </c>
       <c r="F51" s="42" t="str">
         <f>_xll.qlSimpleQuote(E51,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS10Y_Quote#0001</v>
+        <v>SEKOIS10Y_Quote#0000</v>
       </c>
       <c r="G51" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F51)</f>
@@ -10452,7 +10444,7 @@
       </c>
       <c r="Y51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F51,X51/100,Trigger)</f>
-        <v>4.2750000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="Z51" s="34"/>
     </row>
@@ -10470,7 +10462,7 @@
       </c>
       <c r="F52" s="42" t="str">
         <f>_xll.qlSimpleQuote(E52,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS12Y_Quote#0001</v>
+        <v>SEKOIS12Y_Quote#0000</v>
       </c>
       <c r="G52" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F52)</f>
@@ -10522,7 +10514,7 @@
       </c>
       <c r="Y52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F52,X52/100,Trigger)</f>
-        <v>4.5750000000000027E-3</v>
+        <v>0</v>
       </c>
       <c r="Z52" s="34"/>
     </row>
@@ -10540,7 +10532,7 @@
       </c>
       <c r="F53" s="42" t="str">
         <f>_xll.qlSimpleQuote(E53,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS15Y_Quote#0001</v>
+        <v>SEKOIS15Y_Quote#0000</v>
       </c>
       <c r="G53" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F53)</f>
@@ -10592,7 +10584,7 @@
       </c>
       <c r="Y53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F53,X53/100,Trigger)</f>
-        <v>4.8500000000000019E-3</v>
+        <v>0</v>
       </c>
       <c r="Z53" s="34"/>
     </row>
@@ -10610,7 +10602,7 @@
       </c>
       <c r="F54" s="42" t="str">
         <f>_xll.qlSimpleQuote(E54,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS20Y_Quote#0001</v>
+        <v>SEKOIS20Y_Quote#0000</v>
       </c>
       <c r="G54" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F54)</f>
@@ -10662,7 +10654,7 @@
       </c>
       <c r="Y54" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F54,X54/100,Trigger)</f>
-        <v>5.0250000000000034E-3</v>
+        <v>0</v>
       </c>
       <c r="Z54" s="34"/>
     </row>
@@ -10680,7 +10672,7 @@
       </c>
       <c r="F55" s="42" t="str">
         <f>_xll.qlSimpleQuote(E55,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS25Y_Quote#0001</v>
+        <v>SEKOIS25Y_Quote#0000</v>
       </c>
       <c r="G55" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F55)</f>
@@ -10732,7 +10724,7 @@
       </c>
       <c r="Y55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F55,X55/100,Trigger)</f>
-        <v>5.025E-3</v>
+        <v>0</v>
       </c>
       <c r="Z55" s="34"/>
     </row>
@@ -10750,7 +10742,7 @@
       </c>
       <c r="F56" s="42" t="str">
         <f>_xll.qlSimpleQuote(E56,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS27Y_Quote#0001</v>
+        <v>SEKOIS27Y_Quote#0000</v>
       </c>
       <c r="G56" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F56)</f>
@@ -10820,7 +10812,7 @@
       </c>
       <c r="F57" s="42" t="str">
         <f>_xll.qlSimpleQuote(E57,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS30Y_Quote#0001</v>
+        <v>SEKOIS30Y_Quote#0000</v>
       </c>
       <c r="G57" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F57)</f>
@@ -10872,7 +10864,7 @@
       </c>
       <c r="Y57" s="48">
         <f>_xll.qlSimpleQuoteSetValue(F57,X57/100,Trigger)</f>
-        <v>5.0750000000000031E-3</v>
+        <v>0</v>
       </c>
       <c r="Z57" s="34"/>
     </row>
@@ -10890,7 +10882,7 @@
       </c>
       <c r="F58" s="42" t="str">
         <f>_xll.qlSimpleQuote(E58,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS35Y_Quote#0001</v>
+        <v>SEKOIS35Y_Quote#0000</v>
       </c>
       <c r="G58" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F58)</f>
@@ -10960,7 +10952,7 @@
       </c>
       <c r="F59" s="42" t="str">
         <f>_xll.qlSimpleQuote(E59,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS40Y_Quote#0001</v>
+        <v>SEKOIS40Y_Quote#0000</v>
       </c>
       <c r="G59" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F59)</f>
@@ -11030,7 +11022,7 @@
       </c>
       <c r="F60" s="42" t="str">
         <f>_xll.qlSimpleQuote(E60,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS45Y_Quote#0001</v>
+        <v>SEKOIS45Y_Quote#0000</v>
       </c>
       <c r="G60" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(F60)</f>
@@ -11100,7 +11092,7 @@
       </c>
       <c r="F61" s="49" t="str">
         <f>_xll.qlSimpleQuote(E61,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKOIS50Y_Quote#0001</v>
+        <v>SEKOIS50Y_Quote#0000</v>
       </c>
       <c r="G61" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(F61)</f>
@@ -11429,7 +11421,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -11456,7 +11448,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -11503,7 +11495,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>_xll.qlSimpleQuote(F6,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3SSW_Quote#0001</v>
+        <v>SEKAB3SSW_Quote#0000</v>
       </c>
       <c r="H6" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(G6)</f>
@@ -11578,7 +11570,7 @@
       </c>
       <c r="G7" s="42" t="str">
         <f>_xll.qlSimpleQuote(F7,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S2W_Quote#0001</v>
+        <v>SEKAB3S2W_Quote#0000</v>
       </c>
       <c r="H7" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G7)</f>
@@ -11651,7 +11643,7 @@
       </c>
       <c r="G8" s="42" t="str">
         <f>_xll.qlSimpleQuote(F8,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S3W_Quote#0001</v>
+        <v>SEKAB3S3W_Quote#0000</v>
       </c>
       <c r="H8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G8)</f>
@@ -11724,7 +11716,7 @@
       </c>
       <c r="G9" s="42" t="str">
         <f>_xll.qlSimpleQuote(F9,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S1M_Quote#0001</v>
+        <v>SEKAB3S1M_Quote#0000</v>
       </c>
       <c r="H9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G9)</f>
@@ -11798,7 +11790,7 @@
       </c>
       <c r="G10" s="42" t="str">
         <f>_xll.qlSimpleQuote(F10,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S2M_Quote#0001</v>
+        <v>SEKAB3S2M_Quote#0000</v>
       </c>
       <c r="H10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G10)</f>
@@ -11871,7 +11863,7 @@
       </c>
       <c r="G11" s="42" t="str">
         <f>_xll.qlSimpleQuote(F11,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S3M_Quote#0001</v>
+        <v>SEKAB3S3M_Quote#0000</v>
       </c>
       <c r="H11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G11)</f>
@@ -11944,7 +11936,7 @@
       </c>
       <c r="G12" s="42" t="str">
         <f>_xll.qlSimpleQuote(F12,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S4M_Quote#0001</v>
+        <v>SEKAB3S4M_Quote#0000</v>
       </c>
       <c r="H12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G12)</f>
@@ -12017,7 +12009,7 @@
       </c>
       <c r="G13" s="42" t="str">
         <f>_xll.qlSimpleQuote(F13,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S5M_Quote#0001</v>
+        <v>SEKAB3S5M_Quote#0000</v>
       </c>
       <c r="H13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G13)</f>
@@ -12090,7 +12082,7 @@
       </c>
       <c r="G14" s="42" t="str">
         <f>_xll.qlSimpleQuote(F14,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S6M_Quote#0001</v>
+        <v>SEKAB3S6M_Quote#0000</v>
       </c>
       <c r="H14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G14)</f>
@@ -12163,7 +12155,7 @@
       </c>
       <c r="G15" s="42" t="str">
         <f>_xll.qlSimpleQuote(F15,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S7M_Quote#0001</v>
+        <v>SEKAB3S7M_Quote#0000</v>
       </c>
       <c r="H15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G15)</f>
@@ -12237,7 +12229,7 @@
       </c>
       <c r="G16" s="42" t="str">
         <f>_xll.qlSimpleQuote(F16,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S8M_Quote#0001</v>
+        <v>SEKAB3S8M_Quote#0000</v>
       </c>
       <c r="H16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G16)</f>
@@ -12310,7 +12302,7 @@
       </c>
       <c r="G17" s="42" t="str">
         <f>_xll.qlSimpleQuote(F17,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S9M_Quote#0001</v>
+        <v>SEKAB3S9M_Quote#0000</v>
       </c>
       <c r="H17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G17)</f>
@@ -12384,7 +12376,7 @@
       </c>
       <c r="G18" s="42" t="str">
         <f>_xll.qlSimpleQuote(F18,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S10M_Quote#0001</v>
+        <v>SEKAB3S10M_Quote#0000</v>
       </c>
       <c r="H18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G18)</f>
@@ -12457,7 +12449,7 @@
       </c>
       <c r="G19" s="42" t="str">
         <f>_xll.qlSimpleQuote(F19,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S11M_Quote#0001</v>
+        <v>SEKAB3S11M_Quote#0000</v>
       </c>
       <c r="H19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G19)</f>
@@ -12530,7 +12522,7 @@
       </c>
       <c r="G20" s="42" t="str">
         <f>_xll.qlSimpleQuote(F20,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S1Y_Quote#0001</v>
+        <v>SEKAB3S1Y_Quote#0000</v>
       </c>
       <c r="H20" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G20)</f>
@@ -12582,7 +12574,7 @@
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/100,Trigger)</f>
-        <v>-1.4249999999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -12603,7 +12595,7 @@
       </c>
       <c r="G21" s="42" t="str">
         <f>_xll.qlSimpleQuote(F21,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S13M_Quote#0001</v>
+        <v>SEKAB3S13M_Quote#0000</v>
       </c>
       <c r="H21" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G21)</f>
@@ -12676,7 +12668,7 @@
       </c>
       <c r="G22" s="42" t="str">
         <f>_xll.qlSimpleQuote(F22,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S14M_Quote#0001</v>
+        <v>SEKAB3S14M_Quote#0000</v>
       </c>
       <c r="H22" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G22)</f>
@@ -12749,7 +12741,7 @@
       </c>
       <c r="G23" s="42" t="str">
         <f>_xll.qlSimpleQuote(F23,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S15M_Quote#0001</v>
+        <v>SEKAB3S15M_Quote#0000</v>
       </c>
       <c r="H23" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G23)</f>
@@ -12822,7 +12814,7 @@
       </c>
       <c r="G24" s="42" t="str">
         <f>_xll.qlSimpleQuote(F24,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S16M_Quote#0001</v>
+        <v>SEKAB3S16M_Quote#0000</v>
       </c>
       <c r="H24" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G24)</f>
@@ -12895,7 +12887,7 @@
       </c>
       <c r="G25" s="42" t="str">
         <f>_xll.qlSimpleQuote(F25,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S17M_Quote#0001</v>
+        <v>SEKAB3S17M_Quote#0000</v>
       </c>
       <c r="H25" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G25)</f>
@@ -12968,7 +12960,7 @@
       </c>
       <c r="G26" s="42" t="str">
         <f>_xll.qlSimpleQuote(F26,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S18M_Quote#0001</v>
+        <v>SEKAB3S18M_Quote#0000</v>
       </c>
       <c r="H26" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G26)</f>
@@ -13041,7 +13033,7 @@
       </c>
       <c r="G27" s="42" t="str">
         <f>_xll.qlSimpleQuote(F27,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S19M_Quote#0001</v>
+        <v>SEKAB3S19M_Quote#0000</v>
       </c>
       <c r="H27" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G27)</f>
@@ -13115,7 +13107,7 @@
       </c>
       <c r="G28" s="42" t="str">
         <f>_xll.qlSimpleQuote(F28,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S20M_Quote#0001</v>
+        <v>SEKAB3S20M_Quote#0000</v>
       </c>
       <c r="H28" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G28)</f>
@@ -13188,7 +13180,7 @@
       </c>
       <c r="G29" s="42" t="str">
         <f>_xll.qlSimpleQuote(F29,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S21M_Quote#0001</v>
+        <v>SEKAB3S21M_Quote#0000</v>
       </c>
       <c r="H29" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G29)</f>
@@ -13261,7 +13253,7 @@
       </c>
       <c r="G30" s="42" t="str">
         <f>_xll.qlSimpleQuote(F30,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S22M_Quote#0001</v>
+        <v>SEKAB3S22M_Quote#0000</v>
       </c>
       <c r="H30" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G30)</f>
@@ -13334,7 +13326,7 @@
       </c>
       <c r="G31" s="42" t="str">
         <f>_xll.qlSimpleQuote(F31,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S23M_Quote#0001</v>
+        <v>SEKAB3S23M_Quote#0000</v>
       </c>
       <c r="H31" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G31)</f>
@@ -13407,7 +13399,7 @@
       </c>
       <c r="G32" s="42" t="str">
         <f>_xll.qlSimpleQuote(F32,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S2Y_Quote#0001</v>
+        <v>SEKAB3S2Y_Quote#0000</v>
       </c>
       <c r="H32" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G32)</f>
@@ -13459,7 +13451,7 @@
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/100,Trigger)</f>
-        <v>-8.9999999999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -13480,7 +13472,7 @@
       </c>
       <c r="G33" s="42" t="str">
         <f>_xll.qlSimpleQuote(F33,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S27M_Quote#0001</v>
+        <v>SEKAB3S27M_Quote#0000</v>
       </c>
       <c r="H33" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G33)</f>
@@ -13553,7 +13545,7 @@
       </c>
       <c r="G34" s="42" t="str">
         <f>_xll.qlSimpleQuote(F34,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S30M_Quote#0001</v>
+        <v>SEKAB3S30M_Quote#0000</v>
       </c>
       <c r="H34" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G34)</f>
@@ -13626,7 +13618,7 @@
       </c>
       <c r="G35" s="42" t="str">
         <f>_xll.qlSimpleQuote(F35,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S33M_Quote#0001</v>
+        <v>SEKAB3S33M_Quote#0000</v>
       </c>
       <c r="H35" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G35)</f>
@@ -13699,7 +13691,7 @@
       </c>
       <c r="G36" s="42" t="str">
         <f>_xll.qlSimpleQuote(F36,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S3Y_Quote#0001</v>
+        <v>SEKAB3S3Y_Quote#0000</v>
       </c>
       <c r="H36" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G36)</f>
@@ -13751,7 +13743,7 @@
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/100,Trigger)</f>
-        <v>-9.9999999999999829E-5</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -13772,7 +13764,7 @@
       </c>
       <c r="G37" s="42" t="str">
         <f>_xll.qlSimpleQuote(F37,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S39M_Quote#0001</v>
+        <v>SEKAB3S39M_Quote#0000</v>
       </c>
       <c r="H37" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G37)</f>
@@ -13845,7 +13837,7 @@
       </c>
       <c r="G38" s="42" t="str">
         <f>_xll.qlSimpleQuote(F38,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S42M_Quote#0001</v>
+        <v>SEKAB3S42M_Quote#0000</v>
       </c>
       <c r="H38" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G38)</f>
@@ -13918,7 +13910,7 @@
       </c>
       <c r="G39" s="42" t="str">
         <f>_xll.qlSimpleQuote(F39,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S45M_Quote#0001</v>
+        <v>SEKAB3S45M_Quote#0000</v>
       </c>
       <c r="H39" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G39)</f>
@@ -13991,7 +13983,7 @@
       </c>
       <c r="G40" s="42" t="str">
         <f>_xll.qlSimpleQuote(F40,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S4Y_Quote#0001</v>
+        <v>SEKAB3S4Y_Quote#0000</v>
       </c>
       <c r="H40" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G40)</f>
@@ -14043,7 +14035,7 @@
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/100,Trigger)</f>
-        <v>7.0000000000000053E-4</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -14064,7 +14056,7 @@
       </c>
       <c r="G41" s="42" t="str">
         <f>_xll.qlSimpleQuote(F41,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S51M_Quote#0001</v>
+        <v>SEKAB3S51M_Quote#0000</v>
       </c>
       <c r="H41" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G41)</f>
@@ -14137,7 +14129,7 @@
       </c>
       <c r="G42" s="42" t="str">
         <f>_xll.qlSimpleQuote(F42,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S54M_Quote#0001</v>
+        <v>SEKAB3S54M_Quote#0000</v>
       </c>
       <c r="H42" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G42)</f>
@@ -14210,7 +14202,7 @@
       </c>
       <c r="G43" s="42" t="str">
         <f>_xll.qlSimpleQuote(F43,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S57M_Quote#0001</v>
+        <v>SEKAB3S57M_Quote#0000</v>
       </c>
       <c r="H43" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G43)</f>
@@ -14283,7 +14275,7 @@
       </c>
       <c r="G44" s="42" t="str">
         <f>_xll.qlSimpleQuote(F44,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S5Y_Quote#0001</v>
+        <v>SEKAB3S5Y_Quote#0000</v>
       </c>
       <c r="H44" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G44)</f>
@@ -14335,7 +14327,7 @@
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/100,Trigger)</f>
-        <v>1.5249999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -14356,7 +14348,7 @@
       </c>
       <c r="G45" s="42" t="str">
         <f>_xll.qlSimpleQuote(F45,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S6Y_Quote#0001</v>
+        <v>SEKAB3S6Y_Quote#0000</v>
       </c>
       <c r="H45" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G45)</f>
@@ -14408,7 +14400,7 @@
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/100,Trigger)</f>
-        <v>2.2000000000000006E-3</v>
+        <v>0</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -14429,7 +14421,7 @@
       </c>
       <c r="G46" s="42" t="str">
         <f>_xll.qlSimpleQuote(F46,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S7Y_Quote#0001</v>
+        <v>SEKAB3S7Y_Quote#0000</v>
       </c>
       <c r="H46" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G46)</f>
@@ -14481,7 +14473,7 @@
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/100,Trigger)</f>
-        <v>2.8250000000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -14502,7 +14494,7 @@
       </c>
       <c r="G47" s="42" t="str">
         <f>_xll.qlSimpleQuote(F47,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S8Y_Quote#0001</v>
+        <v>SEKAB3S8Y_Quote#0000</v>
       </c>
       <c r="H47" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G47)</f>
@@ -14554,7 +14546,7 @@
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/100,Trigger)</f>
-        <v>3.3249999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -14575,7 +14567,7 @@
       </c>
       <c r="G48" s="42" t="str">
         <f>_xll.qlSimpleQuote(F48,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S9Y_Quote#0001</v>
+        <v>SEKAB3S9Y_Quote#0000</v>
       </c>
       <c r="H48" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G48)</f>
@@ -14627,7 +14619,7 @@
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/100,Trigger)</f>
-        <v>3.6999999999999984E-3</v>
+        <v>0</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -14648,7 +14640,7 @@
       </c>
       <c r="G49" s="42" t="str">
         <f>_xll.qlSimpleQuote(F49,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S10Y_Quote#0001</v>
+        <v>SEKAB3S10Y_Quote#0000</v>
       </c>
       <c r="H49" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G49)</f>
@@ -14700,7 +14692,7 @@
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/100,Trigger)</f>
-        <v>3.9750000000000028E-3</v>
+        <v>0</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -14721,7 +14713,7 @@
       </c>
       <c r="G50" s="42" t="str">
         <f>_xll.qlSimpleQuote(F50,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S12Y_Quote#0001</v>
+        <v>SEKAB3S12Y_Quote#0000</v>
       </c>
       <c r="H50" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G50)</f>
@@ -14773,7 +14765,7 @@
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/100,Trigger)</f>
-        <v>4.2500000000000003E-3</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -14794,7 +14786,7 @@
       </c>
       <c r="G51" s="42" t="str">
         <f>_xll.qlSimpleQuote(F51,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S15Y_Quote#0001</v>
+        <v>SEKAB3S15Y_Quote#0000</v>
       </c>
       <c r="H51" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G51)</f>
@@ -14846,7 +14838,7 @@
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/100,Trigger)</f>
-        <v>4.5250000000000012E-3</v>
+        <v>0</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -14867,7 +14859,7 @@
       </c>
       <c r="G52" s="42" t="str">
         <f>_xll.qlSimpleQuote(F52,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S20Y_Quote#0001</v>
+        <v>SEKAB3S20Y_Quote#0000</v>
       </c>
       <c r="H52" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G52)</f>
@@ -14919,7 +14911,7 @@
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/100,Trigger)</f>
-        <v>4.6999999999999993E-3</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -14940,7 +14932,7 @@
       </c>
       <c r="G53" s="42" t="str">
         <f>_xll.qlSimpleQuote(F53,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S25Y_Quote#0001</v>
+        <v>SEKAB3S25Y_Quote#0000</v>
       </c>
       <c r="H53" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G53)</f>
@@ -14992,7 +14984,7 @@
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/100,Trigger)</f>
-        <v>4.7500000000000007E-3</v>
+        <v>0</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -15013,7 +15005,7 @@
       </c>
       <c r="G54" s="42" t="str">
         <f>_xll.qlSimpleQuote(F54,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S27Y_Quote#0001</v>
+        <v>SEKAB3S27Y_Quote#0000</v>
       </c>
       <c r="H54" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G54)</f>
@@ -15086,7 +15078,7 @@
       </c>
       <c r="G55" s="42" t="str">
         <f>_xll.qlSimpleQuote(F55,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S30Y_Quote#0001</v>
+        <v>SEKAB3S30Y_Quote#0000</v>
       </c>
       <c r="H55" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G55)</f>
@@ -15138,7 +15130,7 @@
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/100,Trigger)</f>
-        <v>4.8000000000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -15159,7 +15151,7 @@
       </c>
       <c r="G56" s="42" t="str">
         <f>_xll.qlSimpleQuote(F56,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S35Y_Quote#0001</v>
+        <v>SEKAB3S35Y_Quote#0000</v>
       </c>
       <c r="H56" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G56)</f>
@@ -15232,7 +15224,7 @@
       </c>
       <c r="G57" s="42" t="str">
         <f>_xll.qlSimpleQuote(F57,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S40Y_Quote#0001</v>
+        <v>SEKAB3S40Y_Quote#0000</v>
       </c>
       <c r="H57" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G57)</f>
@@ -15305,7 +15297,7 @@
       </c>
       <c r="G58" s="42" t="str">
         <f>_xll.qlSimpleQuote(F58,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S45Y_Quote#0001</v>
+        <v>SEKAB3S45Y_Quote#0000</v>
       </c>
       <c r="H58" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G58)</f>
@@ -15378,7 +15370,7 @@
       </c>
       <c r="G59" s="49" t="str">
         <f>_xll.qlSimpleQuote(F59,,RateTickValue,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>SEKAB3S50Y_Quote#0001</v>
+        <v>SEKAB3S50Y_Quote#0000</v>
       </c>
       <c r="H59" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(G59)</f>
@@ -15708,7 +15700,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -15735,7 +15727,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -15782,7 +15774,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>_xll.qlSimpleQuote(F6,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6SSW_Quote#0001</v>
+        <v>SEK3S6SSW_Quote#0000</v>
       </c>
       <c r="H6" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(G6)</f>
@@ -15857,7 +15849,7 @@
       </c>
       <c r="G7" s="42" t="str">
         <f>_xll.qlSimpleQuote(F7,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S2W_Quote#0001</v>
+        <v>SEK3S6S2W_Quote#0000</v>
       </c>
       <c r="H7" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G7)</f>
@@ -15930,7 +15922,7 @@
       </c>
       <c r="G8" s="42" t="str">
         <f>_xll.qlSimpleQuote(F8,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S3W_Quote#0001</v>
+        <v>SEK3S6S3W_Quote#0000</v>
       </c>
       <c r="H8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G8)</f>
@@ -16003,7 +15995,7 @@
       </c>
       <c r="G9" s="42" t="str">
         <f>_xll.qlSimpleQuote(F9,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S1M_Quote#0001</v>
+        <v>SEK3S6S1M_Quote#0000</v>
       </c>
       <c r="H9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G9)</f>
@@ -16077,7 +16069,7 @@
       </c>
       <c r="G10" s="42" t="str">
         <f>_xll.qlSimpleQuote(F10,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S2M_Quote#0001</v>
+        <v>SEK3S6S2M_Quote#0000</v>
       </c>
       <c r="H10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G10)</f>
@@ -16150,7 +16142,7 @@
       </c>
       <c r="G11" s="42" t="str">
         <f>_xll.qlSimpleQuote(F11,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S3M_Quote#0001</v>
+        <v>SEK3S6S3M_Quote#0000</v>
       </c>
       <c r="H11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G11)</f>
@@ -16223,7 +16215,7 @@
       </c>
       <c r="G12" s="42" t="str">
         <f>_xll.qlSimpleQuote(F12,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S4M_Quote#0001</v>
+        <v>SEK3S6S4M_Quote#0000</v>
       </c>
       <c r="H12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G12)</f>
@@ -16296,7 +16288,7 @@
       </c>
       <c r="G13" s="42" t="str">
         <f>_xll.qlSimpleQuote(F13,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S5M_Quote#0001</v>
+        <v>SEK3S6S5M_Quote#0000</v>
       </c>
       <c r="H13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G13)</f>
@@ -16369,7 +16361,7 @@
       </c>
       <c r="G14" s="42" t="str">
         <f>_xll.qlSimpleQuote(F14,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S6M_Quote#0001</v>
+        <v>SEK3S6S6M_Quote#0000</v>
       </c>
       <c r="H14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G14)</f>
@@ -16442,7 +16434,7 @@
       </c>
       <c r="G15" s="42" t="str">
         <f>_xll.qlSimpleQuote(F15,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S7M_Quote#0001</v>
+        <v>SEK3S6S7M_Quote#0000</v>
       </c>
       <c r="H15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G15)</f>
@@ -16516,7 +16508,7 @@
       </c>
       <c r="G16" s="42" t="str">
         <f>_xll.qlSimpleQuote(F16,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S8M_Quote#0001</v>
+        <v>SEK3S6S8M_Quote#0000</v>
       </c>
       <c r="H16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G16)</f>
@@ -16589,7 +16581,7 @@
       </c>
       <c r="G17" s="42" t="str">
         <f>_xll.qlSimpleQuote(F17,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S9M_Quote#0001</v>
+        <v>SEK3S6S9M_Quote#0000</v>
       </c>
       <c r="H17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G17)</f>
@@ -16663,7 +16655,7 @@
       </c>
       <c r="G18" s="42" t="str">
         <f>_xll.qlSimpleQuote(F18,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S10M_Quote#0001</v>
+        <v>SEK3S6S10M_Quote#0000</v>
       </c>
       <c r="H18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G18)</f>
@@ -16736,7 +16728,7 @@
       </c>
       <c r="G19" s="42" t="str">
         <f>_xll.qlSimpleQuote(F19,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S11M_Quote#0001</v>
+        <v>SEK3S6S11M_Quote#0000</v>
       </c>
       <c r="H19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G19)</f>
@@ -16809,7 +16801,7 @@
       </c>
       <c r="G20" s="42" t="str">
         <f>_xll.qlSimpleQuote(F20,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S1Y_Quote#0001</v>
+        <v>SEK3S6S1Y_Quote#0000</v>
       </c>
       <c r="H20" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G20)</f>
@@ -16861,7 +16853,7 @@
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
-        <v>1.4000000000000004E-4</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -16882,7 +16874,7 @@
       </c>
       <c r="G21" s="42" t="str">
         <f>_xll.qlSimpleQuote(F21,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S13M_Quote#0001</v>
+        <v>SEK3S6S13M_Quote#0000</v>
       </c>
       <c r="H21" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G21)</f>
@@ -16955,7 +16947,7 @@
       </c>
       <c r="G22" s="42" t="str">
         <f>_xll.qlSimpleQuote(F22,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S14M_Quote#0001</v>
+        <v>SEK3S6S14M_Quote#0000</v>
       </c>
       <c r="H22" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G22)</f>
@@ -17028,7 +17020,7 @@
       </c>
       <c r="G23" s="42" t="str">
         <f>_xll.qlSimpleQuote(F23,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S15M_Quote#0001</v>
+        <v>SEK3S6S15M_Quote#0000</v>
       </c>
       <c r="H23" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G23)</f>
@@ -17101,7 +17093,7 @@
       </c>
       <c r="G24" s="42" t="str">
         <f>_xll.qlSimpleQuote(F24,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S16M_Quote#0001</v>
+        <v>SEK3S6S16M_Quote#0000</v>
       </c>
       <c r="H24" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G24)</f>
@@ -17174,7 +17166,7 @@
       </c>
       <c r="G25" s="42" t="str">
         <f>_xll.qlSimpleQuote(F25,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S17M_Quote#0001</v>
+        <v>SEK3S6S17M_Quote#0000</v>
       </c>
       <c r="H25" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G25)</f>
@@ -17247,7 +17239,7 @@
       </c>
       <c r="G26" s="42" t="str">
         <f>_xll.qlSimpleQuote(F26,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S18M_Quote#0001</v>
+        <v>SEK3S6S18M_Quote#0000</v>
       </c>
       <c r="H26" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G26)</f>
@@ -17320,7 +17312,7 @@
       </c>
       <c r="G27" s="42" t="str">
         <f>_xll.qlSimpleQuote(F27,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S19M_Quote#0001</v>
+        <v>SEK3S6S19M_Quote#0000</v>
       </c>
       <c r="H27" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G27)</f>
@@ -17394,7 +17386,7 @@
       </c>
       <c r="G28" s="42" t="str">
         <f>_xll.qlSimpleQuote(F28,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S20M_Quote#0001</v>
+        <v>SEK3S6S20M_Quote#0000</v>
       </c>
       <c r="H28" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G28)</f>
@@ -17467,7 +17459,7 @@
       </c>
       <c r="G29" s="42" t="str">
         <f>_xll.qlSimpleQuote(F29,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S21M_Quote#0001</v>
+        <v>SEK3S6S21M_Quote#0000</v>
       </c>
       <c r="H29" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G29)</f>
@@ -17540,7 +17532,7 @@
       </c>
       <c r="G30" s="42" t="str">
         <f>_xll.qlSimpleQuote(F30,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S22M_Quote#0001</v>
+        <v>SEK3S6S22M_Quote#0000</v>
       </c>
       <c r="H30" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G30)</f>
@@ -17613,7 +17605,7 @@
       </c>
       <c r="G31" s="42" t="str">
         <f>_xll.qlSimpleQuote(F31,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S23M_Quote#0001</v>
+        <v>SEK3S6S23M_Quote#0000</v>
       </c>
       <c r="H31" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G31)</f>
@@ -17686,7 +17678,7 @@
       </c>
       <c r="G32" s="42" t="str">
         <f>_xll.qlSimpleQuote(F32,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S2Y_Quote#0001</v>
+        <v>SEK3S6S2Y_Quote#0000</v>
       </c>
       <c r="H32" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G32)</f>
@@ -17738,7 +17730,7 @@
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
-        <v>7.1000000000000099E-5</v>
+        <v>0</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -17759,7 +17751,7 @@
       </c>
       <c r="G33" s="42" t="str">
         <f>_xll.qlSimpleQuote(F33,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S27M_Quote#0001</v>
+        <v>SEK3S6S27M_Quote#0000</v>
       </c>
       <c r="H33" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G33)</f>
@@ -17832,7 +17824,7 @@
       </c>
       <c r="G34" s="42" t="str">
         <f>_xll.qlSimpleQuote(F34,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S30M_Quote#0001</v>
+        <v>SEK3S6S30M_Quote#0000</v>
       </c>
       <c r="H34" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G34)</f>
@@ -17905,7 +17897,7 @@
       </c>
       <c r="G35" s="42" t="str">
         <f>_xll.qlSimpleQuote(F35,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S33M_Quote#0001</v>
+        <v>SEK3S6S33M_Quote#0000</v>
       </c>
       <c r="H35" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G35)</f>
@@ -17978,7 +17970,7 @@
       </c>
       <c r="G36" s="42" t="str">
         <f>_xll.qlSimpleQuote(F36,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S3Y_Quote#0001</v>
+        <v>SEK3S6S3Y_Quote#0000</v>
       </c>
       <c r="H36" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G36)</f>
@@ -18030,7 +18022,7 @@
       </c>
       <c r="Z36" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G36,Y36/10000,Trigger)</f>
-        <v>4.6000000000000034E-5</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="34"/>
     </row>
@@ -18051,7 +18043,7 @@
       </c>
       <c r="G37" s="42" t="str">
         <f>_xll.qlSimpleQuote(F37,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S39M_Quote#0001</v>
+        <v>SEK3S6S39M_Quote#0000</v>
       </c>
       <c r="H37" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G37)</f>
@@ -18124,7 +18116,7 @@
       </c>
       <c r="G38" s="42" t="str">
         <f>_xll.qlSimpleQuote(F38,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S42M_Quote#0001</v>
+        <v>SEK3S6S42M_Quote#0000</v>
       </c>
       <c r="H38" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G38)</f>
@@ -18197,7 +18189,7 @@
       </c>
       <c r="G39" s="42" t="str">
         <f>_xll.qlSimpleQuote(F39,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S45M_Quote#0001</v>
+        <v>SEK3S6S45M_Quote#0000</v>
       </c>
       <c r="H39" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G39)</f>
@@ -18270,7 +18262,7 @@
       </c>
       <c r="G40" s="42" t="str">
         <f>_xll.qlSimpleQuote(F40,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S4Y_Quote#0001</v>
+        <v>SEK3S6S4Y_Quote#0000</v>
       </c>
       <c r="H40" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G40)</f>
@@ -18322,7 +18314,7 @@
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
-        <v>3.2999999999999935E-5</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -18343,7 +18335,7 @@
       </c>
       <c r="G41" s="42" t="str">
         <f>_xll.qlSimpleQuote(F41,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S51M_Quote#0001</v>
+        <v>SEK3S6S51M_Quote#0000</v>
       </c>
       <c r="H41" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G41)</f>
@@ -18416,7 +18408,7 @@
       </c>
       <c r="G42" s="42" t="str">
         <f>_xll.qlSimpleQuote(F42,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S54M_Quote#0001</v>
+        <v>SEK3S6S54M_Quote#0000</v>
       </c>
       <c r="H42" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G42)</f>
@@ -18489,7 +18481,7 @@
       </c>
       <c r="G43" s="42" t="str">
         <f>_xll.qlSimpleQuote(F43,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S57M_Quote#0001</v>
+        <v>SEK3S6S57M_Quote#0000</v>
       </c>
       <c r="H43" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G43)</f>
@@ -18562,7 +18554,7 @@
       </c>
       <c r="G44" s="42" t="str">
         <f>_xll.qlSimpleQuote(F44,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S5Y_Quote#0001</v>
+        <v>SEK3S6S5Y_Quote#0000</v>
       </c>
       <c r="H44" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G44)</f>
@@ -18614,7 +18606,7 @@
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
-        <v>2.5000000000000066E-5</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -18635,7 +18627,7 @@
       </c>
       <c r="G45" s="42" t="str">
         <f>_xll.qlSimpleQuote(F45,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S6Y_Quote#0001</v>
+        <v>SEK3S6S6Y_Quote#0000</v>
       </c>
       <c r="H45" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G45)</f>
@@ -18687,7 +18679,7 @@
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
-        <v>1.9999999999999944E-5</v>
+        <v>0</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -18708,7 +18700,7 @@
       </c>
       <c r="G46" s="42" t="str">
         <f>_xll.qlSimpleQuote(F46,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S7Y_Quote#0001</v>
+        <v>SEK3S6S7Y_Quote#0000</v>
       </c>
       <c r="H46" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G46)</f>
@@ -18760,7 +18752,7 @@
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/10000,Trigger)</f>
-        <v>1.5000000000000039E-5</v>
+        <v>0</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -18781,7 +18773,7 @@
       </c>
       <c r="G47" s="42" t="str">
         <f>_xll.qlSimpleQuote(F47,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S8Y_Quote#0001</v>
+        <v>SEK3S6S8Y_Quote#0000</v>
       </c>
       <c r="H47" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G47)</f>
@@ -18833,7 +18825,7 @@
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>1.0999999999999942E-5</v>
+        <v>0</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -18854,7 +18846,7 @@
       </c>
       <c r="G48" s="42" t="str">
         <f>_xll.qlSimpleQuote(F48,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S9Y_Quote#0001</v>
+        <v>SEK3S6S9Y_Quote#0000</v>
       </c>
       <c r="H48" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G48)</f>
@@ -18906,7 +18898,7 @@
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>8.000000000000086E-6</v>
+        <v>0</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -18927,7 +18919,7 @@
       </c>
       <c r="G49" s="42" t="str">
         <f>_xll.qlSimpleQuote(F49,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S10Y_Quote#0001</v>
+        <v>SEK3S6S10Y_Quote#0000</v>
       </c>
       <c r="H49" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G49)</f>
@@ -18979,7 +18971,7 @@
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/10000,Trigger)</f>
-        <v>5.9999999999998206E-6</v>
+        <v>0</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -19000,7 +18992,7 @@
       </c>
       <c r="G50" s="42" t="str">
         <f>_xll.qlSimpleQuote(F50,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S12Y_Quote#0001</v>
+        <v>SEK3S6S12Y_Quote#0000</v>
       </c>
       <c r="H50" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G50)</f>
@@ -19052,7 +19044,7 @@
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/10000,Trigger)</f>
-        <v>4.9999999999999047E-6</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -19073,7 +19065,7 @@
       </c>
       <c r="G51" s="42" t="str">
         <f>_xll.qlSimpleQuote(F51,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S15Y_Quote#0001</v>
+        <v>SEK3S6S15Y_Quote#0000</v>
       </c>
       <c r="H51" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G51)</f>
@@ -19125,7 +19117,7 @@
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
-        <v>4.0000000000000972E-6</v>
+        <v>0</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -19146,7 +19138,7 @@
       </c>
       <c r="G52" s="42" t="str">
         <f>_xll.qlSimpleQuote(F52,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S20Y_Quote#0001</v>
+        <v>SEK3S6S20Y_Quote#0000</v>
       </c>
       <c r="H52" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G52)</f>
@@ -19198,7 +19190,7 @@
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/10000,Trigger)</f>
-        <v>6.9999999999999533E-6</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -19219,7 +19211,7 @@
       </c>
       <c r="G53" s="42" t="str">
         <f>_xll.qlSimpleQuote(F53,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S25Y_Quote#0001</v>
+        <v>SEK3S6S25Y_Quote#0000</v>
       </c>
       <c r="H53" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G53)</f>
@@ -19271,7 +19263,7 @@
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
-        <v>9.9999999999999178E-6</v>
+        <v>0</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -19292,7 +19284,7 @@
       </c>
       <c r="G54" s="42" t="str">
         <f>_xll.qlSimpleQuote(F54,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S27Y_Quote#0001</v>
+        <v>SEK3S6S27Y_Quote#0000</v>
       </c>
       <c r="H54" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G54)</f>
@@ -19365,7 +19357,7 @@
       </c>
       <c r="G55" s="42" t="str">
         <f>_xll.qlSimpleQuote(F55,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S30Y_Quote#0001</v>
+        <v>SEK3S6S30Y_Quote#0000</v>
       </c>
       <c r="H55" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G55)</f>
@@ -19417,7 +19409,7 @@
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/10000,Trigger)</f>
-        <v>1.1999999999999966E-5</v>
+        <v>0</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -19438,7 +19430,7 @@
       </c>
       <c r="G56" s="42" t="str">
         <f>_xll.qlSimpleQuote(F56,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S35Y_Quote#0001</v>
+        <v>SEK3S6S35Y_Quote#0000</v>
       </c>
       <c r="H56" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G56)</f>
@@ -19511,7 +19503,7 @@
       </c>
       <c r="G57" s="42" t="str">
         <f>_xll.qlSimpleQuote(F57,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S40Y_Quote#0001</v>
+        <v>SEK3S6S40Y_Quote#0000</v>
       </c>
       <c r="H57" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G57)</f>
@@ -19584,7 +19576,7 @@
       </c>
       <c r="G58" s="42" t="str">
         <f>_xll.qlSimpleQuote(F58,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S45Y_Quote#0001</v>
+        <v>SEK3S6S45Y_Quote#0000</v>
       </c>
       <c r="H58" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G58)</f>
@@ -19657,7 +19649,7 @@
       </c>
       <c r="G59" s="49" t="str">
         <f>_xll.qlSimpleQuote(F59,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK3S6S50Y_Quote#0001</v>
+        <v>SEK3S6S50Y_Quote#0000</v>
       </c>
       <c r="H59" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(G59)</f>
@@ -19987,7 +19979,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="33">
         <f>_xll.ohTrigger(Z6:Z59)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="34"/>
     </row>
@@ -20014,7 +20006,7 @@
       <c r="O5" s="234"/>
       <c r="P5" s="235" t="str">
         <f>_xll.RData(P6:P59,Q5:T5,"RTFEED:IDN",ReutersRtMode,,Q6)</f>
-        <v>Updated at 13:02:50</v>
+        <v>Updated at 16:46:14</v>
       </c>
       <c r="Q5" s="190" t="s">
         <v>106</v>
@@ -20061,7 +20053,7 @@
       </c>
       <c r="G6" s="35" t="str">
         <f>_xll.qlSimpleQuote(F6,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3SSW_Quote#0001</v>
+        <v>SEK1S3SSW_Quote#0000</v>
       </c>
       <c r="H6" s="192" t="str">
         <f>_xll.ohRangeRetrieveError(G6)</f>
@@ -20136,7 +20128,7 @@
       </c>
       <c r="G7" s="42" t="str">
         <f>_xll.qlSimpleQuote(F7,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S2W_Quote#0001</v>
+        <v>SEK1S3S2W_Quote#0000</v>
       </c>
       <c r="H7" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G7)</f>
@@ -20209,7 +20201,7 @@
       </c>
       <c r="G8" s="42" t="str">
         <f>_xll.qlSimpleQuote(F8,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S3W_Quote#0001</v>
+        <v>SEK1S3S3W_Quote#0000</v>
       </c>
       <c r="H8" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G8)</f>
@@ -20282,7 +20274,7 @@
       </c>
       <c r="G9" s="42" t="str">
         <f>_xll.qlSimpleQuote(F9,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S1M_Quote#0001</v>
+        <v>SEK1S3S1M_Quote#0000</v>
       </c>
       <c r="H9" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G9)</f>
@@ -20356,7 +20348,7 @@
       </c>
       <c r="G10" s="42" t="str">
         <f>_xll.qlSimpleQuote(F10,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S2M_Quote#0001</v>
+        <v>SEK1S3S2M_Quote#0000</v>
       </c>
       <c r="H10" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G10)</f>
@@ -20429,7 +20421,7 @@
       </c>
       <c r="G11" s="42" t="str">
         <f>_xll.qlSimpleQuote(F11,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S3M_Quote#0001</v>
+        <v>SEK1S3S3M_Quote#0000</v>
       </c>
       <c r="H11" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G11)</f>
@@ -20502,7 +20494,7 @@
       </c>
       <c r="G12" s="42" t="str">
         <f>_xll.qlSimpleQuote(F12,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S4M_Quote#0001</v>
+        <v>SEK1S3S4M_Quote#0000</v>
       </c>
       <c r="H12" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G12)</f>
@@ -20575,7 +20567,7 @@
       </c>
       <c r="G13" s="42" t="str">
         <f>_xll.qlSimpleQuote(F13,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S5M_Quote#0001</v>
+        <v>SEK1S3S5M_Quote#0000</v>
       </c>
       <c r="H13" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G13)</f>
@@ -20648,7 +20640,7 @@
       </c>
       <c r="G14" s="42" t="str">
         <f>_xll.qlSimpleQuote(F14,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S6M_Quote#0001</v>
+        <v>SEK1S3S6M_Quote#0000</v>
       </c>
       <c r="H14" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G14)</f>
@@ -20721,7 +20713,7 @@
       </c>
       <c r="G15" s="42" t="str">
         <f>_xll.qlSimpleQuote(F15,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S7M_Quote#0001</v>
+        <v>SEK1S3S7M_Quote#0000</v>
       </c>
       <c r="H15" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G15)</f>
@@ -20795,7 +20787,7 @@
       </c>
       <c r="G16" s="42" t="str">
         <f>_xll.qlSimpleQuote(F16,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S8M_Quote#0001</v>
+        <v>SEK1S3S8M_Quote#0000</v>
       </c>
       <c r="H16" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G16)</f>
@@ -20868,7 +20860,7 @@
       </c>
       <c r="G17" s="42" t="str">
         <f>_xll.qlSimpleQuote(F17,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S9M_Quote#0001</v>
+        <v>SEK1S3S9M_Quote#0000</v>
       </c>
       <c r="H17" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G17)</f>
@@ -20942,7 +20934,7 @@
       </c>
       <c r="G18" s="42" t="str">
         <f>_xll.qlSimpleQuote(F18,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S10M_Quote#0001</v>
+        <v>SEK1S3S10M_Quote#0000</v>
       </c>
       <c r="H18" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G18)</f>
@@ -21015,7 +21007,7 @@
       </c>
       <c r="G19" s="42" t="str">
         <f>_xll.qlSimpleQuote(F19,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S11M_Quote#0001</v>
+        <v>SEK1S3S11M_Quote#0000</v>
       </c>
       <c r="H19" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G19)</f>
@@ -21088,7 +21080,7 @@
       </c>
       <c r="G20" s="42" t="str">
         <f>_xll.qlSimpleQuote(F20,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S1Y_Quote#0001</v>
+        <v>SEK1S3S1Y_Quote#0000</v>
       </c>
       <c r="H20" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G20)</f>
@@ -21140,7 +21132,7 @@
       </c>
       <c r="Z20" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G20,Y20/10000,Trigger)</f>
-        <v>1.0000000000000243E-6</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="34"/>
     </row>
@@ -21161,7 +21153,7 @@
       </c>
       <c r="G21" s="42" t="str">
         <f>_xll.qlSimpleQuote(F21,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S13M_Quote#0001</v>
+        <v>SEK1S3S13M_Quote#0000</v>
       </c>
       <c r="H21" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G21)</f>
@@ -21234,7 +21226,7 @@
       </c>
       <c r="G22" s="42" t="str">
         <f>_xll.qlSimpleQuote(F22,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S14M_Quote#0001</v>
+        <v>SEK1S3S14M_Quote#0000</v>
       </c>
       <c r="H22" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G22)</f>
@@ -21307,7 +21299,7 @@
       </c>
       <c r="G23" s="42" t="str">
         <f>_xll.qlSimpleQuote(F23,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S15M_Quote#0001</v>
+        <v>SEK1S3S15M_Quote#0000</v>
       </c>
       <c r="H23" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G23)</f>
@@ -21380,7 +21372,7 @@
       </c>
       <c r="G24" s="42" t="str">
         <f>_xll.qlSimpleQuote(F24,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S16M_Quote#0001</v>
+        <v>SEK1S3S16M_Quote#0000</v>
       </c>
       <c r="H24" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G24)</f>
@@ -21453,7 +21445,7 @@
       </c>
       <c r="G25" s="42" t="str">
         <f>_xll.qlSimpleQuote(F25,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S17M_Quote#0001</v>
+        <v>SEK1S3S17M_Quote#0000</v>
       </c>
       <c r="H25" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G25)</f>
@@ -21526,7 +21518,7 @@
       </c>
       <c r="G26" s="42" t="str">
         <f>_xll.qlSimpleQuote(F26,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S18M_Quote#0001</v>
+        <v>SEK1S3S18M_Quote#0000</v>
       </c>
       <c r="H26" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G26)</f>
@@ -21599,7 +21591,7 @@
       </c>
       <c r="G27" s="42" t="str">
         <f>_xll.qlSimpleQuote(F27,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S19M_Quote#0001</v>
+        <v>SEK1S3S19M_Quote#0000</v>
       </c>
       <c r="H27" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G27)</f>
@@ -21673,7 +21665,7 @@
       </c>
       <c r="G28" s="42" t="str">
         <f>_xll.qlSimpleQuote(F28,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S20M_Quote#0001</v>
+        <v>SEK1S3S20M_Quote#0000</v>
       </c>
       <c r="H28" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G28)</f>
@@ -21746,7 +21738,7 @@
       </c>
       <c r="G29" s="42" t="str">
         <f>_xll.qlSimpleQuote(F29,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S21M_Quote#0001</v>
+        <v>SEK1S3S21M_Quote#0000</v>
       </c>
       <c r="H29" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G29)</f>
@@ -21819,7 +21811,7 @@
       </c>
       <c r="G30" s="42" t="str">
         <f>_xll.qlSimpleQuote(F30,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S22M_Quote#0001</v>
+        <v>SEK1S3S22M_Quote#0000</v>
       </c>
       <c r="H30" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G30)</f>
@@ -21892,7 +21884,7 @@
       </c>
       <c r="G31" s="42" t="str">
         <f>_xll.qlSimpleQuote(F31,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S23M_Quote#0001</v>
+        <v>SEK1S3S23M_Quote#0000</v>
       </c>
       <c r="H31" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G31)</f>
@@ -21965,7 +21957,7 @@
       </c>
       <c r="G32" s="42" t="str">
         <f>_xll.qlSimpleQuote(F32,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S2Y_Quote#0001</v>
+        <v>SEK1S3S2Y_Quote#0000</v>
       </c>
       <c r="H32" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G32)</f>
@@ -22017,7 +22009,7 @@
       </c>
       <c r="Z32" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G32,Y32/10000,Trigger)</f>
-        <v>1.0000000000000243E-6</v>
+        <v>0</v>
       </c>
       <c r="AA32" s="34"/>
     </row>
@@ -22038,7 +22030,7 @@
       </c>
       <c r="G33" s="42" t="str">
         <f>_xll.qlSimpleQuote(F33,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S27M_Quote#0001</v>
+        <v>SEK1S3S27M_Quote#0000</v>
       </c>
       <c r="H33" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G33)</f>
@@ -22111,7 +22103,7 @@
       </c>
       <c r="G34" s="42" t="str">
         <f>_xll.qlSimpleQuote(F34,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S30M_Quote#0001</v>
+        <v>SEK1S3S30M_Quote#0000</v>
       </c>
       <c r="H34" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G34)</f>
@@ -22184,7 +22176,7 @@
       </c>
       <c r="G35" s="42" t="str">
         <f>_xll.qlSimpleQuote(F35,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S33M_Quote#0001</v>
+        <v>SEK1S3S33M_Quote#0000</v>
       </c>
       <c r="H35" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G35)</f>
@@ -22257,7 +22249,7 @@
       </c>
       <c r="G36" s="42" t="str">
         <f>_xll.qlSimpleQuote(F36,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S3Y_Quote#0001</v>
+        <v>SEK1S3S3Y_Quote#0000</v>
       </c>
       <c r="H36" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G36)</f>
@@ -22330,7 +22322,7 @@
       </c>
       <c r="G37" s="42" t="str">
         <f>_xll.qlSimpleQuote(F37,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S39M_Quote#0001</v>
+        <v>SEK1S3S39M_Quote#0000</v>
       </c>
       <c r="H37" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G37)</f>
@@ -22403,7 +22395,7 @@
       </c>
       <c r="G38" s="42" t="str">
         <f>_xll.qlSimpleQuote(F38,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S42M_Quote#0001</v>
+        <v>SEK1S3S42M_Quote#0000</v>
       </c>
       <c r="H38" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G38)</f>
@@ -22476,7 +22468,7 @@
       </c>
       <c r="G39" s="42" t="str">
         <f>_xll.qlSimpleQuote(F39,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S45M_Quote#0001</v>
+        <v>SEK1S3S45M_Quote#0000</v>
       </c>
       <c r="H39" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G39)</f>
@@ -22549,7 +22541,7 @@
       </c>
       <c r="G40" s="42" t="str">
         <f>_xll.qlSimpleQuote(F40,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S4Y_Quote#0001</v>
+        <v>SEK1S3S4Y_Quote#0000</v>
       </c>
       <c r="H40" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G40)</f>
@@ -22601,7 +22593,7 @@
       </c>
       <c r="Z40" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G40,Y40/10000,Trigger)</f>
-        <v>-2.0000000000000486E-6</v>
+        <v>0</v>
       </c>
       <c r="AA40" s="34"/>
     </row>
@@ -22622,7 +22614,7 @@
       </c>
       <c r="G41" s="42" t="str">
         <f>_xll.qlSimpleQuote(F41,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S51M_Quote#0001</v>
+        <v>SEK1S3S51M_Quote#0000</v>
       </c>
       <c r="H41" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G41)</f>
@@ -22695,7 +22687,7 @@
       </c>
       <c r="G42" s="42" t="str">
         <f>_xll.qlSimpleQuote(F42,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S54M_Quote#0001</v>
+        <v>SEK1S3S54M_Quote#0000</v>
       </c>
       <c r="H42" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G42)</f>
@@ -22768,7 +22760,7 @@
       </c>
       <c r="G43" s="42" t="str">
         <f>_xll.qlSimpleQuote(F43,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S57M_Quote#0001</v>
+        <v>SEK1S3S57M_Quote#0000</v>
       </c>
       <c r="H43" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G43)</f>
@@ -22841,7 +22833,7 @@
       </c>
       <c r="G44" s="42" t="str">
         <f>_xll.qlSimpleQuote(F44,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S5Y_Quote#0001</v>
+        <v>SEK1S3S5Y_Quote#0000</v>
       </c>
       <c r="H44" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G44)</f>
@@ -22893,7 +22885,7 @@
       </c>
       <c r="Z44" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G44,Y44/10000,Trigger)</f>
-        <v>-2.9999999999999645E-6</v>
+        <v>0</v>
       </c>
       <c r="AA44" s="34"/>
     </row>
@@ -22914,7 +22906,7 @@
       </c>
       <c r="G45" s="42" t="str">
         <f>_xll.qlSimpleQuote(F45,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S6Y_Quote#0001</v>
+        <v>SEK1S3S6Y_Quote#0000</v>
       </c>
       <c r="H45" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G45)</f>
@@ -22966,7 +22958,7 @@
       </c>
       <c r="Z45" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G45,Y45/10000,Trigger)</f>
-        <v>-4.0000000000000972E-6</v>
+        <v>0</v>
       </c>
       <c r="AA45" s="34"/>
     </row>
@@ -22987,7 +22979,7 @@
       </c>
       <c r="G46" s="42" t="str">
         <f>_xll.qlSimpleQuote(F46,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S7Y_Quote#0001</v>
+        <v>SEK1S3S7Y_Quote#0000</v>
       </c>
       <c r="H46" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G46)</f>
@@ -23039,7 +23031,7 @@
       </c>
       <c r="Z46" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G46,Y46/10000,Trigger)</f>
-        <v>-5.999999999999929E-6</v>
+        <v>0</v>
       </c>
       <c r="AA46" s="34"/>
     </row>
@@ -23060,7 +23052,7 @@
       </c>
       <c r="G47" s="42" t="str">
         <f>_xll.qlSimpleQuote(F47,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S8Y_Quote#0001</v>
+        <v>SEK1S3S8Y_Quote#0000</v>
       </c>
       <c r="H47" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G47)</f>
@@ -23112,7 +23104,7 @@
       </c>
       <c r="Z47" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G47,Y47/10000,Trigger)</f>
-        <v>-7.0000000000000617E-6</v>
+        <v>0</v>
       </c>
       <c r="AA47" s="34"/>
     </row>
@@ -23133,7 +23125,7 @@
       </c>
       <c r="G48" s="42" t="str">
         <f>_xll.qlSimpleQuote(F48,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S9Y_Quote#0001</v>
+        <v>SEK1S3S9Y_Quote#0000</v>
       </c>
       <c r="H48" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G48)</f>
@@ -23185,7 +23177,7 @@
       </c>
       <c r="Z48" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G48,Y48/10000,Trigger)</f>
-        <v>-7.9999999999999776E-6</v>
+        <v>0</v>
       </c>
       <c r="AA48" s="34"/>
     </row>
@@ -23206,7 +23198,7 @@
       </c>
       <c r="G49" s="42" t="str">
         <f>_xll.qlSimpleQuote(F49,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S10Y_Quote#0001</v>
+        <v>SEK1S3S10Y_Quote#0000</v>
       </c>
       <c r="H49" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G49)</f>
@@ -23258,7 +23250,7 @@
       </c>
       <c r="Z49" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G49,Y49/10000,Trigger)</f>
-        <v>-8.9999999999998935E-6</v>
+        <v>0</v>
       </c>
       <c r="AA49" s="34"/>
     </row>
@@ -23279,7 +23271,7 @@
       </c>
       <c r="G50" s="42" t="str">
         <f>_xll.qlSimpleQuote(F50,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S12Y_Quote#0001</v>
+        <v>SEK1S3S12Y_Quote#0000</v>
       </c>
       <c r="H50" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G50)</f>
@@ -23331,7 +23323,7 @@
       </c>
       <c r="Z50" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G50,Y50/10000,Trigger)</f>
-        <v>-9.0000000000001103E-6</v>
+        <v>0</v>
       </c>
       <c r="AA50" s="34"/>
     </row>
@@ -23352,7 +23344,7 @@
       </c>
       <c r="G51" s="42" t="str">
         <f>_xll.qlSimpleQuote(F51,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S15Y_Quote#0001</v>
+        <v>SEK1S3S15Y_Quote#0000</v>
       </c>
       <c r="H51" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G51)</f>
@@ -23404,7 +23396,7 @@
       </c>
       <c r="Z51" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G51,Y51/10000,Trigger)</f>
-        <v>-8.9999999999998935E-6</v>
+        <v>0</v>
       </c>
       <c r="AA51" s="34"/>
     </row>
@@ -23425,7 +23417,7 @@
       </c>
       <c r="G52" s="42" t="str">
         <f>_xll.qlSimpleQuote(F52,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S20Y_Quote#0001</v>
+        <v>SEK1S3S20Y_Quote#0000</v>
       </c>
       <c r="H52" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G52)</f>
@@ -23477,7 +23469,7 @@
       </c>
       <c r="Z52" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G52,Y52/10000,Trigger)</f>
-        <v>-7.0000000000000617E-6</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="34"/>
     </row>
@@ -23498,7 +23490,7 @@
       </c>
       <c r="G53" s="42" t="str">
         <f>_xll.qlSimpleQuote(F53,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S25Y_Quote#0001</v>
+        <v>SEK1S3S25Y_Quote#0000</v>
       </c>
       <c r="H53" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G53)</f>
@@ -23550,7 +23542,7 @@
       </c>
       <c r="Z53" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G53,Y53/10000,Trigger)</f>
-        <v>-3.9999999999999888E-6</v>
+        <v>0</v>
       </c>
       <c r="AA53" s="34"/>
     </row>
@@ -23571,7 +23563,7 @@
       </c>
       <c r="G54" s="42" t="str">
         <f>_xll.qlSimpleQuote(F54,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S27Y_Quote#0001</v>
+        <v>SEK1S3S27Y_Quote#0000</v>
       </c>
       <c r="H54" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G54)</f>
@@ -23644,7 +23636,7 @@
       </c>
       <c r="G55" s="42" t="str">
         <f>_xll.qlSimpleQuote(F55,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S30Y_Quote#0001</v>
+        <v>SEK1S3S30Y_Quote#0000</v>
       </c>
       <c r="H55" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G55)</f>
@@ -23696,7 +23688,7 @@
       </c>
       <c r="Z55" s="48">
         <f>_xll.qlSimpleQuoteSetValue(G55,Y55/10000,Trigger)</f>
-        <v>-1.9999999999999402E-6</v>
+        <v>0</v>
       </c>
       <c r="AA55" s="34"/>
     </row>
@@ -23717,7 +23709,7 @@
       </c>
       <c r="G56" s="42" t="str">
         <f>_xll.qlSimpleQuote(F56,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S35Y_Quote#0001</v>
+        <v>SEK1S3S35Y_Quote#0000</v>
       </c>
       <c r="H56" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G56)</f>
@@ -23790,7 +23782,7 @@
       </c>
       <c r="G57" s="42" t="str">
         <f>_xll.qlSimpleQuote(F57,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S40Y_Quote#0001</v>
+        <v>SEK1S3S40Y_Quote#0000</v>
       </c>
       <c r="H57" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G57)</f>
@@ -23863,7 +23855,7 @@
       </c>
       <c r="G58" s="42" t="str">
         <f>_xll.qlSimpleQuote(F58,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S45Y_Quote#0001</v>
+        <v>SEK1S3S45Y_Quote#0000</v>
       </c>
       <c r="H58" s="193" t="str">
         <f>_xll.ohRangeRetrieveError(G58)</f>
@@ -23936,7 +23928,7 @@
       </c>
       <c r="G59" s="49" t="str">
         <f>_xll.qlSimpleQuote(F59,,RateTickValue,Permanent,Trigger,TRUE)</f>
-        <v>SEK1S3S50Y_Quote#0001</v>
+        <v>SEK1S3S50Y_Quote#0000</v>
       </c>
       <c r="H59" s="194" t="str">
         <f>_xll.ohRangeRetrieveError(G59)</f>

</xml_diff>